<commit_message>
Update gh-pages to output generated at cd6937a
</commit_message>
<xml_diff>
--- a/上海-漫展信息.xlsx
+++ b/上海-漫展信息.xlsx
@@ -629,7 +629,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -711,7 +711,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -834,7 +834,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>1135</v>
+        <v>1137</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -875,7 +875,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -916,7 +916,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -998,7 +998,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1039,7 +1039,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1080,7 +1080,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1121,7 +1121,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1203,7 +1203,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1244,7 +1244,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>1461</v>
+        <v>1468</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1326,7 +1326,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1449,7 +1449,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>2206</v>
+        <v>2208</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1531,7 +1531,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1613,7 +1613,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1654,7 +1654,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -2087,7 +2087,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -2292,7 +2292,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -2766,7 +2766,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -2807,7 +2807,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -3199,7 +3199,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -3322,7 +3322,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -3404,7 +3404,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -3486,7 +3486,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -3609,7 +3609,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>1135</v>
+        <v>1137</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -3650,7 +3650,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -3691,7 +3691,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -3814,7 +3814,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -3855,7 +3855,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -3896,7 +3896,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -3937,7 +3937,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -4060,7 +4060,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -4101,7 +4101,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -4142,7 +4142,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -4183,7 +4183,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -4265,7 +4265,7 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>1461</v>
+        <v>1468</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -4388,7 +4388,7 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -4511,7 +4511,7 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>2206</v>
+        <v>2208</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -4634,7 +4634,7 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -4757,7 +4757,7 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -4798,7 +4798,7 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update gh-pages to output generated at 8a634ce
</commit_message>
<xml_diff>
--- a/上海-漫展信息.xlsx
+++ b/上海-漫展信息.xlsx
@@ -834,7 +834,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>1137</v>
+        <v>1141</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -875,7 +875,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -916,7 +916,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>738</v>
+        <v>741</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1039,7 +1039,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1121,7 +1121,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1203,7 +1203,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1244,7 +1244,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>1468</v>
+        <v>1471</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1449,7 +1449,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>2208</v>
+        <v>2209</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1531,7 +1531,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1654,7 +1654,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -2292,7 +2292,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -2602,7 +2602,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -2643,7 +2643,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1764</v>
+        <v>1767</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -2684,7 +2684,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1768</v>
+        <v>1769</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -2725,7 +2725,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -2766,7 +2766,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -2807,7 +2807,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -3035,7 +3035,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1764</v>
+        <v>1767</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -3076,7 +3076,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1768</v>
+        <v>1769</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -3117,7 +3117,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -3322,7 +3322,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -3404,7 +3404,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -3609,7 +3609,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>1137</v>
+        <v>1141</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -3650,7 +3650,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -3691,7 +3691,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -3814,7 +3814,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>738</v>
+        <v>741</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -3896,7 +3896,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -4101,7 +4101,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -4183,7 +4183,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -4265,7 +4265,7 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>1468</v>
+        <v>1471</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -4511,7 +4511,7 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>2208</v>
+        <v>2209</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -4634,7 +4634,7 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -4798,7 +4798,7 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update gh-pages to output generated at e2eb17a
</commit_message>
<xml_diff>
--- a/上海-漫展信息.xlsx
+++ b/上海-漫展信息.xlsx
@@ -547,7 +547,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>2139</v>
+        <v>2138</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -629,7 +629,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1563</v>
+        <v>1566</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -711,7 +711,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>364</v>
+        <v>375</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -793,7 +793,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -834,7 +834,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>1141</v>
+        <v>1156</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -875,7 +875,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>668</v>
+        <v>683</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -916,7 +916,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>449</v>
+        <v>457</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>741</v>
+        <v>750</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -998,7 +998,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1039,7 +1039,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1080,7 +1080,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1121,7 +1121,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1203,7 +1203,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>279</v>
+        <v>293</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1244,7 +1244,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>1471</v>
+        <v>1508</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1285,7 +1285,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1326,7 +1326,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1367,7 +1367,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1408,7 +1408,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1449,7 +1449,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>2209</v>
+        <v>2217</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1490,7 +1490,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1531,7 +1531,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>775</v>
+        <v>778</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1572,7 +1572,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1613,7 +1613,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1654,7 +1654,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1800,7 +1800,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -2005,7 +2005,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -2169,7 +2169,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -2292,7 +2292,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>437</v>
+        <v>449</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -2333,7 +2333,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -2374,7 +2374,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -2415,7 +2415,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -2520,7 +2520,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1663</v>
+        <v>1668</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -2643,7 +2643,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1767</v>
+        <v>1771</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -2684,7 +2684,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1769</v>
+        <v>1779</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -2725,7 +2725,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -2766,7 +2766,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>579</v>
+        <v>583</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -2807,7 +2807,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>447</v>
+        <v>459</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -2912,7 +2912,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1663</v>
+        <v>1668</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -2975,30 +2975,30 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2023.11.02</t>
+          <t>2023.10.25</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>上海·Hello Kitty Cosmos 50周年光影特展</t>
+          <t>上海·方块大战（豫园店）</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>漕宝路3055号 宝龙美术馆</t>
+          <t>丽水路88号2楼213 城隍庙第一购物中心</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023.11.02 10:00-2024.01.28 18:00</t>
+          <t>2023.10.25 10:00-2024.10.20 21:00</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>105</v>
+        <v>28</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>139</t>
+          <t>49</t>
         </is>
       </c>
       <c r="H4" t="b">
@@ -3006,7 +3006,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77862&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79057&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3016,30 +3016,30 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2023.12.01</t>
+          <t>2023.11.02</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>上海·2023《蔚蓝档案》x  萌果酱谷子咖啡</t>
+          <t>上海·Hello Kitty Cosmos 50周年光影特展</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>南京东路340号百联ZX 萌果酱谷子咖啡（百联）</t>
+          <t>漕宝路3055号 宝龙美术馆</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023.12.01 00:00-2024.01.31 23:59</t>
+          <t>2023.11.02 10:00-2024.01.28 18:00</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1767</v>
+        <v>105</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>139</t>
         </is>
       </c>
       <c r="H5" t="b">
@@ -3047,7 +3047,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79005&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=77862&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3057,26 +3057,26 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2023.12.06</t>
+          <t>2023.12.01</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>上海·「咒术回战  × animate cafe」</t>
+          <t>上海·2023《蔚蓝档案》x  萌果酱谷子咖啡</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>西藏北路198号大悦城北座8楼N809-1 animate cafe上海店</t>
+          <t>南京东路340号百联ZX 萌果酱谷子咖啡（百联）</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023.12.06 00:00-2024.01.24 23:59</t>
+          <t>2023.12.01 00:00-2024.01.31 23:59</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1769</v>
+        <v>1771</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -3088,7 +3088,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79292&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79005&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3098,26 +3098,26 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2023.12.09</t>
+          <t>2023.12.06</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>上海·非人哉官方授权主题店</t>
+          <t>上海·「咒术回战  × animate cafe」</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>南京东路830号第一百货商业中心B馆5楼(海底捞旁边) 第一百货商业中心</t>
+          <t>西藏北路198号大悦城北座8楼N809-1 animate cafe上海店</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023.12.09 00:00-2024.01.22 23:59</t>
+          <t>2023.12.06 00:00-2024.01.24 23:59</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>595</v>
+        <v>1779</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -3129,7 +3129,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79240&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79292&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3139,30 +3139,30 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2023.12.10</t>
+          <t>2023.12.09</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>上海·多维跃迁-2023 红点设计概念大奖获奖作品展</t>
+          <t>上海·非人哉官方授权主题店</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>国展路1099号 上海世博展览馆</t>
+          <t>南京东路830号第一百货商业中心B馆5楼(海底捞旁边) 第一百货商业中心</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023.12.10 12:00-2024.02.16 17:00</t>
+          <t>2023.12.09 00:00-2024.01.22 23:59</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>24</v>
+        <v>596</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>30</t>
         </is>
       </c>
       <c r="H8" t="b">
@@ -3170,7 +3170,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78809&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79240&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3180,30 +3180,30 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2023.12.22</t>
+          <t>2023.12.10</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>上海·新海诚导演作品《铃芽之旅》展 丨 购票抽新海诚见面会门票丨 超限定复刻原画发售</t>
+          <t>上海·多维跃迁-2023 红点设计概念大奖获奖作品展</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>湖滨路168号 上海无限极荟购物中心</t>
+          <t>国展路1099号 上海世博展览馆</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2023.12.22 10:00-2024.02.16 22:00</t>
+          <t>2023.12.10 12:00-2024.02.16 17:00</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>1563</v>
+        <v>24</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>80</t>
         </is>
       </c>
       <c r="H9" t="b">
@@ -3211,7 +3211,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79166&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78809&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3221,30 +3221,30 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2023.12.25</t>
+          <t>2023.12.22</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>上海·爱乐汇“浪漫经典·一生必听”永恒精选2023烛光音乐会</t>
+          <t>上海·新海诚导演作品《铃芽之旅》展 丨 购票抽新海诚见面会门票丨 超限定复刻原画发售</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>南京西路1376号 上海商城剧院</t>
+          <t>湖滨路168号 上海无限极荟购物中心</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2023.12.25 19:30-2024.02.27 21:00</t>
+          <t>2023.12.22 10:00-2024.02.16 22:00</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>16</v>
+        <v>1566</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H10" t="b">
@@ -3252,7 +3252,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80057&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79166&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3281,7 +3281,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -3322,7 +3322,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>579</v>
+        <v>583</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -3404,7 +3404,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>447</v>
+        <v>459</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -3445,7 +3445,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -3486,7 +3486,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -3527,7 +3527,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>364</v>
+        <v>375</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -3568,7 +3568,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -3609,7 +3609,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>1141</v>
+        <v>1156</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -3650,7 +3650,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>668</v>
+        <v>683</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -3691,7 +3691,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>449</v>
+        <v>457</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -3773,7 +3773,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -3814,7 +3814,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>741</v>
+        <v>750</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -3855,7 +3855,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -3896,7 +3896,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -4019,7 +4019,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -4060,7 +4060,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -4101,7 +4101,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -4142,7 +4142,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -4183,7 +4183,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>279</v>
+        <v>293</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -4265,7 +4265,7 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>1471</v>
+        <v>1508</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -4306,7 +4306,7 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>437</v>
+        <v>449</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -4388,7 +4388,7 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -4429,7 +4429,7 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -4470,7 +4470,7 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -4511,7 +4511,7 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>2209</v>
+        <v>2217</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -4552,7 +4552,7 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -4593,7 +4593,7 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -4634,7 +4634,7 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>775</v>
+        <v>778</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -4675,7 +4675,7 @@
         </is>
       </c>
       <c r="F45" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -4716,7 +4716,7 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -4757,7 +4757,7 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -4798,7 +4798,7 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update gh-pages to output generated at dd351a1
</commit_message>
<xml_diff>
--- a/上海-漫展信息.xlsx
+++ b/上海-漫展信息.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -629,7 +629,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -711,7 +711,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -793,7 +793,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -834,7 +834,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>1156</v>
+        <v>1164</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -875,7 +875,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>683</v>
+        <v>691</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -916,7 +916,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>750</v>
+        <v>753</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -998,7 +998,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1039,7 +1039,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1066,25 +1066,25 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>上海·SISPmini动漫游戏嘉年华</t>
+          <t>上海·25时主题同人茶会</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>淞虹路377号 长宁ArtPark大融城</t>
+          <t>沪太路3100号 尚大国际</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2024.01.27 13:00-01.28 19:00</t>
+          <t>2024.01.27 12:00-01.27 18:00</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>183</v>
+        <v>1</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>58</t>
         </is>
       </c>
       <c r="H16" t="b">
@@ -1092,7 +1092,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79046&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80548&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1107,25 +1107,25 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>上海·同好召集令火影only</t>
+          <t>上海·SISPmini动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>市真南路1199弄1号 智创TOP综合体产城</t>
+          <t>淞虹路377号 长宁ArtPark大融城</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.28 18:00</t>
+          <t>2024.01.27 13:00-01.28 19:00</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>246</v>
+        <v>183</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>48</t>
         </is>
       </c>
       <c r="H17" t="b">
@@ -1133,7 +1133,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80284&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79046&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1148,25 +1148,25 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>上海·咒术only-幽暗之森1.0</t>
+          <t>上海·同好召集令火影only</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
+          <t>市真南路1199弄1号 智创TOP综合体产城</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.27 16:00</t>
+          <t>2024.01.27 10:00-01.28 18:00</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>154</v>
+        <v>246</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>78</t>
         </is>
       </c>
       <c r="H18" t="b">
@@ -1174,7 +1174,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80045&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80284&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1189,7 +1189,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>上海·魔都寒假漫展-CF01</t>
+          <t>上海·咒术only-幽暗之森1.0</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1199,15 +1199,15 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.28 16:00</t>
+          <t>2024.01.27 10:00-01.27 16:00</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>293</v>
+        <v>157</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>59</t>
         </is>
       </c>
       <c r="H19" t="b">
@@ -1215,7 +1215,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80204&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80045&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1225,30 +1225,30 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2024.01.28</t>
+          <t>2024.01.27</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>上海·Comic World动漫游园会</t>
+          <t>上海·魔都寒假漫展-CF01</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>康梧路519号2门 猩际野球室内足球馆</t>
+          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2024.01.28 09:30-01.28 17:00</t>
+          <t>2024.01.27 10:00-01.28 16:00</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>1508</v>
+        <v>295</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>49</t>
         </is>
       </c>
       <c r="H20" t="b">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78523&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80204&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1266,30 +1266,30 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2024.01.31</t>
+          <t>2024.01.28</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>上海·寻迹冬日LOVELIVE同好会</t>
+          <t>上海·Comic World动漫游园会</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>愚园路1250号 新歌空间</t>
+          <t>康梧路519号2门 猩际野球室内足球馆</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2024.01.31 11:30-01.31 17:00</t>
+          <t>2024.01.28 09:30-01.28 17:00</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>139</v>
+        <v>1519</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>70</t>
         </is>
       </c>
       <c r="H21" t="b">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79332&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78523&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1307,30 +1307,30 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2024.02.03</t>
+          <t>2024.01.31</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>上海·第七届次元鹿角动漫游戏展</t>
+          <t>上海·寻迹冬日LOVELIVE同好会</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>长宁路1191号长宁来福士B1 长宁来福士</t>
+          <t>愚园路1250号 新歌空间</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2024.02.03 10:00-02.04 17:00</t>
+          <t>2024.01.31 11:30-01.31 17:00</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>72</v>
+        <v>139</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>83</t>
         </is>
       </c>
       <c r="H22" t="b">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79938&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79332&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1348,30 +1348,30 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2024.02.16</t>
+          <t>2024.02.03</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>上海·第九届次元鹿角动漫游戏展</t>
+          <t>上海·第七届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
+          <t>长宁路1191号长宁来福士B1 长宁来福士</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2024.02.16 11:00-02.17 18:00</t>
+          <t>2024.02.03 10:00-02.04 17:00</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>68</t>
         </is>
       </c>
       <c r="H23" t="b">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80497&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79938&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1389,30 +1389,30 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2024.02.24</t>
+          <t>2024.02.16</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>上海·SISP动漫游戏嘉年华</t>
+          <t>上海·第九届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>年家浜路518号 周浦万达广场</t>
+          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2024.02.24 13:00-02.25 19:00</t>
+          <t>2024.02.16 11:00-02.17 18:00</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H24" t="b">
@@ -1420,7 +1420,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80339&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80497&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1435,33 +1435,33 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>上海·第三届燃梦BACG PRO游戏动漫展</t>
+          <t>上海·SISP动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
+          <t>年家浜路518号 周浦万达广场</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2024.02.24 11:00-02.25 16:30</t>
+          <t>2024.02.24 13:00-02.25 19:00</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>2217</v>
+        <v>54</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>48</t>
         </is>
       </c>
       <c r="H25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77754&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80339&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1471,38 +1471,38 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2024.03.02</t>
+          <t>2024.02.24</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>上海·原神X星穹铁道ONLY</t>
+          <t>上海·第三届燃梦BACG PRO游戏动漫展</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>逸仙路301号靠纪念路路口 上海宝丰联大酒店</t>
+          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2024.03.02 10:00-03.02 17:00</t>
+          <t>2024.02.24 11:00-02.25 16:30</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>115</v>
+        <v>2221</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80299&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=77754&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1512,30 +1512,30 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2024.03.09</t>
+          <t>2024.03.02</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
+          <t>上海·原神X星穹铁道ONLY</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>漕宝路1688号 诺宝中心酒店</t>
+          <t>逸仙路301号靠纪念路路口 上海宝丰联大酒店</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2024.03.09 10:00-03.09 16:30</t>
+          <t>2024.03.02 10:00-03.02 17:00</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>778</v>
+        <v>118</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>60</t>
         </is>
       </c>
       <c r="H27" t="b">
@@ -1543,7 +1543,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=76410&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80299&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1553,30 +1553,30 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2024.04.05</t>
+          <t>2024.03.09</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>上海·第四届次元鹿角动漫游戏展</t>
+          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>顾村镇蕰川路6号 智慧湾科创园</t>
+          <t>漕宝路1688号 诺宝中心酒店</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2024.04.05 10:00-04.06 17:00</t>
+          <t>2024.03.09 10:00-03.09 16:30</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>53</v>
+        <v>779</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>73</t>
         </is>
       </c>
       <c r="H28" t="b">
@@ -1584,7 +1584,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78228&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=76410&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1594,30 +1594,30 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2024.05.01</t>
+          <t>2024.04.05</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>上海·  第五十三届妖漫动漫游戏展</t>
+          <t>上海·第四届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>安蒲汇塘路50号 安垦徐汇创意园</t>
+          <t>顾村镇蕰川路6号 智慧湾科创园</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2024.05.01 10:00-05.02 17:00</t>
+          <t>2024.04.05 10:00-04.06 17:00</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>60</t>
         </is>
       </c>
       <c r="H29" t="b">
@@ -1625,7 +1625,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78657&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78228&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1640,31 +1640,72 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
+          <t>上海·  第五十三届妖漫动漫游戏展</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>安蒲汇塘路50号 安垦徐汇创意园</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>2024.05.01 10:00-05.02 17:00</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>76</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="H30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=78657&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2024.05.01</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
           <t>上海·魔都野良神only</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>南京东路830号 第一百货</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="E31" t="inlineStr">
         <is>
           <t>2024.05.01 10:00-05.01 17:00</t>
         </is>
       </c>
-      <c r="F30" t="n">
-        <v>57</v>
-      </c>
-      <c r="G30" t="inlineStr">
+      <c r="F31" t="n">
+        <v>61</v>
+      </c>
+      <c r="G31" t="inlineStr">
         <is>
           <t>79</t>
         </is>
       </c>
-      <c r="H30" t="b">
-        <v>0</v>
-      </c>
-      <c r="I30" t="inlineStr">
+      <c r="H31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80321&amp;msource=Msearch_colligation</t>
         </is>
@@ -2292,7 +2333,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -2415,7 +2456,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -2520,7 +2561,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1668</v>
+        <v>1671</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -2643,7 +2684,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1771</v>
+        <v>1772</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -2684,7 +2725,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1779</v>
+        <v>1782</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -2766,7 +2807,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -2807,7 +2848,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -2912,7 +2953,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1668</v>
+        <v>1671</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -3076,7 +3117,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1771</v>
+        <v>1772</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -3117,7 +3158,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>1779</v>
+        <v>1782</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -3240,7 +3281,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -3322,7 +3363,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -3404,7 +3445,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -3486,7 +3527,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -3527,7 +3568,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -3568,7 +3609,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -3609,7 +3650,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>1156</v>
+        <v>1164</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -3650,7 +3691,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>683</v>
+        <v>691</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -3691,7 +3732,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -3814,7 +3855,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>750</v>
+        <v>753</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -3855,7 +3896,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -3896,7 +3937,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -4142,7 +4183,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -4183,7 +4224,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -4265,7 +4306,7 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>1508</v>
+        <v>1519</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -4347,7 +4388,7 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -4429,7 +4470,7 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -4470,7 +4511,7 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -4511,7 +4552,7 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>2217</v>
+        <v>2221</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -4593,7 +4634,7 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -4634,7 +4675,7 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -4716,7 +4757,7 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -4757,7 +4798,7 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -4798,7 +4839,7 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update gh-pages to output generated at 4e2132f
</commit_message>
<xml_diff>
--- a/上海-漫展信息.xlsx
+++ b/上海-漫展信息.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -629,7 +629,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1567</v>
+        <v>1569</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -656,25 +656,25 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>上海 ·WOW潮元 原神主题二次元音乐派对</t>
+          <t>上海·代号鸢广陵江东联合only</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>政通路189号五角场万达广场C栋 元气森林livehouse</t>
+          <t>逸仙路270号  上海宝丰联大酒店</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2024.01.13 14:00-01.13 19:00</t>
+          <t>2024.01.13 10:00-01.13 18:00</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>153</v>
+        <v>225</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>129</t>
+          <t>88</t>
         </is>
       </c>
       <c r="H6" t="b">
@@ -682,7 +682,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80167&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79877&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -697,25 +697,25 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>上海·代号鸢广陵江东联合only</t>
+          <t>上海·月遇国乙+代号鸢only</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>逸仙路270号  上海宝丰联大酒店</t>
+          <t>汶水路40号 格乐利雅GALLERIA艺术中心(大宁店)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2024.01.13 10:00-01.13 18:00</t>
+          <t>2024.01.13 10:40-01.13 21:00</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>219</v>
+        <v>384</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>95</t>
         </is>
       </c>
       <c r="H7" t="b">
@@ -723,7 +723,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79877&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79833&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -738,25 +738,25 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>上海·月遇国乙+代号鸢only</t>
+          <t>上海·灵能百分百ONLY</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>汶水路40号 格乐利雅GALLERIA艺术中心(大宁店)</t>
+          <t>长江路258号 中成智谷</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2024.01.13 10:40-01.13 21:00</t>
+          <t>2024.01.13 10:00-01.13 16:30</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>380</v>
+        <v>248</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>79</t>
         </is>
       </c>
       <c r="H8" t="b">
@@ -764,7 +764,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79833&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80008&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -779,25 +779,25 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>上海·灵能百分百ONLY</t>
+          <t>上海·第五十二届妖漫动漫游戏展</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>长江路258号 中成智谷</t>
+          <t>漕溪北路339号百脑汇4楼 百脑汇</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2024.01.13 10:00-01.13 16:30</t>
+          <t>2024.01.13 11:00-01.14 18:00</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>242</v>
+        <v>1178</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>19</t>
         </is>
       </c>
       <c r="H9" t="b">
@@ -805,7 +805,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80008&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80235&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -820,25 +820,25 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>上海·第五十二届妖漫动漫游戏展</t>
+          <t>上海·第五十届燃梦星辰动漫展-原X铁X崩免费同好交流会</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>漕溪北路339号百脑汇4楼 百脑汇</t>
+          <t>云台路800号 亿丰时代广场</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2024.01.13 11:00-01.14 18:00</t>
+          <t>2024.01.13 11:00-01.14 16:30</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>1164</v>
+        <v>700</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>58</t>
         </is>
       </c>
       <c r="H10" t="b">
@@ -846,7 +846,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80235&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80382&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -856,30 +856,30 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2024.01.13</t>
+          <t>2024.01.14</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>上海·第五十届燃梦星辰动漫展-原X铁X崩免费同好交流会</t>
+          <t>上海·1.14想见你光夜only</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>云台路800号 亿丰时代广场</t>
+          <t>汶水路210号 日本嘉美麓德婚礼公馆(大宁店)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2024.01.13 11:00-01.14 16:30</t>
+          <t>2024.01.14 09:30-01.14 21:30</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>691</v>
+        <v>465</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>68</t>
         </is>
       </c>
       <c r="H11" t="b">
@@ -887,7 +887,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80382&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79284&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -897,30 +897,30 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2024.01.14</t>
+          <t>2024.01.20</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>上海·1.14想见你光夜only</t>
+          <t>上海·坏孩纸物语の第31届动漫节之寒假篇</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>汶水路210号 日本嘉美麓德婚礼公馆(大宁店)</t>
+          <t>东大名路1118号(提篮桥地铁站1号口步行340米) 影梦里</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2024.01.14 09:30-01.14 21:30</t>
+          <t>2024.01.20 11:00-01.20 17:00</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>458</v>
+        <v>170</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>49</t>
         </is>
       </c>
       <c r="H12" t="b">
@@ -928,7 +928,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79284&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80597&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>753</v>
+        <v>764</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -998,7 +998,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1039,7 +1039,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1080,7 +1080,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1121,7 +1121,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1203,7 +1203,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1244,7 +1244,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>295</v>
+        <v>306</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1271,25 +1271,25 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>上海·Comic World动漫游园会</t>
+          <t>上海 ·WOW潮元原神x星铁主题二次元狂欢派对</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>康梧路519号2门 猩际野球室内足球馆</t>
+          <t>政通路189号五角场万达广场C栋 元气森林livehouse</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2024.01.28 09:30-01.28 17:00</t>
+          <t>2024.01.28 14:00-01.28 19:00</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>1519</v>
+        <v>156</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>109</t>
         </is>
       </c>
       <c r="H21" t="b">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78523&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80167&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1307,30 +1307,30 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2024.01.31</t>
+          <t>2024.01.28</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>上海·寻迹冬日LOVELIVE同好会</t>
+          <t>上海·Comic World动漫游园会</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>愚园路1250号 新歌空间</t>
+          <t>康梧路519号2门 猩际野球室内足球馆</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2024.01.31 11:30-01.31 17:00</t>
+          <t>2024.01.28 09:30-01.28 17:00</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>139</v>
+        <v>1560</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>70</t>
         </is>
       </c>
       <c r="H22" t="b">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79332&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78523&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1348,30 +1348,30 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2024.02.03</t>
+          <t>2024.01.31</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>上海·第七届次元鹿角动漫游戏展</t>
+          <t>上海·寻迹冬日LOVELIVE同好会</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>长宁路1191号长宁来福士B1 长宁来福士</t>
+          <t>愚园路1250号 新歌空间</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2024.02.03 10:00-02.04 17:00</t>
+          <t>2024.01.31 11:30-01.31 17:00</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>72</v>
+        <v>139</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>83</t>
         </is>
       </c>
       <c r="H23" t="b">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79938&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79332&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1389,30 +1389,30 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2024.02.16</t>
+          <t>2024.02.03</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>上海·第九届次元鹿角动漫游戏展</t>
+          <t>上海·第七届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
+          <t>长宁路1191号长宁来福士B1 长宁来福士</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2024.02.16 11:00-02.17 18:00</t>
+          <t>2024.02.03 10:00-02.04 17:00</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>68</t>
         </is>
       </c>
       <c r="H24" t="b">
@@ -1420,7 +1420,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80497&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79938&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1430,30 +1430,30 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2024.02.24</t>
+          <t>2024.02.16</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>上海·SISP动漫游戏嘉年华</t>
+          <t>上海·第九届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>年家浜路518号 周浦万达广场</t>
+          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2024.02.24 13:00-02.25 19:00</t>
+          <t>2024.02.16 11:00-02.17 18:00</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H25" t="b">
@@ -1461,7 +1461,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80339&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80497&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1476,33 +1476,33 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>上海·第三届燃梦BACG PRO游戏动漫展</t>
+          <t>上海·SISP动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
+          <t>年家浜路518号 周浦万达广场</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2024.02.24 11:00-02.25 16:30</t>
+          <t>2024.02.24 13:00-02.25 19:00</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>2221</v>
+        <v>55</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>48</t>
         </is>
       </c>
       <c r="H26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77754&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80339&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1512,38 +1512,38 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2024.03.02</t>
+          <t>2024.02.24</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>上海·原神X星穹铁道ONLY</t>
+          <t>上海·第三届燃梦BACG PRO游戏动漫展</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>逸仙路301号靠纪念路路口 上海宝丰联大酒店</t>
+          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2024.03.02 10:00-03.02 17:00</t>
+          <t>2024.02.24 11:00-02.25 16:30</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>118</v>
+        <v>2228</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80299&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=77754&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1553,30 +1553,30 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2024.03.09</t>
+          <t>2024.03.02</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
+          <t>上海·原神X星穹铁道ONLY</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>漕宝路1688号 诺宝中心酒店</t>
+          <t>逸仙路301号靠纪念路路口 上海宝丰联大酒店</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2024.03.09 10:00-03.09 16:30</t>
+          <t>2024.03.02 10:00-03.02 17:00</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>779</v>
+        <v>119</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>60</t>
         </is>
       </c>
       <c r="H28" t="b">
@@ -1584,7 +1584,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=76410&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80299&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1594,26 +1594,26 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2024.04.05</t>
+          <t>2024.03.03</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>上海·第四届次元鹿角动漫游戏展</t>
+          <t>上海·怀旧番ONLY</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>顾村镇蕰川路6号 智慧湾科创园</t>
+          <t>逸仙路270号  上海宝丰联大酒店</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2024.04.05 10:00-04.06 17:00</t>
+          <t>2024.03.03 10:00-03.03 17:00</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1625,7 +1625,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78228&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80575&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1635,38 +1635,38 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2024.05.01</t>
+          <t>2024.03.09</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>上海·  第五十三届妖漫动漫游戏展</t>
+          <t>上海·第五十三届燃梦星辰动漫嘉年华-随机宅舞</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>安蒲汇塘路50号 安垦徐汇创意园</t>
+          <t>周家嘴路3608号 宝龙旭辉广场</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2024.05.01 10:00-05.02 17:00</t>
+          <t>2024.03.09 10:20-03.10 16:30</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>58</t>
         </is>
       </c>
       <c r="H30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78657&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80571&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1676,36 +1676,159 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
+          <t>2024.03.09</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>漕宝路1688号 诺宝中心酒店</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>2024.03.09 10:00-03.09 16:30</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>783</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="H31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=76410&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2024.04.05</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>上海·第四届次元鹿角动漫游戏展</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>顾村镇蕰川路6号 智慧湾科创园</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>2024.04.05 10:00-04.06 17:00</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>53</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="H32" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=78228&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
           <t>2024.05.01</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>上海·  第五十三届妖漫动漫游戏展</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>安蒲汇塘路50号 安垦徐汇创意园</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>2024.05.01 10:00-05.02 17:00</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>77</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="H33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=78657&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2024.05.01</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
         <is>
           <t>上海·魔都野良神only</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>南京东路830号 第一百货</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>2024.05.01 10:00-05.01 17:00</t>
         </is>
       </c>
-      <c r="F31" t="n">
-        <v>61</v>
-      </c>
-      <c r="G31" t="inlineStr">
+      <c r="F34" t="n">
+        <v>72</v>
+      </c>
+      <c r="G34" t="inlineStr">
         <is>
           <t>79</t>
         </is>
       </c>
-      <c r="H31" t="b">
-        <v>0</v>
-      </c>
-      <c r="I31" t="inlineStr">
+      <c r="H34" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80321&amp;msource=Msearch_colligation</t>
         </is>
@@ -1800,7 +1923,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -1841,7 +1964,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -1909,7 +2032,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>上海 |【经典回归】2024等爱重启《女人万岁》舞台剧</t>
+          <t>上海 |【经典回归】2024等爱重启《女人万岁》舞台剧（取消）</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1927,7 +2050,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>180</t>
+          <t>不可售</t>
         </is>
       </c>
       <c r="H5" t="b">
@@ -2046,7 +2169,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -2169,7 +2292,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -2292,7 +2415,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -2333,7 +2456,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -2456,7 +2579,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -2561,7 +2684,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1671</v>
+        <v>1672</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -2684,7 +2807,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1772</v>
+        <v>1778</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -2725,7 +2848,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1782</v>
+        <v>1789</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -2766,7 +2889,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -2807,7 +2930,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -2848,7 +2971,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -2953,7 +3076,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1671</v>
+        <v>1672</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -3117,7 +3240,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1772</v>
+        <v>1778</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -3158,7 +3281,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>1782</v>
+        <v>1789</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -3199,7 +3322,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -3281,7 +3404,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>1567</v>
+        <v>1569</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -3303,12 +3426,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2023.12.27</t>
+          <t>2023.12.25</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>上海·爱乐汇《天空之城》久石让&amp;宫崎骏动漫经典音乐作品演奏会</t>
+          <t>上海·爱乐汇“浪漫经典·一生必听”永恒精选2023烛光音乐会</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -3318,11 +3441,11 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2023.12.27 19:30-2024.02.03 12:00</t>
+          <t>2023.12.25 19:30-2024.02.27 21:00</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -3334,7 +3457,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80103&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80057&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3344,30 +3467,30 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2023.12.31</t>
+          <t>2023.12.27</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>上海·次元波板糖×时光代理人「锦瑟华年主题快闪店」</t>
+          <t>上海·爱乐汇《天空之城》久石让&amp;宫崎骏动漫经典音乐作品演奏会</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>西藏北路166静安大悦城北座6楼611号 次元波板糖</t>
+          <t>南京西路1376号 上海商城剧院</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2023.12.31 00:00-2024.01.29 23:59</t>
+          <t>2023.12.27 19:30-2024.02.03 12:00</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>586</v>
+        <v>27</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>90</t>
         </is>
       </c>
       <c r="H12" t="b">
@@ -3375,7 +3498,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79972&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80103&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3385,30 +3508,30 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2024.01.01</t>
+          <t>2023.12.31</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>上海·沉浸式悬念剧场《9号秘事》</t>
+          <t>上海·次元波板糖×时光代理人「锦瑟华年主题快闪店」</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>人民大道300号 上海大剧院</t>
+          <t>西藏北路166静安大悦城北座6楼611号 次元波板糖</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2024.01.01 19:30-01.28 16:20</t>
+          <t>2023.12.31 00:00-2024.01.29 23:59</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>41</v>
+        <v>588</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>489</t>
+          <t>30</t>
         </is>
       </c>
       <c r="H13" t="b">
@@ -3416,7 +3539,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79939&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79972&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3426,30 +3549,30 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2024.01.06</t>
+          <t>2024.01.01</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>上海·罗小黑 x HAPPY ZOO主题Cafe</t>
+          <t>上海·沉浸式悬念剧场《9号秘事》</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>南京东路340号 百联zx创趣场</t>
+          <t>人民大道300号 上海大剧院</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2024.01.06 00:00-01.31 23:59</t>
+          <t>2024.01.01 19:30-01.28 16:20</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>463</v>
+        <v>41</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>489</t>
         </is>
       </c>
       <c r="H14" t="b">
@@ -3457,7 +3580,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80171&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79939&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3467,30 +3590,30 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2024.01.13</t>
+          <t>2024.01.06</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>上海 ·WOW潮元 原神主题二次元音乐派对</t>
+          <t>上海·罗小黑 x HAPPY ZOO主题Cafe</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>政通路189号五角场万达广场C栋 元气森林livehouse</t>
+          <t>南京东路340号 百联zx创趣场</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2024.01.13 14:00-01.13 19:00</t>
+          <t>2024.01.06 00:00-01.31 23:59</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>153</v>
+        <v>469</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>129</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H15" t="b">
@@ -3498,7 +3621,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80167&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80171&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3513,25 +3636,25 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>上海·代号鸢广陵江东联合only</t>
+          <t>上海·月遇国乙+代号鸢only</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>逸仙路270号  上海宝丰联大酒店</t>
+          <t>汶水路40号 格乐利雅GALLERIA艺术中心(大宁店)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2024.01.13 10:00-01.13 18:00</t>
+          <t>2024.01.13 10:40-01.13 21:00</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>219</v>
+        <v>384</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>95</t>
         </is>
       </c>
       <c r="H16" t="b">
@@ -3539,7 +3662,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79877&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79833&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3554,25 +3677,25 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>上海·月遇国乙+代号鸢only</t>
+          <t>上海·灵能百分百ONLY</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>汶水路40号 格乐利雅GALLERIA艺术中心(大宁店)</t>
+          <t>长江路258号 中成智谷</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2024.01.13 10:40-01.13 21:00</t>
+          <t>2024.01.13 10:00-01.13 16:30</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>380</v>
+        <v>248</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>79</t>
         </is>
       </c>
       <c r="H17" t="b">
@@ -3580,7 +3703,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79833&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80008&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3595,25 +3718,25 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>上海·灵能百分百ONLY</t>
+          <t>上海·第五十二届妖漫动漫游戏展</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>长江路258号 中成智谷</t>
+          <t>漕溪北路339号百脑汇4楼 百脑汇</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2024.01.13 10:00-01.13 16:30</t>
+          <t>2024.01.13 11:00-01.14 18:00</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>242</v>
+        <v>1178</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>19</t>
         </is>
       </c>
       <c r="H18" t="b">
@@ -3621,7 +3744,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80008&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80235&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3636,25 +3759,25 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>上海·第五十二届妖漫动漫游戏展</t>
+          <t>上海·第五十届燃梦星辰动漫展-原X铁X崩免费同好交流会</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>漕溪北路339号百脑汇4楼 百脑汇</t>
+          <t>云台路800号 亿丰时代广场</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2024.01.13 11:00-01.14 18:00</t>
+          <t>2024.01.13 11:00-01.14 16:30</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>1164</v>
+        <v>700</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>58</t>
         </is>
       </c>
       <c r="H19" t="b">
@@ -3662,7 +3785,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80235&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80382&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3672,30 +3795,30 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2024.01.13</t>
+          <t>2024.01.14</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>上海·第五十届燃梦星辰动漫展-原X铁X崩免费同好交流会</t>
+          <t>上海·1.14想见你光夜only</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>云台路800号 亿丰时代广场</t>
+          <t>汶水路210号 日本嘉美麓德婚礼公馆(大宁店)</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2024.01.13 11:00-01.14 16:30</t>
+          <t>2024.01.14 09:30-01.14 21:30</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>691</v>
+        <v>465</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>68</t>
         </is>
       </c>
       <c r="H20" t="b">
@@ -3703,7 +3826,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80382&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79284&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3713,38 +3836,38 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2024.01.14</t>
+          <t>2024.01.19</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>上海·1.14想见你光夜only</t>
+          <t>上海·音乐剧《三星堆》</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>汶水路210号 日本嘉美麓德婚礼公馆(大宁店)</t>
+          <t>汾阳路6号 上音歌剧院</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2024.01.14 09:30-01.14 21:30</t>
+          <t>2024.01.19 19:30-01.21 22:00</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>458</v>
+        <v>12</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>180</t>
         </is>
       </c>
       <c r="H21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79284&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79832&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3754,38 +3877,38 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2024.01.19</t>
+          <t>2024.01.20</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>上海·音乐剧《三星堆》</t>
+          <t>上海·奥井雅美出道突破30周年演唱会</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>汾阳路6号 上音歌剧院</t>
+          <t>宜昌路179号 万代南梦宫上海文化中心</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2024.01.19 19:30-01.21 22:00</t>
+          <t>2024.01.20 18:30-01.20 20:10</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>180</t>
+          <t>480</t>
         </is>
       </c>
       <c r="H22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79832&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80373&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3800,25 +3923,25 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>上海·奥井雅美出道突破30周年演唱会</t>
+          <t>上海·排球少年X蓝锁X灌篮ONLY</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>宜昌路179号 万代南梦宫上海文化中心</t>
+          <t>逸仙路270号  上海宝丰联大酒店</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2024.01.20 18:30-01.20 20:10</t>
+          <t>2024.01.20 10:00-01.20 17:00</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>15</v>
+        <v>764</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>480</t>
+          <t>60</t>
         </is>
       </c>
       <c r="H23" t="b">
@@ -3826,7 +3949,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80373&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79261&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3841,12 +3964,12 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>上海·排球少年X蓝锁X灌篮ONLY</t>
+          <t>上海·赛马娘party·华亭迎春</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>逸仙路270号  上海宝丰联大酒店</t>
+          <t>淞宝路96号化成路淞宝路 新长江大酒店</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -3855,7 +3978,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>753</v>
+        <v>84</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -3867,7 +3990,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79261&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80384&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3882,25 +4005,25 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>上海·赛马娘party·华亭迎春</t>
+          <t>上海·霓虹次元·运动番ONLY夜场2.0</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>淞宝路96号化成路淞宝路 新长江大酒店</t>
+          <t>万航渡路849号海森国际大厦3楼 Miss Club</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2024.01.20 10:00-01.20 17:00</t>
+          <t>2024.01.20 16:30-01.20 21:30</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>81</v>
+        <v>233</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>168</t>
         </is>
       </c>
       <c r="H25" t="b">
@@ -3908,7 +4031,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80384&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80234&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3918,38 +4041,38 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2024.01.20</t>
+          <t>2024.01.23</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>上海·霓虹次元·运动番ONLY夜场2.0</t>
+          <t>上海·七音阿卡莉 NANAOAKARI 2024 专场演出</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>万航渡路849号海森国际大厦3楼 Miss Club</t>
+          <t>嘉兴路街道瑞虹路188号瑞虹天地月亮湾3层 Modern Sky LAB摩登天空(瑞虹天地店)</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2024.01.20 16:30-01.20 21:30</t>
+          <t>2024.01.23 20:00-01.23 22:00</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>225</v>
+        <v>74</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>168</t>
+          <t>380</t>
         </is>
       </c>
       <c r="H26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80234&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79641&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3959,30 +4082,30 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2024.01.23</t>
+          <t>2024.01.26</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>上海·七音阿卡莉 NANAOAKARI 2024 专场演出</t>
+          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>嘉兴路街道瑞虹路188号瑞虹天地月亮湾3层 Modern Sky LAB摩登天空(瑞虹天地店)</t>
+          <t>丁香路425号 上海东方艺术中心</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2024.01.23 20:00-01.23 22:00</t>
+          <t>2024.01.26 19:30-01.26 21:30</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>80</t>
         </is>
       </c>
       <c r="H27" t="b">
@@ -3990,7 +4113,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79641&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78418&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -4000,38 +4123,38 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2024.01.26</t>
+          <t>2024.01.27</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
+          <t>上海·Azurock」Azurose ACG Cover Live</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>丁香路425号 上海东方艺术中心</t>
+          <t>愚园路1398号 育音堂音乐公园</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2024.01.26 19:30-01.26 21:30</t>
+          <t>2024.01.27 19:00-01.27 21:30</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>132</v>
+        <v>34</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>88</t>
         </is>
       </c>
       <c r="H28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78418&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80277&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -4046,25 +4169,25 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>上海·Azurock」Azurose ACG Cover Live</t>
+          <t>上海·SISPmini动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>愚园路1398号 育音堂音乐公园</t>
+          <t>淞虹路377号 长宁ArtPark大融城</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2024.01.27 19:00-01.27 21:30</t>
+          <t>2024.01.27 13:00-01.28 19:00</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>34</v>
+        <v>187</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>48</t>
         </is>
       </c>
       <c r="H29" t="b">
@@ -4072,7 +4195,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80277&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79046&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -4087,25 +4210,25 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>上海·SISPmini动漫游戏嘉年华</t>
+          <t>上海·同好召集令火影only</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>淞虹路377号 长宁ArtPark大融城</t>
+          <t>市真南路1199弄1号 智创TOP综合体产城</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2024.01.27 13:00-01.28 19:00</t>
+          <t>2024.01.27 10:00-01.28 18:00</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>183</v>
+        <v>253</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>78</t>
         </is>
       </c>
       <c r="H30" t="b">
@@ -4113,7 +4236,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79046&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80284&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -4128,25 +4251,25 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>上海·同好召集令火影only</t>
+          <t>上海·咒术only-幽暗之森1.0</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>市真南路1199弄1号 智创TOP综合体产城</t>
+          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.28 18:00</t>
+          <t>2024.01.27 10:00-01.27 16:00</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>246</v>
+        <v>161</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>59</t>
         </is>
       </c>
       <c r="H31" t="b">
@@ -4154,7 +4277,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80284&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80045&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -4169,7 +4292,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>上海·咒术only-幽暗之森1.0</t>
+          <t>上海·魔都寒假漫展-CF01</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -4179,15 +4302,15 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.27 16:00</t>
+          <t>2024.01.27 10:00-01.28 16:00</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>157</v>
+        <v>306</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>49</t>
         </is>
       </c>
       <c r="H32" t="b">
@@ -4195,7 +4318,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80045&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80204&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -4210,33 +4333,33 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>上海·魔都寒假漫展-CF01</t>
+          <t>上海•Risa Yuzuki 1st ONEMAN LIVE 「Future Interlink」 追加公演</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
+          <t>愚园路1250号 新歌空间</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.28 16:00</t>
+          <t>2024.01.27 18:30-01.27 21:00</t>
         </is>
       </c>
       <c r="F33" t="n">
-        <v>295</v>
+        <v>270</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>278</t>
         </is>
       </c>
       <c r="H33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80204&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=77773&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -4246,38 +4369,38 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2024.01.27</t>
+          <t>2024.01.28</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>上海•Risa Yuzuki 1st ONEMAN LIVE 「Future Interlink」 追加公演</t>
+          <t>上海 ·WOW潮元原神x星铁主题二次元狂欢派对</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>愚园路1250号 新歌空间</t>
+          <t>政通路189号五角场万达广场C栋 元气森林livehouse</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2024.01.27 18:30-01.27 21:00</t>
+          <t>2024.01.28 14:00-01.28 19:00</t>
         </is>
       </c>
       <c r="F34" t="n">
-        <v>268</v>
+        <v>156</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>278</t>
+          <t>109</t>
         </is>
       </c>
       <c r="H34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77773&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80167&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -4306,7 +4429,7 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>1519</v>
+        <v>1560</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -4388,7 +4511,7 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -4429,7 +4552,7 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -4470,7 +4593,7 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -4511,7 +4634,7 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -4552,7 +4675,7 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>2221</v>
+        <v>2228</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -4634,7 +4757,7 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -4675,7 +4798,7 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>779</v>
+        <v>783</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -4757,7 +4880,7 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -4798,7 +4921,7 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -4839,7 +4962,7 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update gh-pages to output generated at 74db155
</commit_message>
<xml_diff>
--- a/上海-漫展信息.xlsx
+++ b/上海-漫展信息.xlsx
@@ -711,7 +711,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -793,7 +793,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>1178</v>
+        <v>1184</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -834,7 +834,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -875,7 +875,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -916,7 +916,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>170</v>
+        <v>202</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>764</v>
+        <v>767</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -998,7 +998,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1080,11 +1080,11 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>68</t>
         </is>
       </c>
       <c r="H16" t="b">
@@ -1121,7 +1121,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1244,7 +1244,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1285,7 +1285,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1326,7 +1326,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>1560</v>
+        <v>1569</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1367,7 +1367,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1408,7 +1408,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1531,7 +1531,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>2228</v>
+        <v>2229</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1572,7 +1572,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1613,7 +1613,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1818,7 +1818,7 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -2456,7 +2456,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -2497,7 +2497,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -2889,7 +2889,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -3322,7 +3322,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -3650,7 +3650,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -3732,7 +3732,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>1178</v>
+        <v>1184</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -3773,7 +3773,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -3814,7 +3814,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -3937,7 +3937,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>764</v>
+        <v>767</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -3978,7 +3978,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -4183,7 +4183,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -4224,7 +4224,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -4306,7 +4306,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -4388,7 +4388,7 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -4429,7 +4429,7 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>1560</v>
+        <v>1569</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -4470,7 +4470,7 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -4511,7 +4511,7 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -4552,7 +4552,7 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -4675,7 +4675,7 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>2228</v>
+        <v>2229</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -4716,7 +4716,7 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -4757,7 +4757,7 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -4962,7 +4962,7 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update gh-pages to output generated at 2291077
</commit_message>
<xml_diff>
--- a/上海-漫展信息.xlsx
+++ b/上海-漫展信息.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,6 +480,11 @@
           <t>Link</t>
         </is>
       </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Cover</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -521,6 +526,11 @@
           <t>https://show.bilibili.com/platform/detail.html?id=77862&amp;msource=Msearch_colligation</t>
         </is>
       </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202310/QnmD4yOd1698652192047.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -562,6 +572,11 @@
           <t>https://show.bilibili.com/platform/detail.html?id=78203&amp;msource=Msearch_colligation</t>
         </is>
       </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202311/myyekKWe1699337305424.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -603,6 +618,11 @@
           <t>https://show.bilibili.com/platform/detail.html?id=78809&amp;msource=Msearch_colligation</t>
         </is>
       </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202311/YsBoZAOW1700551290654.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -629,7 +649,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1572</v>
+        <v>1578</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -642,6 +662,11 @@
       <c r="I5" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79166&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202311/MjTiIYlk1701242361853.jpeg</t>
         </is>
       </c>
     </row>
@@ -670,7 +695,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -683,6 +708,11 @@
       <c r="I6" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79877&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/RoaxwRJq1703729569231.png</t>
         </is>
       </c>
     </row>
@@ -711,7 +741,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -724,6 +754,11 @@
       <c r="I7" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79833&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/Ca51ySIK1702607429682.jpeg</t>
         </is>
       </c>
     </row>
@@ -752,7 +787,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -765,6 +800,11 @@
       <c r="I8" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80008&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/rSR9XSX01703041035213.jpeg</t>
         </is>
       </c>
     </row>
@@ -793,7 +833,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>1194</v>
+        <v>1224</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -806,6 +846,11 @@
       <c r="I9" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80235&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/VytCJsEX1703647558135.jpeg</t>
         </is>
       </c>
     </row>
@@ -834,7 +879,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>708</v>
+        <v>723</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -847,6 +892,11 @@
       <c r="I10" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80382&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/FIZYJ68n1704179640046.jpeg</t>
         </is>
       </c>
     </row>
@@ -875,7 +925,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>471</v>
+        <v>478</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -888,6 +938,11 @@
       <c r="I11" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79284&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/zsveqtuG1701764030936.jpeg</t>
         </is>
       </c>
     </row>
@@ -916,7 +971,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>210</v>
+        <v>232</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -929,6 +984,11 @@
       <c r="I12" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80597&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/UoNyFL4G1704707294378.png</t>
         </is>
       </c>
     </row>
@@ -957,7 +1017,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>775</v>
+        <v>782</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -970,6 +1030,11 @@
       <c r="I13" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79261&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/mmvCkYYH1701411372879.jpeg</t>
         </is>
       </c>
     </row>
@@ -984,21 +1049,21 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>上海·赛马娘party·华亭迎春</t>
+          <t>上海·次元裂缝-X Anikura二次元迎春派对</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>淞宝路96号化成路淞宝路 新长江大酒店</t>
+          <t>海潮路133号B1 JUMP工坊</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2024.01.20 10:00-01.20 17:00</t>
+          <t>2024.01.20 14:00-01.20 22:00</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1010,7 +1075,12 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80384&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80638&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/N7gT4Tza1704782642832.jpeg</t>
         </is>
       </c>
     </row>
@@ -1025,25 +1095,25 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>上海·霓虹次元·运动番ONLY夜场2.0</t>
+          <t>上海·赛马娘party·华亭迎春</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>万航渡路849号海森国际大厦3楼 Miss Club</t>
+          <t>淞宝路96号化成路淞宝路 新长江大酒店</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2024.01.20 16:30-01.20 21:30</t>
+          <t>2024.01.20 10:00-01.20 17:00</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>238</v>
+        <v>94</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>168</t>
+          <t>60</t>
         </is>
       </c>
       <c r="H15" t="b">
@@ -1051,7 +1121,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80234&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80384&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/JHXTpHAw1704181759660.jpeg</t>
         </is>
       </c>
     </row>
@@ -1061,30 +1136,30 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2024.01.27</t>
+          <t>2024.01.20</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>上海·25时主题同人茶会</t>
+          <t>上海·霓虹次元·运动番ONLY夜场2.0</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>沪太路3100号 尚大国际</t>
+          <t>万航渡路849号海森国际大厦3楼 Miss Club</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2024.01.27 12:00-01.27 18:00</t>
+          <t>2024.01.20 16:30-01.20 21:30</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>22</v>
+        <v>251</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>168</t>
         </is>
       </c>
       <c r="H16" t="b">
@@ -1092,7 +1167,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80548&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80234&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/Idm7h4dK1703646683782.jpeg</t>
         </is>
       </c>
     </row>
@@ -1107,25 +1187,25 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>上海·SISPmini动漫游戏嘉年华</t>
+          <t>上海·25时主题同人茶会</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>淞虹路377号 长宁ArtPark大融城</t>
+          <t>沪太路3100号 尚大国际</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2024.01.27 13:00-01.28 19:00</t>
+          <t>2024.01.27 12:00-01.27 18:00</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>188</v>
+        <v>30</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>68</t>
         </is>
       </c>
       <c r="H17" t="b">
@@ -1133,7 +1213,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79046&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80548&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/dQ4DrxCk1704683144116.png</t>
         </is>
       </c>
     </row>
@@ -1148,25 +1233,25 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>上海·同好召集令火影only</t>
+          <t>上海·SISPmini动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>市真南路1199弄1号 智创TOP综合体产城</t>
+          <t>淞虹路377号 长宁ArtPark大融城</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.28 18:00</t>
+          <t>2024.01.27 13:00-01.28 19:00</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>270</v>
+        <v>192</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>48</t>
         </is>
       </c>
       <c r="H18" t="b">
@@ -1174,7 +1259,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80284&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79046&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202311/XmP03Vf31701070803044.jpeg</t>
         </is>
       </c>
     </row>
@@ -1189,25 +1279,25 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>上海·咒术only-幽暗之森1.0</t>
+          <t>上海·同好召集令火影only</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
+          <t>市真南路1199弄1号 智创TOP综合体产城</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.27 16:00</t>
+          <t>2024.01.27 10:00-01.28 18:00</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>165</v>
+        <v>301</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>78</t>
         </is>
       </c>
       <c r="H19" t="b">
@@ -1215,7 +1305,12 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80045&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80284&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/9xGb6MXN1704183627126.jpeg</t>
         </is>
       </c>
     </row>
@@ -1230,7 +1325,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>上海·魔都寒假漫展-CF01</t>
+          <t>上海·咒术only-幽暗之森1.0</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1240,15 +1335,15 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.28 16:00</t>
+          <t>2024.01.27 10:00-01.27 16:00</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>310</v>
+        <v>167</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>59</t>
         </is>
       </c>
       <c r="H20" t="b">
@@ -1256,7 +1351,12 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80204&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80045&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/hUfcrw3y1703055422885.jpeg</t>
         </is>
       </c>
     </row>
@@ -1266,30 +1366,30 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2024.01.28</t>
+          <t>2024.01.27</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>上海 ·WOW潮元原神x星铁主题二次元狂欢派对</t>
+          <t>上海·魔都寒假漫展-CF01</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>政通路189号五角场万达广场C栋 元气森林livehouse</t>
+          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2024.01.28 14:00-01.28 19:00</t>
+          <t>2024.01.27 10:00-01.28 16:00</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>160</v>
+        <v>327</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>109</t>
+          <t>49</t>
         </is>
       </c>
       <c r="H21" t="b">
@@ -1297,7 +1397,12 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80167&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80204&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/eK96fdcg1703573110264.jpeg</t>
         </is>
       </c>
     </row>
@@ -1312,25 +1417,25 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>上海·Comic World动漫游园会</t>
+          <t>上海 ·WOW潮元原神x星铁主题二次元狂欢派对</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>康梧路519号2门 猩际野球室内足球馆</t>
+          <t>政通路189号五角场万达广场C栋 元气森林livehouse</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2024.01.28 09:30-01.28 17:00</t>
+          <t>2024.01.28 14:00-01.28 19:00</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>1604</v>
+        <v>210</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>109</t>
         </is>
       </c>
       <c r="H22" t="b">
@@ -1338,7 +1443,12 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78523&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80167&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/cMpTD3gV1703571795332.png</t>
         </is>
       </c>
     </row>
@@ -1348,30 +1458,30 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2024.01.31</t>
+          <t>2024.01.28</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>上海·寻迹冬日LOVELIVE同好会</t>
+          <t>上海·Comic World动漫游园会</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>愚园路1250号 新歌空间</t>
+          <t>康梧路519号2门 猩际野球室内足球馆</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2024.01.31 11:30-01.31 17:00</t>
+          <t>2024.01.28 09:30-01.28 17:00</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>140</v>
+        <v>1679</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>70</t>
         </is>
       </c>
       <c r="H23" t="b">
@@ -1379,7 +1489,12 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79332&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78523&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202311/30WzGyPz1699943734625.jpeg</t>
         </is>
       </c>
     </row>
@@ -1389,30 +1504,30 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2024.02.03</t>
+          <t>2024.01.31</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>上海·第七届次元鹿角动漫游戏展</t>
+          <t>上海·寻迹冬日LOVELIVE同好会</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>长宁路1191号长宁来福士B1 长宁来福士</t>
+          <t>愚园路1250号 新歌空间</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2024.02.03 10:00-02.04 17:00</t>
+          <t>2024.01.31 11:30-01.31 17:00</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>76</v>
+        <v>143</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>83</t>
         </is>
       </c>
       <c r="H24" t="b">
@@ -1420,7 +1535,12 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79938&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79332&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/Ewreg1JT1701677993728.jpeg</t>
         </is>
       </c>
     </row>
@@ -1430,30 +1550,30 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2024.02.16</t>
+          <t>2024.02.03</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>上海·第九届次元鹿角动漫游戏展</t>
+          <t>上海·Coser迎春动漫展</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
+          <t>海潮路133号B1 JUMP工坊</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2024.02.16 11:00-02.17 18:00</t>
+          <t>2024.02.03 10:00-02.04 17:00</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>60</t>
         </is>
       </c>
       <c r="H25" t="b">
@@ -1461,7 +1581,12 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80497&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80646&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/4WVkFc4d1704787729064.jpeg</t>
         </is>
       </c>
     </row>
@@ -1471,30 +1596,30 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2024.02.24</t>
+          <t>2024.02.03</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>上海·SISP动漫游戏嘉年华</t>
+          <t>上海·第七届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>年家浜路518号 周浦万达广场</t>
+          <t>长宁路1191号长宁来福士B1 长宁来福士</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2024.02.24 13:00-02.25 19:00</t>
+          <t>2024.02.03 10:00-02.04 17:00</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>68</t>
         </is>
       </c>
       <c r="H26" t="b">
@@ -1502,7 +1627,12 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80339&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79938&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/TWEj0Z7l1702954736529.jpeg</t>
         </is>
       </c>
     </row>
@@ -1512,12 +1642,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2024.02.24</t>
+          <t>2024.02.16</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>上海·第三届燃梦BACG PRO游戏动漫展</t>
+          <t>上海·第九届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1527,11 +1657,11 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2024.02.24 11:00-02.25 16:30</t>
+          <t>2024.02.16 11:00-02.17 18:00</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>2239</v>
+        <v>1023</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1539,11 +1669,16 @@
         </is>
       </c>
       <c r="H27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77754&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80497&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/0duSXTQy1704423309244.jpeg</t>
         </is>
       </c>
     </row>
@@ -1553,30 +1688,30 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2024.03.02</t>
+          <t>2024.02.24</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>上海·原神X星穹铁道ONLY</t>
+          <t>上海·SISP动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>逸仙路301号靠纪念路路口 上海宝丰联大酒店</t>
+          <t>年家浜路518号 周浦万达广场</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2024.03.02 10:00-03.02 17:00</t>
+          <t>2024.02.24 13:00-02.25 19:00</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>122</v>
+        <v>58</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>48</t>
         </is>
       </c>
       <c r="H28" t="b">
@@ -1584,7 +1719,12 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80299&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80339&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/a8iuOufB1703832570508.jpeg</t>
         </is>
       </c>
     </row>
@@ -1594,38 +1734,43 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2024.03.03</t>
+          <t>2024.02.24</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>上海·怀旧番ONLY</t>
+          <t>上海·第三届燃梦BACG PRO游戏动漫展</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>逸仙路270号  上海宝丰联大酒店</t>
+          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2024.03.03 10:00-03.03 17:00</t>
+          <t>2024.02.24 11:00-02.25 16:30</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>21</v>
+        <v>2254</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80575&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=77754&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/7eGZETK91701943985671.jpeg</t>
         </is>
       </c>
     </row>
@@ -1635,38 +1780,43 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2024.03.09</t>
+          <t>2024.03.02</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>上海·第五十三届燃梦星辰动漫嘉年华-随机宅舞</t>
+          <t>上海·原神X星穹铁道ONLY</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>周家嘴路3608号 宝龙旭辉广场</t>
+          <t>逸仙路301号靠纪念路路口 上海宝丰联大酒店</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2024.03.09 10:20-03.10 16:30</t>
+          <t>2024.03.02 10:00-03.02 17:00</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>4</v>
+        <v>133</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>60</t>
         </is>
       </c>
       <c r="H30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80571&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80299&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/V0xu26Cl1703753850690.jpeg</t>
         </is>
       </c>
     </row>
@@ -1676,30 +1826,30 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2024.03.09</t>
+          <t>2024.03.03</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
+          <t>上海·怀旧番ONLY</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>漕宝路1688号 诺宝中心酒店</t>
+          <t>逸仙路270号  上海宝丰联大酒店</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2024.03.09 10:00-03.09 16:30</t>
+          <t>2024.03.03 10:00-03.03 17:00</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>783</v>
+        <v>36</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>60</t>
         </is>
       </c>
       <c r="H31" t="b">
@@ -1707,7 +1857,12 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=76410&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80575&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/y4uWdyPT1704700763902.jpeg</t>
         </is>
       </c>
     </row>
@@ -1717,38 +1872,43 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2024.04.05</t>
+          <t>2024.03.09</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>上海·第四届次元鹿角动漫游戏展</t>
+          <t>上海·第五十三届燃梦星辰动漫嘉年华-随机宅舞</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>顾村镇蕰川路6号 智慧湾科创园</t>
+          <t>周家嘴路3608号 宝龙旭辉广场</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2024.04.05 10:00-04.06 17:00</t>
+          <t>2024.03.09 10:20-03.10 16:30</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>58</t>
         </is>
       </c>
       <c r="H32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78228&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80571&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/SHH70VXN1704700240858.jpeg</t>
         </is>
       </c>
     </row>
@@ -1758,30 +1918,30 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2024.05.01</t>
+          <t>2024.03.09</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>上海·  第五十三届妖漫动漫游戏展</t>
+          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>安蒲汇塘路50号 安垦徐汇创意园</t>
+          <t>漕宝路1688号 诺宝中心酒店</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2024.05.01 10:00-05.02 17:00</t>
+          <t>2024.03.09 10:00-03.09 16:30</t>
         </is>
       </c>
       <c r="F33" t="n">
-        <v>79</v>
+        <v>785</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>73</t>
         </is>
       </c>
       <c r="H33" t="b">
@@ -1789,7 +1949,12 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78657&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=76410&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202309/fVXMrcHy1693971682397.jpeg</t>
         </is>
       </c>
     </row>
@@ -1799,38 +1964,135 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
+          <t>2024.04.05</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>上海·第四届次元鹿角动漫游戏展</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>顾村镇蕰川路6号 智慧湾科创园</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>2024.04.05 10:00-04.06 17:00</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>53</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="H34" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=78228&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202311/jgqIFxhx1699344723568.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
           <t>2024.05.01</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>上海·  第五十三届妖漫动漫游戏展</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>安蒲汇塘路50号 安垦徐汇创意园</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>2024.05.01 10:00-05.02 17:00</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>82</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="H35" t="b">
+        <v>0</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=78657&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202311/qGwPWLzO1700562869315.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2024.05.01</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
         <is>
           <t>上海·魔都野良神only</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>南京东路830号 第一百货</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="E36" t="inlineStr">
         <is>
           <t>2024.05.01 10:00-05.01 17:00</t>
         </is>
       </c>
-      <c r="F34" t="n">
-        <v>76</v>
-      </c>
-      <c r="G34" t="inlineStr">
+      <c r="F36" t="n">
+        <v>86</v>
+      </c>
+      <c r="G36" t="inlineStr">
         <is>
           <t>79</t>
         </is>
       </c>
-      <c r="H34" t="b">
-        <v>0</v>
-      </c>
-      <c r="I34" t="inlineStr">
+      <c r="H36" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80321&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/KBlb0enU1704358750268.jpeg</t>
         </is>
       </c>
     </row>
@@ -1845,7 +2107,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1897,6 +2159,11 @@
           <t>Link</t>
         </is>
       </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Cover</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -1938,6 +2205,11 @@
           <t>https://show.bilibili.com/platform/detail.html?id=80057&amp;msource=Msearch_colligation</t>
         </is>
       </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/AeWGG9Rk1703131189224.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -1964,7 +2236,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -1977,6 +2249,11 @@
       <c r="I3" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80103&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/2h2tIq7l1703144874867.png</t>
         </is>
       </c>
     </row>
@@ -2020,6 +2297,11 @@
           <t>https://show.bilibili.com/platform/detail.html?id=79939&amp;msource=Msearch_colligation</t>
         </is>
       </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/hY6FVnjM1702954652593.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -2061,6 +2343,11 @@
           <t>https://show.bilibili.com/platform/detail.html?id=79965&amp;msource=Msearch_colligation</t>
         </is>
       </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/uQ7J7kBt1702968901415.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -2102,6 +2389,11 @@
           <t>https://show.bilibili.com/platform/detail.html?id=79832&amp;msource=Msearch_colligation</t>
         </is>
       </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/aRlkZiIb1702607587670.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -2143,6 +2435,11 @@
           <t>https://show.bilibili.com/platform/detail.html?id=80101&amp;msource=Msearch_colligation</t>
         </is>
       </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/3iT86tbs1703142892633.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -2169,7 +2466,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -2182,6 +2479,11 @@
       <c r="I8" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80373&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/Ttzqeavz1704167763720.jpeg</t>
         </is>
       </c>
     </row>
@@ -2210,7 +2512,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -2223,6 +2525,11 @@
       <c r="I9" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79842&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/vptlHEg41702610098849.jpeg</t>
         </is>
       </c>
     </row>
@@ -2251,7 +2558,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -2264,6 +2571,11 @@
       <c r="I10" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79641&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/CoNbgCpO1703644783043.jpeg</t>
         </is>
       </c>
     </row>
@@ -2292,7 +2604,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -2305,6 +2617,11 @@
       <c r="I11" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=78418&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202311/GHpvkT5Y1699605760230.jpeg</t>
         </is>
       </c>
     </row>
@@ -2333,7 +2650,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -2346,6 +2663,11 @@
       <c r="I12" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80277&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/5d6O1Rf11703742965244.png</t>
         </is>
       </c>
     </row>
@@ -2389,6 +2711,11 @@
           <t>https://show.bilibili.com/platform/detail.html?id=79783&amp;msource=Msearch_colligation</t>
         </is>
       </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/S6nZ327b1702534484951.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -2415,7 +2742,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -2428,6 +2755,11 @@
       <c r="I14" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=77773&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202310/XKKYWAk51698315607196.png</t>
         </is>
       </c>
     </row>
@@ -2456,7 +2788,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>469</v>
+        <v>479</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -2469,6 +2801,11 @@
       <c r="I15" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80128&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/DEW1XYty1703226993965.jpeg</t>
         </is>
       </c>
     </row>
@@ -2478,30 +2815,30 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2024.02.25</t>
+          <t>2024.02.14</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>上海·青山吉能见面会</t>
+          <t>上海·【情人节特辑】《那年我们》记忆重启韩剧经典OST音乐会《请回答1988》《来自星星的你》</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>虹许路731号4号楼 THE BOXX•城市乐园</t>
+          <t>牛庄路704号 中国大戏院</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2024.02.25 14:30-02.25 19:30</t>
+          <t>2024.02.14 19:30-02.14 21:00</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>170</v>
+        <v>0</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>80</t>
         </is>
       </c>
       <c r="H16" t="b">
@@ -2509,7 +2846,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80142&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80615&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/5DDVhKcO1704767761361.png</t>
         </is>
       </c>
     </row>
@@ -2519,38 +2861,43 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2024.04.06</t>
+          <t>2024.02.25</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
+          <t>上海·青山吉能见面会</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>复兴中路1380号 捷豹上海交响音乐厅</t>
+          <t>虹许路731号4号楼 THE BOXX•城市乐园</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2024.04.06 19:30-04.06 21:30</t>
+          <t>2024.02.25 14:30-02.25 19:30</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>10</v>
+        <v>171</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>380</t>
         </is>
       </c>
       <c r="H17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80050&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80142&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/1npuHFBM1703231674558.jpeg</t>
         </is>
       </c>
     </row>
@@ -2560,26 +2907,26 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2024.04.13</t>
+          <t>2024.04.06</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>上海·《四月是你的谎言》——“公生”与“薰”的钢琴小提琴唯美经典音乐集</t>
+          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>丁香路425号 上海东方艺术中心</t>
+          <t>复兴中路1380号 捷豹上海交响音乐厅</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2024.04.13 19:30-04.13 21:30</t>
+          <t>2024.04.06 19:30-04.06 21:30</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>138</v>
+        <v>10</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -2591,7 +2938,58 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80050&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/0iJP3TY61703056498448.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2024.04.13</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>上海·《四月是你的谎言》——“公生”与“薰”的钢琴小提琴唯美经典音乐集</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>丁香路425号 上海东方艺术中心</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2024.04.13 19:30-04.13 21:30</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>140</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
           <t>https://show.bilibili.com/platform/detail.html?id=78667&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202311/bTP7w6GD1700130122940.jpeg</t>
         </is>
       </c>
     </row>
@@ -2606,7 +3004,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2658,6 +3056,11 @@
           <t>Link</t>
         </is>
       </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Cover</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -2684,7 +3087,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1674</v>
+        <v>1675</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -2697,6 +3100,11 @@
       <c r="I2" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=70666&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202106/okF9H2Uj1623911727887.jpeg</t>
         </is>
       </c>
     </row>
@@ -2740,6 +3148,11 @@
           <t>https://show.bilibili.com/platform/detail.html?id=77530&amp;msource=Msearch_colligation</t>
         </is>
       </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202310/JqP3lHJt1698030195136.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -2766,7 +3179,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -2779,6 +3192,11 @@
       <c r="I4" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79057&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/ASamaqBx1701419480253.jpeg</t>
         </is>
       </c>
     </row>
@@ -2807,7 +3225,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1783</v>
+        <v>1789</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -2820,6 +3238,11 @@
       <c r="I5" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79005&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202311/02P8eD3Z1700821985538.jpeg</t>
         </is>
       </c>
     </row>
@@ -2848,7 +3271,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1794</v>
+        <v>1809</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -2861,6 +3284,11 @@
       <c r="I6" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79292&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/R4eAT2fR1701422895496.png</t>
         </is>
       </c>
     </row>
@@ -2889,7 +3317,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>603</v>
+        <v>609</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -2902,6 +3330,11 @@
       <c r="I7" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79240&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202311/hT5gYzxi1701335584641.jpeg</t>
         </is>
       </c>
     </row>
@@ -2930,7 +3363,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>592</v>
+        <v>608</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -2943,6 +3376,11 @@
       <c r="I8" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79972&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/z7bFCMqM1702972063289.png</t>
         </is>
       </c>
     </row>
@@ -2971,7 +3409,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>476</v>
+        <v>490</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -2984,6 +3422,11 @@
       <c r="I9" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80171&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/chPePM8d1703485388734.png</t>
         </is>
       </c>
     </row>
@@ -2998,7 +3441,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3050,6 +3493,11 @@
           <t>Link</t>
         </is>
       </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Cover</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -3076,7 +3524,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1674</v>
+        <v>1675</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -3089,6 +3537,11 @@
       <c r="I2" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=70666&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202106/okF9H2Uj1623911727887.jpeg</t>
         </is>
       </c>
     </row>
@@ -3132,6 +3585,11 @@
           <t>https://show.bilibili.com/platform/detail.html?id=77530&amp;msource=Msearch_colligation</t>
         </is>
       </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202310/JqP3lHJt1698030195136.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -3173,6 +3631,11 @@
           <t>https://show.bilibili.com/platform/detail.html?id=77862&amp;msource=Msearch_colligation</t>
         </is>
       </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202310/QnmD4yOd1698652192047.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -3199,7 +3662,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1783</v>
+        <v>1789</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -3212,6 +3675,11 @@
       <c r="I5" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79005&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202311/02P8eD3Z1700821985538.jpeg</t>
         </is>
       </c>
     </row>
@@ -3240,7 +3708,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1794</v>
+        <v>1809</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -3253,6 +3721,11 @@
       <c r="I6" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79292&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/R4eAT2fR1701422895496.png</t>
         </is>
       </c>
     </row>
@@ -3281,7 +3754,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>603</v>
+        <v>609</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -3294,6 +3767,11 @@
       <c r="I7" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79240&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202311/hT5gYzxi1701335584641.jpeg</t>
         </is>
       </c>
     </row>
@@ -3337,6 +3815,11 @@
           <t>https://show.bilibili.com/platform/detail.html?id=78809&amp;msource=Msearch_colligation</t>
         </is>
       </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202311/YsBoZAOW1700551290654.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -3363,7 +3846,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>1572</v>
+        <v>1578</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -3376,6 +3859,11 @@
       <c r="I9" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79166&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202311/MjTiIYlk1701242361853.jpeg</t>
         </is>
       </c>
     </row>
@@ -3404,7 +3892,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -3417,6 +3905,11 @@
       <c r="I10" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80103&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/2h2tIq7l1703144874867.png</t>
         </is>
       </c>
     </row>
@@ -3445,7 +3938,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>592</v>
+        <v>608</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -3458,6 +3951,11 @@
       <c r="I11" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79972&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/z7bFCMqM1702972063289.png</t>
         </is>
       </c>
     </row>
@@ -3501,6 +3999,11 @@
           <t>https://show.bilibili.com/platform/detail.html?id=79939&amp;msource=Msearch_colligation</t>
         </is>
       </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/hY6FVnjM1702954652593.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -3527,7 +4030,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>476</v>
+        <v>490</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -3540,6 +4043,11 @@
       <c r="I13" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80171&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/chPePM8d1703485388734.png</t>
         </is>
       </c>
     </row>
@@ -3568,7 +4076,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -3581,6 +4089,11 @@
       <c r="I14" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79833&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/Ca51ySIK1702607429682.jpeg</t>
         </is>
       </c>
     </row>
@@ -3609,7 +4122,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -3622,6 +4135,11 @@
       <c r="I15" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80008&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/rSR9XSX01703041035213.jpeg</t>
         </is>
       </c>
     </row>
@@ -3650,7 +4168,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>1194</v>
+        <v>1224</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -3663,6 +4181,11 @@
       <c r="I16" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80235&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/VytCJsEX1703647558135.jpeg</t>
         </is>
       </c>
     </row>
@@ -3691,7 +4214,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>708</v>
+        <v>723</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -3704,6 +4227,11 @@
       <c r="I17" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80382&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/FIZYJ68n1704179640046.jpeg</t>
         </is>
       </c>
     </row>
@@ -3732,7 +4260,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>471</v>
+        <v>478</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -3745,6 +4273,11 @@
       <c r="I18" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79284&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/zsveqtuG1701764030936.jpeg</t>
         </is>
       </c>
     </row>
@@ -3773,7 +4306,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>210</v>
+        <v>232</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -3786,6 +4319,11 @@
       <c r="I19" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80597&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/UoNyFL4G1704707294378.png</t>
         </is>
       </c>
     </row>
@@ -3814,7 +4352,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>775</v>
+        <v>782</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -3827,6 +4365,11 @@
       <c r="I20" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79261&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/mmvCkYYH1701411372879.jpeg</t>
         </is>
       </c>
     </row>
@@ -3855,7 +4398,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -3868,6 +4411,11 @@
       <c r="I21" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80384&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/JHXTpHAw1704181759660.jpeg</t>
         </is>
       </c>
     </row>
@@ -3896,7 +4444,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -3909,6 +4457,11 @@
       <c r="I22" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80234&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/Idm7h4dK1703646683782.jpeg</t>
         </is>
       </c>
     </row>
@@ -3937,7 +4490,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -3950,6 +4503,11 @@
       <c r="I23" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79641&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/CoNbgCpO1703644783043.jpeg</t>
         </is>
       </c>
     </row>
@@ -3978,7 +4536,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -3991,6 +4549,11 @@
       <c r="I24" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=78418&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202311/GHpvkT5Y1699605760230.jpeg</t>
         </is>
       </c>
     </row>
@@ -4019,7 +4582,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -4032,6 +4595,11 @@
       <c r="I25" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80548&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/dQ4DrxCk1704683144116.png</t>
         </is>
       </c>
     </row>
@@ -4060,7 +4628,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -4073,6 +4641,11 @@
       <c r="I26" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80277&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/5d6O1Rf11703742965244.png</t>
         </is>
       </c>
     </row>
@@ -4101,7 +4674,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -4114,6 +4687,11 @@
       <c r="I27" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79046&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202311/XmP03Vf31701070803044.jpeg</t>
         </is>
       </c>
     </row>
@@ -4142,7 +4720,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>270</v>
+        <v>301</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -4155,6 +4733,11 @@
       <c r="I28" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80284&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/9xGb6MXN1704183627126.jpeg</t>
         </is>
       </c>
     </row>
@@ -4183,7 +4766,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -4196,6 +4779,11 @@
       <c r="I29" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80045&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/hUfcrw3y1703055422885.jpeg</t>
         </is>
       </c>
     </row>
@@ -4224,7 +4812,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>310</v>
+        <v>327</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -4237,6 +4825,11 @@
       <c r="I30" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80204&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/eK96fdcg1703573110264.jpeg</t>
         </is>
       </c>
     </row>
@@ -4265,7 +4858,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -4278,6 +4871,11 @@
       <c r="I31" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=77773&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202310/XKKYWAk51698315607196.png</t>
         </is>
       </c>
     </row>
@@ -4306,7 +4904,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>160</v>
+        <v>210</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -4319,6 +4917,11 @@
       <c r="I32" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80167&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/cMpTD3gV1703571795332.png</t>
         </is>
       </c>
     </row>
@@ -4347,7 +4950,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>1604</v>
+        <v>1679</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -4360,6 +4963,11 @@
       <c r="I33" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=78523&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202311/30WzGyPz1699943734625.jpeg</t>
         </is>
       </c>
     </row>
@@ -4388,7 +4996,7 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -4401,6 +5009,11 @@
       <c r="I34" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79332&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/Ewreg1JT1701677993728.jpeg</t>
         </is>
       </c>
     </row>
@@ -4429,7 +5042,7 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>469</v>
+        <v>479</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -4442,6 +5055,11 @@
       <c r="I35" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80128&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/DEW1XYty1703226993965.jpeg</t>
         </is>
       </c>
     </row>
@@ -4470,7 +5088,7 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -4483,6 +5101,11 @@
       <c r="I36" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79938&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/TWEj0Z7l1702954736529.jpeg</t>
         </is>
       </c>
     </row>
@@ -4511,7 +5134,7 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>15</v>
+        <v>1023</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -4524,6 +5147,11 @@
       <c r="I37" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80497&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/0duSXTQy1704423309244.jpeg</t>
         </is>
       </c>
     </row>
@@ -4552,7 +5180,7 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -4565,6 +5193,11 @@
       <c r="I38" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80339&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/a8iuOufB1703832570508.jpeg</t>
         </is>
       </c>
     </row>
@@ -4593,7 +5226,7 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>2239</v>
+        <v>2254</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -4606,6 +5239,11 @@
       <c r="I39" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=77754&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/7eGZETK91701943985671.jpeg</t>
         </is>
       </c>
     </row>
@@ -4634,7 +5272,7 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -4647,6 +5285,11 @@
       <c r="I40" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80142&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/1npuHFBM1703231674558.jpeg</t>
         </is>
       </c>
     </row>
@@ -4675,7 +5318,7 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -4688,6 +5331,11 @@
       <c r="I41" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80299&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/V0xu26Cl1703753850690.jpeg</t>
         </is>
       </c>
     </row>
@@ -4716,7 +5364,7 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -4729,6 +5377,11 @@
       <c r="I42" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80575&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/y4uWdyPT1704700763902.jpeg</t>
         </is>
       </c>
     </row>
@@ -4757,7 +5410,7 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -4770,6 +5423,11 @@
       <c r="I43" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80571&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/SHH70VXN1704700240858.jpeg</t>
         </is>
       </c>
     </row>
@@ -4798,7 +5456,7 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -4811,6 +5469,11 @@
       <c r="I44" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=76410&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202309/fVXMrcHy1693971682397.jpeg</t>
         </is>
       </c>
     </row>
@@ -4854,6 +5517,11 @@
           <t>https://show.bilibili.com/platform/detail.html?id=80050&amp;msource=Msearch_colligation</t>
         </is>
       </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/0iJP3TY61703056498448.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -4880,7 +5548,7 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -4893,6 +5561,11 @@
       <c r="I46" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=78667&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202311/bTP7w6GD1700130122940.jpeg</t>
         </is>
       </c>
     </row>
@@ -4921,7 +5594,7 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -4934,6 +5607,11 @@
       <c r="I47" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=78657&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202311/qGwPWLzO1700562869315.jpeg</t>
         </is>
       </c>
     </row>
@@ -4962,7 +5640,7 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -4975,6 +5653,11 @@
       <c r="I48" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80321&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/KBlb0enU1704358750268.jpeg</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update gh-pages to output generated at 7948aec
</commit_message>
<xml_diff>
--- a/上海-漫展信息.xlsx
+++ b/上海-漫展信息.xlsx
@@ -603,7 +603,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -649,7 +649,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1578</v>
+        <v>1580</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -695,7 +695,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -741,7 +741,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -787,7 +787,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -833,7 +833,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>1224</v>
+        <v>1229</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -879,7 +879,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>723</v>
+        <v>728</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -971,7 +971,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1017,7 +1017,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1063,7 +1063,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1109,7 +1109,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1155,7 +1155,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1201,7 +1201,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1247,7 +1247,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1293,7 +1293,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1385,7 +1385,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1477,7 +1477,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>1679</v>
+        <v>1704</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1523,7 +1523,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1569,7 +1569,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1615,7 +1615,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1661,7 +1661,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>1023</v>
+        <v>1026</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1707,7 +1707,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1799,7 +1799,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1845,7 +1845,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1891,7 +1891,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -2075,7 +2075,7 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -2107,7 +2107,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2190,7 +2190,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -2236,7 +2236,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -2360,38 +2360,38 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>上海·音乐剧《三星堆》</t>
+          <t xml:space="preserve">上海·Ayasa LIVE TOUR 2024 〜A fraction〜 </t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>汾阳路6号 上音歌剧院</t>
+          <t>宜昌路179号 万代南梦宫上海文化中心</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2024.01.19 19:30-01.21 22:00</t>
+          <t>2024.01.19 19:30-01.19 21:00</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>12</v>
+        <v>673</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>180</t>
+          <t>380</t>
         </is>
       </c>
       <c r="H6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79832&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78926&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/aRlkZiIb1702607587670.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202311/iQMerqQQ1700725727470.png</t>
         </is>
       </c>
     </row>
@@ -2401,43 +2401,43 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024.01.20</t>
+          <t>2024.01.19</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>上海·《进击的巨人》动漫ACG音乐会（取消）</t>
+          <t>上海·音乐剧《三星堆》</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>南京西路1376号上海商城4层 商城剧院</t>
+          <t>汾阳路6号 上音歌剧院</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2024.01.20 15:00-01.20 16:30</t>
+          <t>2024.01.19 19:30-01.21 22:00</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>不可售</t>
+          <t>180</t>
         </is>
       </c>
       <c r="H7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80101&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79832&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/3iT86tbs1703142892633.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/aRlkZiIb1702607587670.jpeg</t>
         </is>
       </c>
     </row>
@@ -2452,25 +2452,25 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>上海·奥井雅美出道突破30周年演唱会</t>
+          <t>上海·《进击的巨人》动漫ACG音乐会（取消）</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>宜昌路179号 万代南梦宫上海文化中心</t>
+          <t>南京西路1376号上海商城4层 商城剧院</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2024.01.20 18:30-01.20 20:10</t>
+          <t>2024.01.20 15:00-01.20 16:30</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>480</t>
+          <t>不可售</t>
         </is>
       </c>
       <c r="H8" t="b">
@@ -2478,12 +2478,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80373&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80101&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/Ttzqeavz1704167763720.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/3iT86tbs1703142892633.jpeg</t>
         </is>
       </c>
     </row>
@@ -2498,25 +2498,25 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>上海·齐藤朱夏2024演唱会</t>
+          <t>上海·奥井雅美出道突破30周年演唱会</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>虹许路731号4号楼 THE BOXX•城市乐园</t>
+          <t>宜昌路179号 万代南梦宫上海文化中心</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2024.01.20 14:00-01.20 15:30</t>
+          <t>2024.01.20 18:30-01.20 20:10</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>804</v>
+        <v>17</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>已售罄</t>
+          <t>480</t>
         </is>
       </c>
       <c r="H9" t="b">
@@ -2524,12 +2524,12 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79842&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80373&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202312/vptlHEg41702610098849.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/Ttzqeavz1704167763720.jpeg</t>
         </is>
       </c>
     </row>
@@ -2539,43 +2539,43 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2024.01.23</t>
+          <t>2024.01.20</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>上海·七音阿卡莉 NANAOAKARI 2024 专场演出</t>
+          <t>上海·齐藤朱夏2024演唱会</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>嘉兴路街道瑞虹路188号瑞虹天地月亮湾3层 Modern Sky LAB摩登天空(瑞虹天地店)</t>
+          <t>虹许路731号4号楼 THE BOXX•城市乐园</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2024.01.23 20:00-01.23 22:00</t>
+          <t>2024.01.20 14:00-01.20 15:30</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>76</v>
+        <v>805</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>已售罄</t>
         </is>
       </c>
       <c r="H10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79641&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79842&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/CoNbgCpO1703644783043.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/vptlHEg41702610098849.jpeg</t>
         </is>
       </c>
     </row>
@@ -2585,30 +2585,30 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2024.01.26</t>
+          <t>2024.01.23</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
+          <t>上海·七音阿卡莉 NANAOAKARI 2024 专场演出</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>丁香路425号 上海东方艺术中心</t>
+          <t>嘉兴路街道瑞虹路188号瑞虹天地月亮湾3层 Modern Sky LAB摩登天空(瑞虹天地店)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2024.01.26 19:30-01.26 21:30</t>
+          <t>2024.01.23 20:00-01.23 22:00</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>137</v>
+        <v>76</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>380</t>
         </is>
       </c>
       <c r="H11" t="b">
@@ -2616,12 +2616,12 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78418&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79641&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202311/GHpvkT5Y1699605760230.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/CoNbgCpO1703644783043.jpeg</t>
         </is>
       </c>
     </row>
@@ -2631,43 +2631,43 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2024.01.27</t>
+          <t>2024.01.26</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>上海·Azurock」Azurose ACG Cover Live</t>
+          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>愚园路1398号 育音堂音乐公园</t>
+          <t>丁香路425号 上海东方艺术中心</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2024.01.27 19:00-01.27 21:30</t>
+          <t>2024.01.26 19:30-01.26 21:30</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>37</v>
+        <v>138</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>80</t>
         </is>
       </c>
       <c r="H12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80277&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78418&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202312/5d6O1Rf11703742965244.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202311/GHpvkT5Y1699605760230.jpeg</t>
         </is>
       </c>
     </row>
@@ -2682,38 +2682,38 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>上海·日本原版《数码宝贝舞台剧：游乐园之谜》</t>
+          <t>上海·Azurock」Azurose ACG Cover Live</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>茂名南路57号近长乐路 上海兰心大戏院</t>
+          <t>愚园路1398号 育音堂音乐公园</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2024.01.27 15:30-01.27 20:55</t>
+          <t>2024.01.27 19:00-01.27 21:30</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>88</t>
         </is>
       </c>
       <c r="H13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79783&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80277&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/S6nZ327b1702534484951.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/5d6O1Rf11703742965244.png</t>
         </is>
       </c>
     </row>
@@ -2728,25 +2728,25 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>上海•Risa Yuzuki 1st ONEMAN LIVE 「Future Interlink」 追加公演</t>
+          <t>上海·日本原版《数码宝贝舞台剧：游乐园之谜》</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>愚园路1250号 新歌空间</t>
+          <t>茂名南路57号近长乐路 上海兰心大戏院</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2024.01.27 18:30-01.27 21:00</t>
+          <t>2024.01.27 15:30-01.27 20:55</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>271</v>
+        <v>19</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>278</t>
+          <t>120</t>
         </is>
       </c>
       <c r="H14" t="b">
@@ -2754,12 +2754,12 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77773&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79783&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202310/XKKYWAk51698315607196.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/S6nZ327b1702534484951.jpeg</t>
         </is>
       </c>
     </row>
@@ -2769,30 +2769,30 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2024.02.02</t>
+          <t>2024.01.27</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>上海·次元LAB 二次元电音节</t>
+          <t>上海•Risa Yuzuki 1st ONEMAN LIVE 「Future Interlink」 追加公演</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>中兴路1683号金融街购物中心L3-27 蜚声上海Livehouse</t>
+          <t>愚园路1250号 新歌空间</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2024.02.02 12:30-02.02 21:00</t>
+          <t>2024.01.27 18:30-01.27 21:00</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>479</v>
+        <v>271</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>278</t>
         </is>
       </c>
       <c r="H15" t="b">
@@ -2800,12 +2800,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80128&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=77773&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202312/DEW1XYty1703226993965.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202310/XKKYWAk51698315607196.png</t>
         </is>
       </c>
     </row>
@@ -2815,43 +2815,43 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2024.02.14</t>
+          <t>2024.02.02</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>上海·【情人节特辑】《那年我们》记忆重启韩剧经典OST音乐会《请回答1988》《来自星星的你》</t>
+          <t>上海·次元LAB 二次元电音节</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>牛庄路704号 中国大戏院</t>
+          <t>中兴路1683号金融街购物中心L3-27 蜚声上海Livehouse</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2024.02.14 19:30-02.14 21:00</t>
+          <t>2024.02.02 12:30-02.02 21:00</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>486</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>380</t>
         </is>
       </c>
       <c r="H16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80615&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80128&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/5DDVhKcO1704767761361.png</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/DEW1XYty1703226993965.jpeg</t>
         </is>
       </c>
     </row>
@@ -2861,30 +2861,30 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2024.02.25</t>
+          <t>2024.02.14</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>上海·青山吉能见面会</t>
+          <t>上海·【情人节特辑】《那年我们》记忆重启韩剧经典OST音乐会《请回答1988》《来自星星的你》</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>虹许路731号4号楼 THE BOXX•城市乐园</t>
+          <t>牛庄路704号 中国大戏院</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2024.02.25 14:30-02.25 19:30</t>
+          <t>2024.02.14 19:30-02.14 21:00</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>171</v>
+        <v>1</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>80</t>
         </is>
       </c>
       <c r="H17" t="b">
@@ -2892,12 +2892,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80142&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80615&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/1npuHFBM1703231674558.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/5DDVhKcO1704767761361.png</t>
         </is>
       </c>
     </row>
@@ -2907,43 +2907,43 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2024.04.06</t>
+          <t>2024.02.25</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
+          <t>上海·青山吉能见面会</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>复兴中路1380号 捷豹上海交响音乐厅</t>
+          <t>虹许路731号4号楼 THE BOXX•城市乐园</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2024.04.06 19:30-04.06 21:30</t>
+          <t>2024.02.25 14:30-02.25 19:30</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>10</v>
+        <v>171</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>380</t>
         </is>
       </c>
       <c r="H18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80050&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80142&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/0iJP3TY61703056498448.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/1npuHFBM1703231674558.jpeg</t>
         </is>
       </c>
     </row>
@@ -2953,26 +2953,26 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2024.04.13</t>
+          <t>2024.04.06</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>上海·《四月是你的谎言》——“公生”与“薰”的钢琴小提琴唯美经典音乐集</t>
+          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>丁香路425号 上海东方艺术中心</t>
+          <t>复兴中路1380号 捷豹上海交响音乐厅</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2024.04.13 19:30-04.13 21:30</t>
+          <t>2024.04.06 19:30-04.06 21:30</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>140</v>
+        <v>10</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -2984,10 +2984,56 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80050&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/0iJP3TY61703056498448.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2024.04.13</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>上海·《四月是你的谎言》——“公生”与“薰”的钢琴小提琴唯美经典音乐集</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>丁香路425号 上海东方艺术中心</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2024.04.13 19:30-04.13 21:30</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>140</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
           <t>https://show.bilibili.com/platform/detail.html?id=78667&amp;msource=Msearch_colligation</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="J20" t="inlineStr">
         <is>
           <t>//i1.hdslb.com/bfs/openplatform/202311/bTP7w6GD1700130122940.jpeg</t>
         </is>
@@ -3087,7 +3133,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1675</v>
+        <v>1677</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -3133,7 +3179,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -3225,7 +3271,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1789</v>
+        <v>1793</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -3271,7 +3317,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1809</v>
+        <v>1814</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -3363,7 +3409,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -3409,7 +3455,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -3441,7 +3487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3524,7 +3570,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1675</v>
+        <v>1677</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -3551,30 +3597,30 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2023.10.16</t>
+          <t>2023.11.02</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>上海·古影文化《1941·新和医院》大型沉浸式互动剧场</t>
+          <t>上海·Hello Kitty Cosmos 50周年光影特展</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>金玉路2号 古影沉浸式互动游戏剧场</t>
+          <t>漕宝路3055号 宝龙美术馆</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023.10.16 10:00-2024.10.15 21:00</t>
+          <t>2023.11.02 10:00-2024.01.28 18:00</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>996</t>
+          <t>139</t>
         </is>
       </c>
       <c r="H3" t="b">
@@ -3582,12 +3628,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77530&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=77862&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202310/JqP3lHJt1698030195136.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202310/QnmD4yOd1698652192047.jpeg</t>
         </is>
       </c>
     </row>
@@ -3597,30 +3643,30 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2023.11.02</t>
+          <t>2023.12.01</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>上海·Hello Kitty Cosmos 50周年光影特展</t>
+          <t>上海·2023《蔚蓝档案》x  萌果酱谷子咖啡</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>漕宝路3055号 宝龙美术馆</t>
+          <t>南京东路340号百联ZX 萌果酱谷子咖啡（百联）</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023.11.02 10:00-2024.01.28 18:00</t>
+          <t>2023.12.01 00:00-2024.01.31 23:59</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>105</v>
+        <v>1793</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>139</t>
+          <t>30</t>
         </is>
       </c>
       <c r="H4" t="b">
@@ -3628,12 +3674,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77862&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79005&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202310/QnmD4yOd1698652192047.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202311/02P8eD3Z1700821985538.jpeg</t>
         </is>
       </c>
     </row>
@@ -3643,26 +3689,26 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2023.12.01</t>
+          <t>2023.12.06</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>上海·2023《蔚蓝档案》x  萌果酱谷子咖啡</t>
+          <t>上海·「咒术回战  × animate cafe」</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>南京东路340号百联ZX 萌果酱谷子咖啡（百联）</t>
+          <t>西藏北路198号大悦城北座8楼N809-1 animate cafe上海店</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023.12.01 00:00-2024.01.31 23:59</t>
+          <t>2023.12.06 00:00-2024.01.24 23:59</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1789</v>
+        <v>1814</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -3674,12 +3720,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79005&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79292&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202311/02P8eD3Z1700821985538.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/R4eAT2fR1701422895496.png</t>
         </is>
       </c>
     </row>
@@ -3689,26 +3735,26 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2023.12.06</t>
+          <t>2023.12.09</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>上海·「咒术回战  × animate cafe」</t>
+          <t>上海·非人哉官方授权主题店</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>西藏北路198号大悦城北座8楼N809-1 animate cafe上海店</t>
+          <t>南京东路830号第一百货商业中心B馆5楼(海底捞旁边) 第一百货商业中心</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023.12.06 00:00-2024.01.24 23:59</t>
+          <t>2023.12.09 00:00-2024.01.22 23:59</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1809</v>
+        <v>609</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -3720,12 +3766,12 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79292&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79240&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/R4eAT2fR1701422895496.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202311/hT5gYzxi1701335584641.jpeg</t>
         </is>
       </c>
     </row>
@@ -3735,30 +3781,30 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2023.12.09</t>
+          <t>2023.12.10</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>上海·非人哉官方授权主题店</t>
+          <t>上海·多维跃迁-2023 红点设计概念大奖获奖作品展</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>南京东路830号第一百货商业中心B馆5楼(海底捞旁边) 第一百货商业中心</t>
+          <t>国展路1099号 上海世博展览馆</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023.12.09 00:00-2024.01.22 23:59</t>
+          <t>2023.12.10 12:00-2024.02.16 17:00</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>609</v>
+        <v>25</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>80</t>
         </is>
       </c>
       <c r="H7" t="b">
@@ -3766,12 +3812,12 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79240&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78809&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202311/hT5gYzxi1701335584641.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202311/YsBoZAOW1700551290654.jpeg</t>
         </is>
       </c>
     </row>
@@ -3781,30 +3827,30 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2023.12.10</t>
+          <t>2023.12.22</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>上海·多维跃迁-2023 红点设计概念大奖获奖作品展</t>
+          <t>上海·新海诚导演作品《铃芽之旅》展 丨 购票抽新海诚见面会门票丨 超限定复刻原画发售</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>国展路1099号 上海世博展览馆</t>
+          <t>湖滨路168号 上海无限极荟购物中心</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023.12.10 12:00-2024.02.16 17:00</t>
+          <t>2023.12.22 10:00-2024.02.16 22:00</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>24</v>
+        <v>1580</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H8" t="b">
@@ -3812,12 +3858,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78809&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79166&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202311/YsBoZAOW1700551290654.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202311/MjTiIYlk1701242361853.jpeg</t>
         </is>
       </c>
     </row>
@@ -3827,30 +3873,30 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2023.12.22</t>
+          <t>2023.12.31</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>上海·新海诚导演作品《铃芽之旅》展 丨 购票抽新海诚见面会门票丨 超限定复刻原画发售</t>
+          <t>上海·次元波板糖×时光代理人「锦瑟华年主题快闪店」</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>湖滨路168号 上海无限极荟购物中心</t>
+          <t>西藏北路166静安大悦城北座6楼611号 次元波板糖</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2023.12.22 10:00-2024.02.16 22:00</t>
+          <t>2023.12.31 00:00-2024.01.29 23:59</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>1578</v>
+        <v>609</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>30</t>
         </is>
       </c>
       <c r="H9" t="b">
@@ -3858,12 +3904,12 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79166&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79972&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202311/MjTiIYlk1701242361853.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/z7bFCMqM1702972063289.png</t>
         </is>
       </c>
     </row>
@@ -3873,30 +3919,30 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2023.12.27</t>
+          <t>2024.01.06</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>上海·爱乐汇《天空之城》久石让&amp;宫崎骏动漫经典音乐作品演奏会</t>
+          <t>上海·罗小黑 x HAPPY ZOO主题Cafe</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>南京西路1376号 上海商城剧院</t>
+          <t>南京东路340号 百联zx创趣场</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2023.12.27 19:30-2024.02.03 12:00</t>
+          <t>2024.01.06 00:00-01.31 23:59</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>29</v>
+        <v>493</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H10" t="b">
@@ -3904,12 +3950,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80103&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80171&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202312/2h2tIq7l1703144874867.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/chPePM8d1703485388734.png</t>
         </is>
       </c>
     </row>
@@ -3919,30 +3965,30 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2023.12.31</t>
+          <t>2024.01.13</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>上海·次元波板糖×时光代理人「锦瑟华年主题快闪店」</t>
+          <t>上海·月遇国乙+代号鸢only</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>西藏北路166静安大悦城北座6楼611号 次元波板糖</t>
+          <t>汶水路40号 格乐利雅GALLERIA艺术中心(大宁店)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2023.12.31 00:00-2024.01.29 23:59</t>
+          <t>2024.01.13 10:40-01.13 21:00</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>608</v>
+        <v>396</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>95</t>
         </is>
       </c>
       <c r="H11" t="b">
@@ -3950,12 +3996,12 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79972&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79833&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/z7bFCMqM1702972063289.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/Ca51ySIK1702607429682.jpeg</t>
         </is>
       </c>
     </row>
@@ -3965,30 +4011,30 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2024.01.01</t>
+          <t>2024.01.13</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>上海·沉浸式悬念剧场《9号秘事》</t>
+          <t>上海·灵能百分百ONLY</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>人民大道300号 上海大剧院</t>
+          <t>长江路258号 中成智谷</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2024.01.01 19:30-01.28 16:20</t>
+          <t>2024.01.13 10:00-01.13 16:30</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>41</v>
+        <v>255</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>489</t>
+          <t>79</t>
         </is>
       </c>
       <c r="H12" t="b">
@@ -3996,12 +4042,12 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79939&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80008&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/hY6FVnjM1702954652593.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/rSR9XSX01703041035213.jpeg</t>
         </is>
       </c>
     </row>
@@ -4011,30 +4057,30 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2024.01.06</t>
+          <t>2024.01.13</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>上海·罗小黑 x HAPPY ZOO主题Cafe</t>
+          <t>上海·第五十二届妖漫动漫游戏展</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>南京东路340号 百联zx创趣场</t>
+          <t>漕溪北路339号百脑汇4楼 百脑汇</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2024.01.06 00:00-01.31 23:59</t>
+          <t>2024.01.13 11:00-01.14 18:00</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>490</v>
+        <v>1229</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>19</t>
         </is>
       </c>
       <c r="H13" t="b">
@@ -4042,12 +4088,12 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80171&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80235&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/chPePM8d1703485388734.png</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/VytCJsEX1703647558135.jpeg</t>
         </is>
       </c>
     </row>
@@ -4062,25 +4108,25 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>上海·月遇国乙+代号鸢only</t>
+          <t>上海·第五十届燃梦星辰动漫展-原X铁X崩免费同好交流会</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>汶水路40号 格乐利雅GALLERIA艺术中心(大宁店)</t>
+          <t>云台路800号 亿丰时代广场</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2024.01.13 10:40-01.13 21:00</t>
+          <t>2024.01.13 11:00-01.14 16:30</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>395</v>
+        <v>728</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>58</t>
         </is>
       </c>
       <c r="H14" t="b">
@@ -4088,12 +4134,12 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79833&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80382&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/Ca51ySIK1702607429682.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/FIZYJ68n1704179640046.jpeg</t>
         </is>
       </c>
     </row>
@@ -4103,30 +4149,30 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2024.01.13</t>
+          <t>2024.01.14</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>上海·灵能百分百ONLY</t>
+          <t>上海·1.14想见你光夜only</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>长江路258号 中成智谷</t>
+          <t>汶水路210号 日本嘉美麓德婚礼公馆(大宁店)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2024.01.13 10:00-01.13 16:30</t>
+          <t>2024.01.14 09:30-01.14 21:30</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>254</v>
+        <v>478</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>68</t>
         </is>
       </c>
       <c r="H15" t="b">
@@ -4134,12 +4180,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80008&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79284&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/rSR9XSX01703041035213.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/zsveqtuG1701764030936.jpeg</t>
         </is>
       </c>
     </row>
@@ -4149,30 +4195,30 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2024.01.13</t>
+          <t>2024.01.19</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>上海·第五十二届妖漫动漫游戏展</t>
+          <t xml:space="preserve">上海·Ayasa LIVE TOUR 2024 〜A fraction〜 </t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>漕溪北路339号百脑汇4楼 百脑汇</t>
+          <t>宜昌路179号 万代南梦宫上海文化中心</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2024.01.13 11:00-01.14 18:00</t>
+          <t>2024.01.19 19:30-01.19 21:00</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>1224</v>
+        <v>673</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>380</t>
         </is>
       </c>
       <c r="H16" t="b">
@@ -4180,12 +4226,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80235&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78926&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/VytCJsEX1703647558135.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202311/iQMerqQQ1700725727470.png</t>
         </is>
       </c>
     </row>
@@ -4195,43 +4241,43 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2024.01.13</t>
+          <t>2024.01.19</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>上海·第五十届燃梦星辰动漫展-原X铁X崩免费同好交流会</t>
+          <t>上海·音乐剧《三星堆》</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>云台路800号 亿丰时代广场</t>
+          <t>汾阳路6号 上音歌剧院</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2024.01.13 11:00-01.14 16:30</t>
+          <t>2024.01.19 19:30-01.21 22:00</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>723</v>
+        <v>12</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>180</t>
         </is>
       </c>
       <c r="H17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80382&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79832&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/FIZYJ68n1704179640046.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/aRlkZiIb1702607587670.jpeg</t>
         </is>
       </c>
     </row>
@@ -4241,30 +4287,30 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2024.01.14</t>
+          <t>2024.01.20</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>上海·1.14想见你光夜only</t>
+          <t>上海·坏孩纸物语の第31届动漫节之寒假篇</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>汶水路210号 日本嘉美麓德婚礼公馆(大宁店)</t>
+          <t>东大名路1118号(提篮桥地铁站1号口步行340米) 影梦里</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2024.01.14 09:30-01.14 21:30</t>
+          <t>2024.01.20 11:00-01.20 17:00</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>478</v>
+        <v>235</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>49</t>
         </is>
       </c>
       <c r="H18" t="b">
@@ -4272,12 +4318,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79284&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80597&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/zsveqtuG1701764030936.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/UoNyFL4G1704707294378.png</t>
         </is>
       </c>
     </row>
@@ -4292,25 +4338,25 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>上海·坏孩纸物语の第31届动漫节之寒假篇</t>
+          <t>上海·排球少年X蓝锁X灌篮ONLY</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>东大名路1118号(提篮桥地铁站1号口步行340米) 影梦里</t>
+          <t>逸仙路270号  上海宝丰联大酒店</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2024.01.20 11:00-01.20 17:00</t>
+          <t>2024.01.20 10:00-01.20 17:00</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>232</v>
+        <v>784</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>60</t>
         </is>
       </c>
       <c r="H19" t="b">
@@ -4318,12 +4364,12 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80597&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79261&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/UoNyFL4G1704707294378.png</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/mmvCkYYH1701411372879.jpeg</t>
         </is>
       </c>
     </row>
@@ -4338,21 +4384,21 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>上海·排球少年X蓝锁X灌篮ONLY</t>
+          <t>上海·次元裂缝-X Anikura二次元迎春派对</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>逸仙路270号  上海宝丰联大酒店</t>
+          <t>海潮路133号B1 JUMP工坊</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2024.01.20 10:00-01.20 17:00</t>
+          <t>2024.01.20 14:00-01.20 22:00</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>782</v>
+        <v>18</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -4364,12 +4410,12 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79261&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80638&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202312/mmvCkYYH1701411372879.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/N7gT4Tza1704782642832.jpeg</t>
         </is>
       </c>
     </row>
@@ -4398,7 +4444,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -4444,7 +4490,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -4536,7 +4582,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -4582,7 +4628,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -4674,7 +4720,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -4720,7 +4766,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -4812,7 +4858,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -4950,7 +4996,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>1679</v>
+        <v>1704</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -4996,7 +5042,7 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -5042,7 +5088,7 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>479</v>
+        <v>486</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -5074,12 +5120,12 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>上海·第七届次元鹿角动漫游戏展</t>
+          <t>上海·Coser迎春动漫展</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>长宁路1191号长宁来福士B1 长宁来福士</t>
+          <t>海潮路133号B1 JUMP工坊</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -5088,11 +5134,11 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>60</t>
         </is>
       </c>
       <c r="H36" t="b">
@@ -5100,12 +5146,12 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79938&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80646&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/TWEj0Z7l1702954736529.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/4WVkFc4d1704787729064.jpeg</t>
         </is>
       </c>
     </row>
@@ -5115,30 +5161,30 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2024.02.16</t>
+          <t>2024.02.03</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>上海·第九届次元鹿角动漫游戏展</t>
+          <t>上海·第七届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
+          <t>长宁路1191号长宁来福士B1 长宁来福士</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2024.02.16 11:00-02.17 18:00</t>
+          <t>2024.02.03 10:00-02.04 17:00</t>
         </is>
       </c>
       <c r="F37" t="n">
-        <v>1023</v>
+        <v>82</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>68</t>
         </is>
       </c>
       <c r="H37" t="b">
@@ -5146,12 +5192,12 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80497&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79938&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/0duSXTQy1704423309244.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/TWEj0Z7l1702954736529.jpeg</t>
         </is>
       </c>
     </row>
@@ -5161,30 +5207,30 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2024.02.24</t>
+          <t>2024.02.16</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>上海·SISP动漫游戏嘉年华</t>
+          <t>上海·第九届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>年家浜路518号 周浦万达广场</t>
+          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2024.02.24 13:00-02.25 19:00</t>
+          <t>2024.02.16 11:00-02.17 18:00</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>58</v>
+        <v>1026</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H38" t="b">
@@ -5192,12 +5238,12 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80339&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80497&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/a8iuOufB1703832570508.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/0duSXTQy1704423309244.jpeg</t>
         </is>
       </c>
     </row>
@@ -5212,38 +5258,38 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>上海·第三届燃梦BACG PRO游戏动漫展</t>
+          <t>上海·SISP动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
+          <t>年家浜路518号 周浦万达广场</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2024.02.24 11:00-02.25 16:30</t>
+          <t>2024.02.24 13:00-02.25 19:00</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>2254</v>
+        <v>60</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>48</t>
         </is>
       </c>
       <c r="H39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77754&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80339&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202312/7eGZETK91701943985671.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/a8iuOufB1703832570508.jpeg</t>
         </is>
       </c>
     </row>
@@ -5253,43 +5299,43 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2024.02.25</t>
+          <t>2024.02.24</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>上海·青山吉能见面会</t>
+          <t>上海·第三届燃梦BACG PRO游戏动漫展</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>虹许路731号4号楼 THE BOXX•城市乐园</t>
+          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2024.02.25 14:30-02.25 19:30</t>
+          <t>2024.02.24 11:00-02.25 16:30</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>171</v>
+        <v>2254</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80142&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=77754&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/1npuHFBM1703231674558.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/7eGZETK91701943985671.jpeg</t>
         </is>
       </c>
     </row>
@@ -5299,30 +5345,30 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2024.03.02</t>
+          <t>2024.02.25</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>上海·原神X星穹铁道ONLY</t>
+          <t>上海·青山吉能见面会</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>逸仙路301号靠纪念路路口 上海宝丰联大酒店</t>
+          <t>虹许路731号4号楼 THE BOXX•城市乐园</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2024.03.02 10:00-03.02 17:00</t>
+          <t>2024.02.25 14:30-02.25 19:30</t>
         </is>
       </c>
       <c r="F41" t="n">
-        <v>133</v>
+        <v>171</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>380</t>
         </is>
       </c>
       <c r="H41" t="b">
@@ -5330,12 +5376,12 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80299&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80142&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/V0xu26Cl1703753850690.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/1npuHFBM1703231674558.jpeg</t>
         </is>
       </c>
     </row>
@@ -5345,26 +5391,26 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2024.03.03</t>
+          <t>2024.03.02</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>上海·怀旧番ONLY</t>
+          <t>上海·原神X星穹铁道ONLY</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>逸仙路270号  上海宝丰联大酒店</t>
+          <t>逸仙路301号靠纪念路路口 上海宝丰联大酒店</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2024.03.03 10:00-03.03 17:00</t>
+          <t>2024.03.02 10:00-03.02 17:00</t>
         </is>
       </c>
       <c r="F42" t="n">
-        <v>36</v>
+        <v>135</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -5376,12 +5422,12 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80575&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80299&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/y4uWdyPT1704700763902.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/V0xu26Cl1703753850690.jpeg</t>
         </is>
       </c>
     </row>
@@ -5391,43 +5437,43 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2024.03.09</t>
+          <t>2024.03.03</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>上海·第五十三届燃梦星辰动漫嘉年华-随机宅舞</t>
+          <t>上海·怀旧番ONLY</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>周家嘴路3608号 宝龙旭辉广场</t>
+          <t>逸仙路270号  上海宝丰联大酒店</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2024.03.09 10:20-03.10 16:30</t>
+          <t>2024.03.03 10:00-03.03 17:00</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>60</t>
         </is>
       </c>
       <c r="H43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80571&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80575&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/SHH70VXN1704700240858.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/y4uWdyPT1704700763902.jpeg</t>
         </is>
       </c>
     </row>
@@ -5442,38 +5488,38 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
+          <t>上海·第五十三届燃梦星辰动漫嘉年华-随机宅舞</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>漕宝路1688号 诺宝中心酒店</t>
+          <t>周家嘴路3608号 宝龙旭辉广场</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2024.03.09 10:00-03.09 16:30</t>
+          <t>2024.03.09 10:20-03.10 16:30</t>
         </is>
       </c>
       <c r="F44" t="n">
-        <v>785</v>
+        <v>9</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>58</t>
         </is>
       </c>
       <c r="H44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=76410&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80571&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202309/fVXMrcHy1693971682397.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/SHH70VXN1704700240858.jpeg</t>
         </is>
       </c>
     </row>
@@ -5483,43 +5529,43 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2024.04.06</t>
+          <t>2024.03.09</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
+          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>复兴中路1380号 捷豹上海交响音乐厅</t>
+          <t>漕宝路1688号 诺宝中心酒店</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2024.04.06 19:30-04.06 21:30</t>
+          <t>2024.03.09 10:00-03.09 16:30</t>
         </is>
       </c>
       <c r="F45" t="n">
-        <v>10</v>
+        <v>787</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>73</t>
         </is>
       </c>
       <c r="H45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80050&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=76410&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/0iJP3TY61703056498448.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202309/fVXMrcHy1693971682397.jpeg</t>
         </is>
       </c>
     </row>
@@ -5529,26 +5575,26 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2024.04.13</t>
+          <t>2024.04.06</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>上海·《四月是你的谎言》——“公生”与“薰”的钢琴小提琴唯美经典音乐集</t>
+          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>丁香路425号 上海东方艺术中心</t>
+          <t>复兴中路1380号 捷豹上海交响音乐厅</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2024.04.13 19:30-04.13 21:30</t>
+          <t>2024.04.06 19:30-04.06 21:30</t>
         </is>
       </c>
       <c r="F46" t="n">
-        <v>140</v>
+        <v>10</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -5560,12 +5606,12 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78667&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80050&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202311/bTP7w6GD1700130122940.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/0iJP3TY61703056498448.jpeg</t>
         </is>
       </c>
     </row>
@@ -5575,26 +5621,26 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2024.05.01</t>
+          <t>2024.04.13</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>上海·  第五十三届妖漫动漫游戏展</t>
+          <t>上海·《四月是你的谎言》——“公生”与“薰”的钢琴小提琴唯美经典音乐集</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>安蒲汇塘路50号 安垦徐汇创意园</t>
+          <t>丁香路425号 上海东方艺术中心</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2024.05.01 10:00-05.02 17:00</t>
+          <t>2024.04.13 19:30-04.13 21:30</t>
         </is>
       </c>
       <c r="F47" t="n">
-        <v>82</v>
+        <v>140</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -5602,16 +5648,16 @@
         </is>
       </c>
       <c r="H47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78657&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78667&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202311/qGwPWLzO1700562869315.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202311/bTP7w6GD1700130122940.jpeg</t>
         </is>
       </c>
     </row>
@@ -5626,36 +5672,82 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
+          <t>上海·  第五十三届妖漫动漫游戏展</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>安蒲汇塘路50号 安垦徐汇创意园</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>2024.05.01 10:00-05.02 17:00</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>82</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="H48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=78657&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202311/qGwPWLzO1700562869315.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2024.05.01</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
           <t>上海·魔都野良神only</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>南京东路830号 第一百货</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr">
+      <c r="E49" t="inlineStr">
         <is>
           <t>2024.05.01 10:00-05.01 17:00</t>
         </is>
       </c>
-      <c r="F48" t="n">
-        <v>86</v>
-      </c>
-      <c r="G48" t="inlineStr">
+      <c r="F49" t="n">
+        <v>90</v>
+      </c>
+      <c r="G49" t="inlineStr">
         <is>
           <t>79</t>
         </is>
       </c>
-      <c r="H48" t="b">
-        <v>0</v>
-      </c>
-      <c r="I48" t="inlineStr">
+      <c r="H49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I49" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80321&amp;msource=Msearch_colligation</t>
         </is>
       </c>
-      <c r="J48" t="inlineStr">
+      <c r="J49" t="inlineStr">
         <is>
           <t>//i2.hdslb.com/bfs/openplatform/202401/KBlb0enU1704358750268.jpeg</t>
         </is>

</xml_diff>

<commit_message>
Update gh-pages to output generated at 2f43792
</commit_message>
<xml_diff>
--- a/上海-漫展信息.xlsx
+++ b/上海-漫展信息.xlsx
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -649,7 +649,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1580</v>
+        <v>1582</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -695,7 +695,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -741,7 +741,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>396</v>
+        <v>406</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -787,11 +787,11 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>已停售</t>
         </is>
       </c>
       <c r="H8" t="b">
@@ -833,7 +833,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>1229</v>
+        <v>1251</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -879,7 +879,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>728</v>
+        <v>756</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -925,7 +925,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>478</v>
+        <v>486</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -971,7 +971,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>235</v>
+        <v>251</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1017,7 +1017,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>784</v>
+        <v>800</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1034,7 +1034,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202312/mmvCkYYH1701411372879.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/84f8DeUY1704878485143.jpeg</t>
         </is>
       </c>
     </row>
@@ -1063,7 +1063,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1109,7 +1109,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1155,7 +1155,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1201,7 +1201,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1247,7 +1247,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1293,7 +1293,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>307</v>
+        <v>334</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1339,7 +1339,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1385,7 +1385,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>332</v>
+        <v>349</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1431,7 +1431,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1477,7 +1477,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>1704</v>
+        <v>1803</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1523,7 +1523,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1569,7 +1569,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1615,11 +1615,11 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>98</t>
         </is>
       </c>
       <c r="H26" t="b">
@@ -1661,7 +1661,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>1026</v>
+        <v>1045</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1707,7 +1707,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1753,7 +1753,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>2254</v>
+        <v>2275</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1799,7 +1799,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1845,7 +1845,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1891,7 +1891,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>787</v>
+        <v>792</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -2029,7 +2029,7 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -2075,7 +2075,7 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -2236,7 +2236,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -2282,7 +2282,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -2374,7 +2374,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>673</v>
+        <v>679</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -2466,7 +2466,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -2512,7 +2512,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -2558,7 +2558,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -2604,7 +2604,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -2696,7 +2696,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -2788,7 +2788,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -2834,7 +2834,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>486</v>
+        <v>500</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -2926,7 +2926,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -3018,7 +3018,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -3133,7 +3133,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1677</v>
+        <v>1682</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -3271,7 +3271,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1793</v>
+        <v>1812</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -3317,7 +3317,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1814</v>
+        <v>1835</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>609</v>
+        <v>615</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -3409,7 +3409,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>609</v>
+        <v>631</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -3455,7 +3455,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>493</v>
+        <v>515</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -3570,7 +3570,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1677</v>
+        <v>1682</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -3597,30 +3597,30 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2023.11.02</t>
+          <t>2023.12.01</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>上海·Hello Kitty Cosmos 50周年光影特展</t>
+          <t>上海·2023《蔚蓝档案》x  萌果酱谷子咖啡</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>漕宝路3055号 宝龙美术馆</t>
+          <t>南京东路340号百联ZX 萌果酱谷子咖啡（百联）</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023.11.02 10:00-2024.01.28 18:00</t>
+          <t>2023.12.01 00:00-2024.01.31 23:59</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>105</v>
+        <v>1812</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>139</t>
+          <t>30</t>
         </is>
       </c>
       <c r="H3" t="b">
@@ -3628,12 +3628,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77862&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79005&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202310/QnmD4yOd1698652192047.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202311/02P8eD3Z1700821985538.jpeg</t>
         </is>
       </c>
     </row>
@@ -3643,26 +3643,26 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2023.12.01</t>
+          <t>2023.12.06</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>上海·2023《蔚蓝档案》x  萌果酱谷子咖啡</t>
+          <t>上海·「咒术回战  × animate cafe」</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>南京东路340号百联ZX 萌果酱谷子咖啡（百联）</t>
+          <t>西藏北路198号大悦城北座8楼N809-1 animate cafe上海店</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023.12.01 00:00-2024.01.31 23:59</t>
+          <t>2023.12.06 00:00-2024.01.24 23:59</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1793</v>
+        <v>1835</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -3674,12 +3674,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79005&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79292&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202311/02P8eD3Z1700821985538.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/R4eAT2fR1701422895496.png</t>
         </is>
       </c>
     </row>
@@ -3689,26 +3689,26 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2023.12.06</t>
+          <t>2023.12.09</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>上海·「咒术回战  × animate cafe」</t>
+          <t>上海·非人哉官方授权主题店</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>西藏北路198号大悦城北座8楼N809-1 animate cafe上海店</t>
+          <t>南京东路830号第一百货商业中心B馆5楼(海底捞旁边) 第一百货商业中心</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023.12.06 00:00-2024.01.24 23:59</t>
+          <t>2023.12.09 00:00-2024.01.22 23:59</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1814</v>
+        <v>615</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -3720,12 +3720,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79292&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79240&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/R4eAT2fR1701422895496.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202311/hT5gYzxi1701335584641.jpeg</t>
         </is>
       </c>
     </row>
@@ -3735,30 +3735,30 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2023.12.09</t>
+          <t>2023.12.10</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>上海·非人哉官方授权主题店</t>
+          <t>上海·多维跃迁-2023 红点设计概念大奖获奖作品展</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>南京东路830号第一百货商业中心B馆5楼(海底捞旁边) 第一百货商业中心</t>
+          <t>国展路1099号 上海世博展览馆</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023.12.09 00:00-2024.01.22 23:59</t>
+          <t>2023.12.10 12:00-2024.02.16 17:00</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>609</v>
+        <v>26</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>80</t>
         </is>
       </c>
       <c r="H6" t="b">
@@ -3766,12 +3766,12 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79240&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78809&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202311/hT5gYzxi1701335584641.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202311/YsBoZAOW1700551290654.jpeg</t>
         </is>
       </c>
     </row>
@@ -3781,30 +3781,30 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2023.12.10</t>
+          <t>2023.12.22</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>上海·多维跃迁-2023 红点设计概念大奖获奖作品展</t>
+          <t>上海·新海诚导演作品《铃芽之旅》展 丨 购票抽新海诚见面会门票丨 超限定复刻原画发售</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>国展路1099号 上海世博展览馆</t>
+          <t>湖滨路168号 上海无限极荟购物中心</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023.12.10 12:00-2024.02.16 17:00</t>
+          <t>2023.12.22 10:00-2024.02.16 22:00</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>25</v>
+        <v>1582</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H7" t="b">
@@ -3812,12 +3812,12 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78809&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79166&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202311/YsBoZAOW1700551290654.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202311/MjTiIYlk1701242361853.jpeg</t>
         </is>
       </c>
     </row>
@@ -3827,30 +3827,30 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2023.12.22</t>
+          <t>2023.12.27</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>上海·新海诚导演作品《铃芽之旅》展 丨 购票抽新海诚见面会门票丨 超限定复刻原画发售</t>
+          <t>上海·爱乐汇《天空之城》久石让&amp;宫崎骏动漫经典音乐作品演奏会</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>湖滨路168号 上海无限极荟购物中心</t>
+          <t>南京西路1376号 上海商城剧院</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023.12.22 10:00-2024.02.16 22:00</t>
+          <t>2023.12.27 19:30-2024.02.03 12:00</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>1580</v>
+        <v>32</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>90</t>
         </is>
       </c>
       <c r="H8" t="b">
@@ -3858,12 +3858,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79166&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80103&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202311/MjTiIYlk1701242361853.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/2h2tIq7l1703144874867.png</t>
         </is>
       </c>
     </row>
@@ -3892,7 +3892,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>609</v>
+        <v>631</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -3919,30 +3919,30 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2024.01.06</t>
+          <t>2024.01.01</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>上海·罗小黑 x HAPPY ZOO主题Cafe</t>
+          <t>上海·沉浸式悬念剧场《9号秘事》</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>南京东路340号 百联zx创趣场</t>
+          <t>人民大道300号 上海大剧院</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2024.01.06 00:00-01.31 23:59</t>
+          <t>2024.01.01 19:30-01.28 16:20</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>493</v>
+        <v>43</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>489</t>
         </is>
       </c>
       <c r="H10" t="b">
@@ -3950,12 +3950,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80171&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79939&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/chPePM8d1703485388734.png</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/hY6FVnjM1702954652593.jpeg</t>
         </is>
       </c>
     </row>
@@ -3965,30 +3965,30 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2024.01.13</t>
+          <t>2024.01.06</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>上海·月遇国乙+代号鸢only</t>
+          <t>上海·罗小黑 x HAPPY ZOO主题Cafe</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>汶水路40号 格乐利雅GALLERIA艺术中心(大宁店)</t>
+          <t>南京东路340号 百联zx创趣场</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2024.01.13 10:40-01.13 21:00</t>
+          <t>2024.01.06 00:00-01.31 23:59</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>396</v>
+        <v>515</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H11" t="b">
@@ -3996,12 +3996,12 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79833&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80171&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/Ca51ySIK1702607429682.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/chPePM8d1703485388734.png</t>
         </is>
       </c>
     </row>
@@ -4016,25 +4016,25 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>上海·灵能百分百ONLY</t>
+          <t>上海·月遇国乙+代号鸢only</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>长江路258号 中成智谷</t>
+          <t>汶水路40号 格乐利雅GALLERIA艺术中心(大宁店)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2024.01.13 10:00-01.13 16:30</t>
+          <t>2024.01.13 10:40-01.13 21:00</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>255</v>
+        <v>406</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>95</t>
         </is>
       </c>
       <c r="H12" t="b">
@@ -4042,12 +4042,12 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80008&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79833&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/rSR9XSX01703041035213.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/Ca51ySIK1702607429682.jpeg</t>
         </is>
       </c>
     </row>
@@ -4076,7 +4076,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>1229</v>
+        <v>1251</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -4122,7 +4122,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>728</v>
+        <v>756</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -4168,7 +4168,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>478</v>
+        <v>486</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -4214,7 +4214,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>673</v>
+        <v>679</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -4306,7 +4306,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>235</v>
+        <v>251</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -4352,7 +4352,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>784</v>
+        <v>800</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -4369,7 +4369,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202312/mmvCkYYH1701411372879.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/84f8DeUY1704878485143.jpeg</t>
         </is>
       </c>
     </row>
@@ -4398,7 +4398,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -4444,7 +4444,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -4490,7 +4490,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -4536,7 +4536,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -4582,7 +4582,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -4628,7 +4628,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -4674,7 +4674,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -4720,7 +4720,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -4766,7 +4766,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>307</v>
+        <v>334</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -4812,7 +4812,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -4844,38 +4844,38 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>上海·魔都寒假漫展-CF01</t>
+          <t>上海·日本原版《数码宝贝舞台剧：游乐园之谜》</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
+          <t>茂名南路57号近长乐路 上海兰心大戏院</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.28 16:00</t>
+          <t>2024.01.27 15:30-01.27 20:55</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>332</v>
+        <v>19</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>120</t>
         </is>
       </c>
       <c r="H30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80204&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79783&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/eK96fdcg1703573110264.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/S6nZ327b1702534484951.jpeg</t>
         </is>
       </c>
     </row>
@@ -4890,38 +4890,38 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>上海•Risa Yuzuki 1st ONEMAN LIVE 「Future Interlink」 追加公演</t>
+          <t>上海·魔都寒假漫展-CF01</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>愚园路1250号 新歌空间</t>
+          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2024.01.27 18:30-01.27 21:00</t>
+          <t>2024.01.27 10:00-01.28 16:00</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>271</v>
+        <v>349</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>278</t>
+          <t>49</t>
         </is>
       </c>
       <c r="H31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77773&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80204&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202310/XKKYWAk51698315607196.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/eK96fdcg1703573110264.jpeg</t>
         </is>
       </c>
     </row>
@@ -4950,7 +4950,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -4996,7 +4996,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>1704</v>
+        <v>1803</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -5042,7 +5042,7 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -5088,7 +5088,7 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>486</v>
+        <v>500</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -5134,7 +5134,7 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -5180,11 +5180,11 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>98</t>
         </is>
       </c>
       <c r="H37" t="b">
@@ -5207,30 +5207,30 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2024.02.16</t>
+          <t>2024.02.14</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>上海·第九届次元鹿角动漫游戏展</t>
+          <t>上海·【情人节特辑】《那年我们》记忆重启韩剧经典OST音乐会《请回答1988》《来自星星的你》</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
+          <t>牛庄路704号 中国大戏院</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2024.02.16 11:00-02.17 18:00</t>
+          <t>2024.02.14 19:30-02.14 21:00</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>1026</v>
+        <v>1</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>80</t>
         </is>
       </c>
       <c r="H38" t="b">
@@ -5238,12 +5238,12 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80497&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80615&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/0duSXTQy1704423309244.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/5DDVhKcO1704767761361.png</t>
         </is>
       </c>
     </row>
@@ -5253,30 +5253,30 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2024.02.24</t>
+          <t>2024.02.16</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>上海·SISP动漫游戏嘉年华</t>
+          <t>上海·第九届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>年家浜路518号 周浦万达广场</t>
+          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2024.02.24 13:00-02.25 19:00</t>
+          <t>2024.02.16 11:00-02.17 18:00</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>60</v>
+        <v>1045</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H39" t="b">
@@ -5284,12 +5284,12 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80339&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80497&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/a8iuOufB1703832570508.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/0duSXTQy1704423309244.jpeg</t>
         </is>
       </c>
     </row>
@@ -5304,38 +5304,38 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>上海·第三届燃梦BACG PRO游戏动漫展</t>
+          <t>上海·SISP动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
+          <t>年家浜路518号 周浦万达广场</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2024.02.24 11:00-02.25 16:30</t>
+          <t>2024.02.24 13:00-02.25 19:00</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>2254</v>
+        <v>61</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>48</t>
         </is>
       </c>
       <c r="H40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77754&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80339&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202312/7eGZETK91701943985671.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/a8iuOufB1703832570508.jpeg</t>
         </is>
       </c>
     </row>
@@ -5345,43 +5345,43 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2024.02.25</t>
+          <t>2024.02.24</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>上海·青山吉能见面会</t>
+          <t>上海·第三届燃梦BACG PRO游戏动漫展</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>虹许路731号4号楼 THE BOXX•城市乐园</t>
+          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2024.02.25 14:30-02.25 19:30</t>
+          <t>2024.02.24 11:00-02.25 16:30</t>
         </is>
       </c>
       <c r="F41" t="n">
-        <v>171</v>
+        <v>2275</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80142&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=77754&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/1npuHFBM1703231674558.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/7eGZETK91701943985671.jpeg</t>
         </is>
       </c>
     </row>
@@ -5391,30 +5391,30 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2024.03.02</t>
+          <t>2024.02.25</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>上海·原神X星穹铁道ONLY</t>
+          <t>上海·青山吉能见面会</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>逸仙路301号靠纪念路路口 上海宝丰联大酒店</t>
+          <t>虹许路731号4号楼 THE BOXX•城市乐园</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2024.03.02 10:00-03.02 17:00</t>
+          <t>2024.02.25 14:30-02.25 19:30</t>
         </is>
       </c>
       <c r="F42" t="n">
-        <v>135</v>
+        <v>173</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>380</t>
         </is>
       </c>
       <c r="H42" t="b">
@@ -5422,12 +5422,12 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80299&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80142&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/V0xu26Cl1703753850690.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/1npuHFBM1703231674558.jpeg</t>
         </is>
       </c>
     </row>
@@ -5437,26 +5437,26 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2024.03.03</t>
+          <t>2024.03.02</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>上海·怀旧番ONLY</t>
+          <t>上海·原神X星穹铁道ONLY</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>逸仙路270号  上海宝丰联大酒店</t>
+          <t>逸仙路301号靠纪念路路口 上海宝丰联大酒店</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2024.03.03 10:00-03.03 17:00</t>
+          <t>2024.03.02 10:00-03.02 17:00</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>38</v>
+        <v>147</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -5468,12 +5468,12 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80575&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80299&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/y4uWdyPT1704700763902.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/V0xu26Cl1703753850690.jpeg</t>
         </is>
       </c>
     </row>
@@ -5483,43 +5483,43 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2024.03.09</t>
+          <t>2024.03.03</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>上海·第五十三届燃梦星辰动漫嘉年华-随机宅舞</t>
+          <t>上海·怀旧番ONLY</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>周家嘴路3608号 宝龙旭辉广场</t>
+          <t>逸仙路270号  上海宝丰联大酒店</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2024.03.09 10:20-03.10 16:30</t>
+          <t>2024.03.03 10:00-03.03 17:00</t>
         </is>
       </c>
       <c r="F44" t="n">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>60</t>
         </is>
       </c>
       <c r="H44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80571&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80575&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/SHH70VXN1704700240858.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/y4uWdyPT1704700763902.jpeg</t>
         </is>
       </c>
     </row>
@@ -5534,38 +5534,38 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
+          <t>上海·第五十三届燃梦星辰动漫嘉年华-随机宅舞</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>漕宝路1688号 诺宝中心酒店</t>
+          <t>周家嘴路3608号 宝龙旭辉广场</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2024.03.09 10:00-03.09 16:30</t>
+          <t>2024.03.09 10:20-03.10 16:30</t>
         </is>
       </c>
       <c r="F45" t="n">
-        <v>787</v>
+        <v>11</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>58</t>
         </is>
       </c>
       <c r="H45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=76410&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80571&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202309/fVXMrcHy1693971682397.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/SHH70VXN1704700240858.jpeg</t>
         </is>
       </c>
     </row>
@@ -5575,43 +5575,43 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2024.04.06</t>
+          <t>2024.03.09</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
+          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>复兴中路1380号 捷豹上海交响音乐厅</t>
+          <t>漕宝路1688号 诺宝中心酒店</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2024.04.06 19:30-04.06 21:30</t>
+          <t>2024.03.09 10:00-03.09 16:30</t>
         </is>
       </c>
       <c r="F46" t="n">
-        <v>10</v>
+        <v>792</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>73</t>
         </is>
       </c>
       <c r="H46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80050&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=76410&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/0iJP3TY61703056498448.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202309/fVXMrcHy1693971682397.jpeg</t>
         </is>
       </c>
     </row>
@@ -5621,26 +5621,26 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2024.04.13</t>
+          <t>2024.04.06</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>上海·《四月是你的谎言》——“公生”与“薰”的钢琴小提琴唯美经典音乐集</t>
+          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>丁香路425号 上海东方艺术中心</t>
+          <t>复兴中路1380号 捷豹上海交响音乐厅</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2024.04.13 19:30-04.13 21:30</t>
+          <t>2024.04.06 19:30-04.06 21:30</t>
         </is>
       </c>
       <c r="F47" t="n">
-        <v>140</v>
+        <v>10</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -5652,12 +5652,12 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78667&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80050&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202311/bTP7w6GD1700130122940.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/0iJP3TY61703056498448.jpeg</t>
         </is>
       </c>
     </row>
@@ -5667,26 +5667,26 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2024.05.01</t>
+          <t>2024.04.13</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>上海·  第五十三届妖漫动漫游戏展</t>
+          <t>上海·《四月是你的谎言》——“公生”与“薰”的钢琴小提琴唯美经典音乐集</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>安蒲汇塘路50号 安垦徐汇创意园</t>
+          <t>丁香路425号 上海东方艺术中心</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2024.05.01 10:00-05.02 17:00</t>
+          <t>2024.04.13 19:30-04.13 21:30</t>
         </is>
       </c>
       <c r="F48" t="n">
-        <v>82</v>
+        <v>143</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -5694,16 +5694,16 @@
         </is>
       </c>
       <c r="H48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78657&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78667&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202311/qGwPWLzO1700562869315.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202311/bTP7w6GD1700130122940.jpeg</t>
         </is>
       </c>
     </row>
@@ -5732,7 +5732,7 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update gh-pages to output generated at a56beed
</commit_message>
<xml_diff>
--- a/上海-漫展信息.xlsx
+++ b/上海-漫展信息.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>2139</v>
+        <v>2140</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -649,7 +649,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1582</v>
+        <v>1590</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -695,7 +695,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -741,7 +741,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -787,11 +787,11 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>已停售</t>
+          <t>79</t>
         </is>
       </c>
       <c r="H8" t="b">
@@ -833,7 +833,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>1251</v>
+        <v>1286</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -879,7 +879,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>756</v>
+        <v>788</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -925,7 +925,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>486</v>
+        <v>496</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -971,7 +971,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>251</v>
+        <v>276</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1017,7 +1017,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>800</v>
+        <v>816</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1063,7 +1063,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1109,7 +1109,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1155,7 +1155,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1201,7 +1201,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1247,7 +1247,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1293,7 +1293,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>334</v>
+        <v>352</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1339,7 +1339,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1385,7 +1385,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>349</v>
+        <v>358</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1431,7 +1431,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1477,7 +1477,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>1803</v>
+        <v>1889</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1569,7 +1569,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1615,7 +1615,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>83</v>
+        <v>1090</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1642,30 +1642,30 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2024.02.16</t>
+          <t>2024.02.14</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>上海·第九届次元鹿角动漫游戏展</t>
+          <t>上海·魔都COS漫展-情人节专场AM01</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
+          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2024.02.16 11:00-02.17 18:00</t>
+          <t>2024.02.14 10:00-02.14 16:00</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>1045</v>
+        <v>0</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>49</t>
         </is>
       </c>
       <c r="H27" t="b">
@@ -1673,12 +1673,12 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80497&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80691&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/0duSXTQy1704423309244.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/aSdjV6Kw1704868345679.jpeg</t>
         </is>
       </c>
     </row>
@@ -1688,30 +1688,30 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2024.02.24</t>
+          <t>2024.02.16</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>上海·SISP动漫游戏嘉年华</t>
+          <t>上海·第九届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>年家浜路518号 周浦万达广场</t>
+          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2024.02.24 13:00-02.25 19:00</t>
+          <t>2024.02.16 11:00-02.17 18:00</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>61</v>
+        <v>1054</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H28" t="b">
@@ -1719,12 +1719,12 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80339&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80497&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/a8iuOufB1703832570508.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/0duSXTQy1704423309244.jpeg</t>
         </is>
       </c>
     </row>
@@ -1739,38 +1739,38 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>上海·第三届燃梦BACG PRO游戏动漫展</t>
+          <t>上海·SISP动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
+          <t>年家浜路518号 周浦万达广场</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2024.02.24 11:00-02.25 16:30</t>
+          <t>2024.02.24 13:00-02.25 19:00</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>2275</v>
+        <v>62</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>48</t>
         </is>
       </c>
       <c r="H29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77754&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80339&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202312/7eGZETK91701943985671.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/a8iuOufB1703832570508.jpeg</t>
         </is>
       </c>
     </row>
@@ -1780,43 +1780,43 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2024.03.02</t>
+          <t>2024.02.24</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>上海·原神X星穹铁道ONLY</t>
+          <t>上海·第三届燃梦BACG PRO游戏动漫展</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>逸仙路301号靠纪念路路口 上海宝丰联大酒店</t>
+          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2024.03.02 10:00-03.02 17:00</t>
+          <t>2024.02.24 11:00-02.25 16:30</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>147</v>
+        <v>2293</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80299&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=77754&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/V0xu26Cl1703753850690.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/7eGZETK91701943985671.jpeg</t>
         </is>
       </c>
     </row>
@@ -1826,26 +1826,26 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2024.03.03</t>
+          <t>2024.03.02</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>上海·怀旧番ONLY</t>
+          <t>上海·原神X星穹铁道ONLY</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>逸仙路270号  上海宝丰联大酒店</t>
+          <t>逸仙路301号靠纪念路路口 上海宝丰联大酒店</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2024.03.03 10:00-03.03 17:00</t>
+          <t>2024.03.02 10:00-03.02 17:00</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>50</v>
+        <v>156</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1857,12 +1857,12 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80575&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80299&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/y4uWdyPT1704700763902.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/V0xu26Cl1703753850690.jpeg</t>
         </is>
       </c>
     </row>
@@ -1872,43 +1872,43 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2024.03.09</t>
+          <t>2024.03.03</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>上海·第五十三届燃梦星辰动漫嘉年华-随机宅舞</t>
+          <t>上海·怀旧番ONLY</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>周家嘴路3608号 宝龙旭辉广场</t>
+          <t>逸仙路270号  上海宝丰联大酒店</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2024.03.09 10:20-03.10 16:30</t>
+          <t>2024.03.03 10:00-03.03 17:00</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>60</t>
         </is>
       </c>
       <c r="H32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80571&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80575&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/SHH70VXN1704700240858.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/y4uWdyPT1704700763902.jpeg</t>
         </is>
       </c>
     </row>
@@ -1923,38 +1923,38 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
+          <t>上海·第五十三届燃梦星辰动漫嘉年华-随机宅舞</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>漕宝路1688号 诺宝中心酒店</t>
+          <t>周家嘴路3608号 宝龙旭辉广场</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2024.03.09 10:00-03.09 16:30</t>
+          <t>2024.03.09 10:20-03.10 16:30</t>
         </is>
       </c>
       <c r="F33" t="n">
-        <v>792</v>
+        <v>18</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>58</t>
         </is>
       </c>
       <c r="H33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=76410&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80571&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202309/fVXMrcHy1693971682397.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/SHH70VXN1704700240858.jpeg</t>
         </is>
       </c>
     </row>
@@ -1964,30 +1964,30 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2024.04.05</t>
+          <t>2024.03.09</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>上海·第四届次元鹿角动漫游戏展</t>
+          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>顾村镇蕰川路6号 智慧湾科创园</t>
+          <t>漕宝路1688号 诺宝中心酒店</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2024.04.05 10:00-04.06 17:00</t>
+          <t>2024.03.09 10:00-03.09 16:30</t>
         </is>
       </c>
       <c r="F34" t="n">
-        <v>53</v>
+        <v>800</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>73</t>
         </is>
       </c>
       <c r="H34" t="b">
@@ -1995,12 +1995,12 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78228&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=76410&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202311/jgqIFxhx1699344723568.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202309/fVXMrcHy1693971682397.jpeg</t>
         </is>
       </c>
     </row>
@@ -2010,30 +2010,30 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2024.05.01</t>
+          <t>2024.04.05</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>上海·  第五十三届妖漫动漫游戏展</t>
+          <t>上海·第四届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>安蒲汇塘路50号 安垦徐汇创意园</t>
+          <t>顾村镇蕰川路6号 智慧湾科创园</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2024.05.01 10:00-05.02 17:00</t>
+          <t>2024.04.05 10:00-04.06 17:00</t>
         </is>
       </c>
       <c r="F35" t="n">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>60</t>
         </is>
       </c>
       <c r="H35" t="b">
@@ -2041,12 +2041,12 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78657&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78228&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202311/qGwPWLzO1700562869315.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202311/jgqIFxhx1699344723568.jpeg</t>
         </is>
       </c>
     </row>
@@ -2061,36 +2061,82 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
+          <t>上海·  第五十三届妖漫动漫游戏展</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>安蒲汇塘路50号 安垦徐汇创意园</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>2024.05.01 10:00-05.02 17:00</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>85</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="H36" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=78657&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>//i1.hdslb.com/bfs/openplatform/202311/qGwPWLzO1700562869315.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2024.05.01</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
           <t>上海·魔都野良神only</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>南京东路830号 第一百货</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>2024.05.01 10:00-05.01 17:00</t>
         </is>
       </c>
-      <c r="F36" t="n">
-        <v>104</v>
-      </c>
-      <c r="G36" t="inlineStr">
+      <c r="F37" t="n">
+        <v>113</v>
+      </c>
+      <c r="G37" t="inlineStr">
         <is>
           <t>79</t>
         </is>
       </c>
-      <c r="H36" t="b">
-        <v>0</v>
-      </c>
-      <c r="I36" t="inlineStr">
+      <c r="H37" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80321&amp;msource=Msearch_colligation</t>
         </is>
       </c>
-      <c r="J36" t="inlineStr">
+      <c r="J37" t="inlineStr">
         <is>
           <t>//i2.hdslb.com/bfs/openplatform/202401/KBlb0enU1704358750268.jpeg</t>
         </is>
@@ -2107,7 +2153,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2282,7 +2328,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -2374,7 +2420,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -2420,7 +2466,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -2558,7 +2604,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -2650,7 +2696,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -2696,7 +2742,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -2742,7 +2788,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -2788,7 +2834,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -2834,7 +2880,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>500</v>
+        <v>514</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -2861,30 +2907,30 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2024.02.14</t>
+          <t>2024.02.04</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>上海·【情人节特辑】《那年我们》记忆重启韩剧经典OST音乐会《请回答1988》《来自星星的你》</t>
+          <t>上海·触手猴钢琴巡演·marasy piano live tour『生音』上海站·Powered by 东方弹幕神乐失落幻想</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>牛庄路704号 中国大戏院</t>
+          <t>丁香路425号(上海科技馆地铁站1号口步行460米) 上海东方艺术中心音乐厅</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2024.02.14 19:30-02.14 21:00</t>
+          <t>2024.02.04 19:30-02.04 21:00</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>不可售</t>
         </is>
       </c>
       <c r="H17" t="b">
@@ -2892,12 +2938,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80615&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80734&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/5DDVhKcO1704767761361.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/IcjPp0TE1704951328918.jpeg</t>
         </is>
       </c>
     </row>
@@ -2907,30 +2953,30 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2024.02.25</t>
+          <t>2024.02.14</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>上海·青山吉能见面会</t>
+          <t>上海·【情人节特辑】《那年我们》记忆重启韩剧经典OST音乐会《请回答1988》《来自星星的你》</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>虹许路731号4号楼 THE BOXX•城市乐园</t>
+          <t>牛庄路704号 中国大戏院</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2024.02.25 14:30-02.25 19:30</t>
+          <t>2024.02.14 19:30-02.14 21:00</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>173</v>
+        <v>1</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>80</t>
         </is>
       </c>
       <c r="H18" t="b">
@@ -2938,12 +2984,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80142&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80615&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/1npuHFBM1703231674558.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/5DDVhKcO1704767761361.png</t>
         </is>
       </c>
     </row>
@@ -2953,43 +2999,43 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2024.04.06</t>
+          <t>2024.02.25</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
+          <t>上海·青山吉能见面会</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>复兴中路1380号 捷豹上海交响音乐厅</t>
+          <t>虹许路731号4号楼 THE BOXX•城市乐园</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2024.04.06 19:30-04.06 21:30</t>
+          <t>2024.02.25 14:30-02.25 19:30</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>10</v>
+        <v>175</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>380</t>
         </is>
       </c>
       <c r="H19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80050&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80142&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/0iJP3TY61703056498448.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/1npuHFBM1703231674558.jpeg</t>
         </is>
       </c>
     </row>
@@ -2999,26 +3045,26 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2024.04.13</t>
+          <t>2024.04.06</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>上海·《四月是你的谎言》——“公生”与“薰”的钢琴小提琴唯美经典音乐集</t>
+          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>丁香路425号 上海东方艺术中心</t>
+          <t>复兴中路1380号 捷豹上海交响音乐厅</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2024.04.13 19:30-04.13 21:30</t>
+          <t>2024.04.06 19:30-04.06 21:30</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>143</v>
+        <v>10</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -3030,10 +3076,56 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80050&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/0iJP3TY61703056498448.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2024.04.13</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>上海·《四月是你的谎言》——“公生”与“薰”的钢琴小提琴唯美经典音乐集</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>丁香路425号 上海东方艺术中心</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2024.04.13 19:30-04.13 21:30</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>146</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
           <t>https://show.bilibili.com/platform/detail.html?id=78667&amp;msource=Msearch_colligation</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr">
+      <c r="J21" t="inlineStr">
         <is>
           <t>//i1.hdslb.com/bfs/openplatform/202311/bTP7w6GD1700130122940.jpeg</t>
         </is>
@@ -3133,7 +3225,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1682</v>
+        <v>1685</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -3179,7 +3271,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -3271,7 +3363,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1812</v>
+        <v>1827</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -3317,7 +3409,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1835</v>
+        <v>1850</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -3363,7 +3455,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -3409,7 +3501,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>631</v>
+        <v>650</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -3455,7 +3547,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>515</v>
+        <v>527</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -3570,7 +3662,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1682</v>
+        <v>1685</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -3616,7 +3708,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1812</v>
+        <v>1827</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -3662,7 +3754,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1835</v>
+        <v>1850</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -3708,7 +3800,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -3754,7 +3846,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -3800,7 +3892,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>1582</v>
+        <v>1590</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -3892,7 +3984,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>631</v>
+        <v>650</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -3919,30 +4011,30 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2024.01.01</t>
+          <t>2024.01.06</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>上海·沉浸式悬念剧场《9号秘事》</t>
+          <t>上海·罗小黑 x HAPPY ZOO主题Cafe</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>人民大道300号 上海大剧院</t>
+          <t>南京东路340号 百联zx创趣场</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2024.01.01 19:30-01.28 16:20</t>
+          <t>2024.01.06 00:00-01.31 23:59</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>43</v>
+        <v>527</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>489</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H10" t="b">
@@ -3950,12 +4042,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79939&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80171&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/hY6FVnjM1702954652593.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/chPePM8d1703485388734.png</t>
         </is>
       </c>
     </row>
@@ -3965,30 +4057,30 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2024.01.06</t>
+          <t>2024.01.13</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>上海·罗小黑 x HAPPY ZOO主题Cafe</t>
+          <t>上海·月遇国乙+代号鸢only</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>南京东路340号 百联zx创趣场</t>
+          <t>汶水路40号 格乐利雅GALLERIA艺术中心(大宁店)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2024.01.06 00:00-01.31 23:59</t>
+          <t>2024.01.13 10:40-01.13 21:00</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>515</v>
+        <v>412</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>95</t>
         </is>
       </c>
       <c r="H11" t="b">
@@ -3996,12 +4088,12 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80171&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79833&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/chPePM8d1703485388734.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/Ca51ySIK1702607429682.jpeg</t>
         </is>
       </c>
     </row>
@@ -4016,25 +4108,25 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>上海·月遇国乙+代号鸢only</t>
+          <t>上海·灵能百分百ONLY</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>汶水路40号 格乐利雅GALLERIA艺术中心(大宁店)</t>
+          <t>长江路258号 中成智谷</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2024.01.13 10:40-01.13 21:00</t>
+          <t>2024.01.13 10:00-01.13 16:30</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>406</v>
+        <v>265</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>79</t>
         </is>
       </c>
       <c r="H12" t="b">
@@ -4042,12 +4134,12 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79833&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80008&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/Ca51ySIK1702607429682.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/rSR9XSX01703041035213.jpeg</t>
         </is>
       </c>
     </row>
@@ -4076,7 +4168,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>1251</v>
+        <v>1286</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -4122,7 +4214,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>756</v>
+        <v>788</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -4168,7 +4260,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>486</v>
+        <v>496</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -4214,7 +4306,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -4241,43 +4333,43 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2024.01.19</t>
+          <t>2024.01.20</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>上海·音乐剧《三星堆》</t>
+          <t>上海·坏孩纸物语の第31届动漫节之寒假篇</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>汾阳路6号 上音歌剧院</t>
+          <t>东大名路1118号(提篮桥地铁站1号口步行340米) 影梦里</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2024.01.19 19:30-01.21 22:00</t>
+          <t>2024.01.20 11:00-01.20 17:00</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>12</v>
+        <v>276</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>180</t>
+          <t>49</t>
         </is>
       </c>
       <c r="H17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79832&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80597&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/aRlkZiIb1702607587670.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/UoNyFL4G1704707294378.png</t>
         </is>
       </c>
     </row>
@@ -4292,25 +4384,25 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>上海·坏孩纸物语の第31届动漫节之寒假篇</t>
+          <t>上海·排球少年X蓝锁X灌篮ONLY</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>东大名路1118号(提篮桥地铁站1号口步行340米) 影梦里</t>
+          <t>逸仙路270号  上海宝丰联大酒店</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2024.01.20 11:00-01.20 17:00</t>
+          <t>2024.01.20 10:00-01.20 17:00</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>251</v>
+        <v>816</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>60</t>
         </is>
       </c>
       <c r="H18" t="b">
@@ -4318,12 +4410,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80597&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79261&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/UoNyFL4G1704707294378.png</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/84f8DeUY1704878485143.jpeg</t>
         </is>
       </c>
     </row>
@@ -4338,21 +4430,21 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>上海·排球少年X蓝锁X灌篮ONLY</t>
+          <t>上海·次元裂缝-X Anikura二次元迎春派对</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>逸仙路270号  上海宝丰联大酒店</t>
+          <t>海潮路133号B1 JUMP工坊</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2024.01.20 10:00-01.20 17:00</t>
+          <t>2024.01.20 14:00-01.20 22:00</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>800</v>
+        <v>57</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -4364,12 +4456,12 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79261&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80638&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/84f8DeUY1704878485143.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/N7gT4Tza1704782642832.jpeg</t>
         </is>
       </c>
     </row>
@@ -4384,21 +4476,21 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>上海·次元裂缝-X Anikura二次元迎春派对</t>
+          <t>上海·赛马娘party·华亭迎春</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>海潮路133号B1 JUMP工坊</t>
+          <t>淞宝路96号化成路淞宝路 新长江大酒店</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2024.01.20 14:00-01.20 22:00</t>
+          <t>2024.01.20 10:00-01.20 17:00</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -4410,12 +4502,12 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80638&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80384&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/N7gT4Tza1704782642832.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/JHXTpHAw1704181759660.jpeg</t>
         </is>
       </c>
     </row>
@@ -4430,25 +4522,25 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>上海·赛马娘party·华亭迎春</t>
+          <t>上海·霓虹次元·运动番ONLY夜场2.0</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>淞宝路96号化成路淞宝路 新长江大酒店</t>
+          <t>万航渡路849号海森国际大厦3楼 Miss Club</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2024.01.20 10:00-01.20 17:00</t>
+          <t>2024.01.20 16:30-01.20 21:30</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>102</v>
+        <v>272</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>168</t>
         </is>
       </c>
       <c r="H21" t="b">
@@ -4456,12 +4548,12 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80384&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80234&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/JHXTpHAw1704181759660.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/Idm7h4dK1703646683782.jpeg</t>
         </is>
       </c>
     </row>
@@ -4471,43 +4563,43 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2024.01.20</t>
+          <t>2024.01.23</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>上海·霓虹次元·运动番ONLY夜场2.0</t>
+          <t>上海·七音阿卡莉 NANAOAKARI 2024 专场演出</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>万航渡路849号海森国际大厦3楼 Miss Club</t>
+          <t>嘉兴路街道瑞虹路188号瑞虹天地月亮湾3层 Modern Sky LAB摩登天空(瑞虹天地店)</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2024.01.20 16:30-01.20 21:30</t>
+          <t>2024.01.23 20:00-01.23 22:00</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>263</v>
+        <v>77</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>168</t>
+          <t>380</t>
         </is>
       </c>
       <c r="H22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80234&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79641&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/Idm7h4dK1703646683782.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/CoNbgCpO1703644783043.jpeg</t>
         </is>
       </c>
     </row>
@@ -4517,30 +4609,30 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2024.01.23</t>
+          <t>2024.01.26</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>上海·七音阿卡莉 NANAOAKARI 2024 专场演出</t>
+          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>嘉兴路街道瑞虹路188号瑞虹天地月亮湾3层 Modern Sky LAB摩登天空(瑞虹天地店)</t>
+          <t>丁香路425号 上海东方艺术中心</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2024.01.23 20:00-01.23 22:00</t>
+          <t>2024.01.26 19:30-01.26 21:30</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>77</v>
+        <v>142</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>80</t>
         </is>
       </c>
       <c r="H23" t="b">
@@ -4548,12 +4640,12 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79641&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78418&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/CoNbgCpO1703644783043.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202311/GHpvkT5Y1699605760230.jpeg</t>
         </is>
       </c>
     </row>
@@ -4563,43 +4655,43 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2024.01.26</t>
+          <t>2024.01.27</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
+          <t>上海·25时主题同人茶会</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>丁香路425号 上海东方艺术中心</t>
+          <t>沪太路3100号 尚大国际</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2024.01.26 19:30-01.26 21:30</t>
+          <t>2024.01.27 12:00-01.27 18:00</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>140</v>
+        <v>46</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>68</t>
         </is>
       </c>
       <c r="H24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78418&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80548&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202311/GHpvkT5Y1699605760230.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/dQ4DrxCk1704683144116.png</t>
         </is>
       </c>
     </row>
@@ -4614,17 +4706,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>上海·25时主题同人茶会</t>
+          <t>上海·Azurock」Azurose ACG Cover Live</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>沪太路3100号 尚大国际</t>
+          <t>愚园路1398号 育音堂音乐公园</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2024.01.27 12:00-01.27 18:00</t>
+          <t>2024.01.27 19:00-01.27 21:30</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -4632,7 +4724,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>88</t>
         </is>
       </c>
       <c r="H25" t="b">
@@ -4640,12 +4732,12 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80548&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80277&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/dQ4DrxCk1704683144116.png</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/5d6O1Rf11703742965244.png</t>
         </is>
       </c>
     </row>
@@ -4660,25 +4752,25 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>上海·Azurock」Azurose ACG Cover Live</t>
+          <t>上海·SISPmini动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>愚园路1398号 育音堂音乐公园</t>
+          <t>淞虹路377号 长宁ArtPark大融城</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2024.01.27 19:00-01.27 21:30</t>
+          <t>2024.01.27 13:00-01.28 19:00</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>39</v>
+        <v>207</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>48</t>
         </is>
       </c>
       <c r="H26" t="b">
@@ -4686,12 +4778,12 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80277&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79046&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202312/5d6O1Rf11703742965244.png</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202311/XmP03Vf31701070803044.jpeg</t>
         </is>
       </c>
     </row>
@@ -4706,25 +4798,25 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>上海·SISPmini动漫游戏嘉年华</t>
+          <t>上海·同好召集令火影only</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>淞虹路377号 长宁ArtPark大融城</t>
+          <t>市真南路1199弄1号 智创TOP综合体产城</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2024.01.27 13:00-01.28 19:00</t>
+          <t>2024.01.27 10:00-01.28 18:00</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>196</v>
+        <v>352</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>78</t>
         </is>
       </c>
       <c r="H27" t="b">
@@ -4732,12 +4824,12 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79046&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80284&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202311/XmP03Vf31701070803044.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/9xGb6MXN1704183627126.jpeg</t>
         </is>
       </c>
     </row>
@@ -4752,25 +4844,25 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>上海·同好召集令火影only</t>
+          <t>上海·咒术only-幽暗之森1.0</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>市真南路1199弄1号 智创TOP综合体产城</t>
+          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.28 18:00</t>
+          <t>2024.01.27 10:00-01.27 16:00</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>334</v>
+        <v>176</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>59</t>
         </is>
       </c>
       <c r="H28" t="b">
@@ -4778,12 +4870,12 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80284&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80045&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/9xGb6MXN1704183627126.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/hUfcrw3y1703055422885.jpeg</t>
         </is>
       </c>
     </row>
@@ -4798,38 +4890,38 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>上海·咒术only-幽暗之森1.0</t>
+          <t>上海·日本原版《数码宝贝舞台剧：游乐园之谜》</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
+          <t>茂名南路57号近长乐路 上海兰心大戏院</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.27 16:00</t>
+          <t>2024.01.27 15:30-01.27 20:55</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>171</v>
+        <v>20</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>120</t>
         </is>
       </c>
       <c r="H29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80045&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79783&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/hUfcrw3y1703055422885.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/S6nZ327b1702534484951.jpeg</t>
         </is>
       </c>
     </row>
@@ -4844,38 +4936,38 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>上海·日本原版《数码宝贝舞台剧：游乐园之谜》</t>
+          <t>上海·魔都寒假漫展-CF01</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>茂名南路57号近长乐路 上海兰心大戏院</t>
+          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2024.01.27 15:30-01.27 20:55</t>
+          <t>2024.01.27 10:00-01.28 16:00</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>19</v>
+        <v>358</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>49</t>
         </is>
       </c>
       <c r="H30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79783&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80204&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/S6nZ327b1702534484951.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/eK96fdcg1703573110264.jpeg</t>
         </is>
       </c>
     </row>
@@ -4890,38 +4982,38 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>上海·魔都寒假漫展-CF01</t>
+          <t>上海•Risa Yuzuki 1st ONEMAN LIVE 「Future Interlink」 追加公演</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
+          <t>愚园路1250号 新歌空间</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.28 16:00</t>
+          <t>2024.01.27 18:30-01.27 21:00</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>349</v>
+        <v>275</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>278</t>
         </is>
       </c>
       <c r="H31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80204&amp;msource=Msearch_colligation</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=77773&amp;msource=Msearch_colligation</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/eK96fdcg1703573110264.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202310/XKKYWAk51698315607196.png</t>
         </is>
       </c>
     </row>
@@ -4950,7 +5042,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -4996,7 +5088,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>1803</v>
+        <v>1889</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -5088,7 +5180,7 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>500</v>
+        <v>514</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -5134,7 +5226,7 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -5180,7 +5272,7 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>83</v>
+        <v>1090</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -5272,7 +5364,7 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>1045</v>
+        <v>1054</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -5318,7 +5410,7 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -5364,7 +5456,7 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>2275</v>
+        <v>2293</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -5410,7 +5502,7 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -5456,7 +5548,7 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -5502,7 +5594,7 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -5548,7 +5640,7 @@
         </is>
       </c>
       <c r="F45" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -5594,7 +5686,7 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>792</v>
+        <v>800</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -5686,7 +5778,7 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -5732,7 +5824,7 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update gh-pages to output generated at 90b4dfc
</commit_message>
<xml_diff>
--- a/上海-漫展信息.xlsx
+++ b/上海-漫展信息.xlsx
@@ -497,7 +497,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>上海·  第五十三届妖漫动漫游戏展</t>
+          <t>上海·Hello Kitty Cosmos 50周年光影特展</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -513,10 +513,8 @@
       <c r="F2" t="n">
         <v>116</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>139</t>
-        </is>
+      <c r="G2" t="n">
+        <v>13900</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -543,7 +541,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>上海·魔都COS漫展-情人节专场AM01</t>
+          <t>上海·多维跃迁-2023 红点设计概念大奖获奖作品展</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -559,10 +557,8 @@
       <c r="F3" t="n">
         <v>30</v>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
+      <c r="G3" t="n">
+        <v>8000</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -589,7 +585,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>上海·寻迹冬日LOVELIVE同好会</t>
+          <t>上海·新海诚导演作品《铃芽之旅》展 丨 购票抽新海诚见面会门票丨 超限定复刻原画发售</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -605,10 +601,8 @@
       <c r="F4" t="n">
         <v>1659</v>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>55</t>
-        </is>
+      <c r="G4" t="n">
+        <v>5500</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -635,7 +629,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>上海 ·WOW潮元原神x星铁主题二次元狂欢派对</t>
+          <t>上海·坏孩纸物语&amp;原神游园会（第31届动漫节）</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -649,12 +643,10 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>543</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>49</t>
-        </is>
+        <v>545</v>
+      </c>
+      <c r="G5" t="n">
+        <v>4900</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -681,38 +673,36 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>上海·Coser迎春动漫展</t>
+          <t>上海·25时主题同人茶会</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>淞虹路377号 长宁ArtPark大融城</t>
+          <t>沪太路3100号 尚大国际</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2024.01.27 13:00-01.28 19:00</t>
+          <t>2024.01.27 12:00-01.27 18:00</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>338</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
+        <v>109</v>
+      </c>
+      <c r="G6" t="n">
+        <v>6800</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79046</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80548</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202311/XmP03Vf31701070803044.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/dQ4DrxCk1704683144116.png</t>
         </is>
       </c>
     </row>
@@ -732,33 +722,31 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
+          <t>淞虹路377号 长宁ArtPark大融城</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.28 16:00</t>
+          <t>2024.01.27 13:00-01.28 19:00</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>808</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>49</t>
-        </is>
+        <v>338</v>
+      </c>
+      <c r="G7" t="n">
+        <v>4800</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80204</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79046</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/eK96fdcg1703573110264.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202311/XmP03Vf31701070803044.jpeg</t>
         </is>
       </c>
     </row>
@@ -773,38 +761,36 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>上海·第七届次元鹿角二次元派对</t>
+          <t>上海·同好召集令火影only</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>吴中路1588号上海爱琴海购物中心F4 竞梦元宇宙</t>
+          <t>市真南路1199弄1号 智创TOP综合体产城</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.28 21:00</t>
+          <t>2024.01.27 10:00-01.28 18:00</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>1094</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>68</t>
-        </is>
+        <v>503</v>
+      </c>
+      <c r="G8" t="n">
+        <v>7800</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80979</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80284</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/xPOF923U1705545223366.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/9xGb6MXN1704183627126.jpeg</t>
         </is>
       </c>
     </row>
@@ -819,38 +805,36 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>上海·第三届燃梦BACG PRO游戏动漫展-原X铁X崩同好交流</t>
+          <t>上海·咒术only-幽暗之森1.0</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>市真南路1199弄1号 智创TOP综合体产城</t>
+          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.28 18:00</t>
+          <t>2024.01.27 10:00-01.27 16:00</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>503</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>78</t>
-        </is>
+        <v>239</v>
+      </c>
+      <c r="G9" t="n">
+        <v>5900</v>
       </c>
       <c r="H9" t="b">
         <v>0</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80284</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80045</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/9xGb6MXN1704183627126.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/hUfcrw3y1703055422885.jpeg</t>
         </is>
       </c>
     </row>
@@ -865,38 +849,36 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>上海·第五十三届燃梦星辰动漫嘉年华-随机宅舞</t>
+          <t>上海·第八届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
+          <t>吴中路1588号上海爱琴海购物中心F4 竞梦元宇宙</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.27 16:00</t>
+          <t>2024.01.27 10:00-01.28 21:00</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>237</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>59</t>
-        </is>
+        <v>1094</v>
+      </c>
+      <c r="G10" t="n">
+        <v>6800</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80045</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80979</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/hUfcrw3y1703055422885.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/xPOF923U1705545223366.jpeg</t>
         </is>
       </c>
     </row>
@@ -911,38 +893,36 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
+          <t>上海·魔都寒假漫展-CF01</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>沪太路3100号 尚大国际</t>
+          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2024.01.27 12:00-01.27 18:00</t>
+          <t>2024.01.27 10:00-01.28 16:00</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>108</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>68</t>
-        </is>
+        <v>811</v>
+      </c>
+      <c r="G11" t="n">
+        <v>4900</v>
       </c>
       <c r="H11" t="b">
         <v>0</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80548</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80204</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/dQ4DrxCk1704683144116.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/eK96fdcg1703573110264.jpeg</t>
         </is>
       </c>
     </row>
@@ -955,36 +935,38 @@
           <t>2024-01-28</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>上海 ·WOW潮元原神x星铁主题二次元狂欢派对</t>
+        </is>
+      </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
+          <t>政通路189号五角场万达广场C栋 元气森林livehouse</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2024.01.28 09:30-01.28 17:00</t>
+          <t>2024.01.28 14:00-01.28 19:00</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>2225</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>不可售</t>
-        </is>
+        <v>396</v>
+      </c>
+      <c r="G12" t="n">
+        <v>12900</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78523</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80167</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/HAkxl2611705480975408.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/QTp32HEM1705028548091.jpeg</t>
         </is>
       </c>
     </row>
@@ -999,38 +981,36 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>上海·ENP电次元派对vol.04</t>
+          <t>上海·Comic World动漫游园会（取消）</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>剑川路1000号 闵行龙湖天街</t>
+          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2024.01.28 14:00-01.28 20:00</t>
+          <t>2024.01.28 09:30-01.28 17:00</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>549</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
+        <v>2225</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80871</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78523</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/5fmQrQJ81705573963752.png</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/HAkxl2611705480975408.jpeg</t>
         </is>
       </c>
     </row>
@@ -1050,33 +1030,31 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>海潮路133号B1 JUMP工坊</t>
+          <t>剑川路1000号 闵行龙湖天街</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2024.01.28 14:00-01.28 18:00</t>
+          <t>2024.01.28 14:00-01.28 20:00</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>29</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+        <v>551</v>
+      </c>
+      <c r="G14" t="n">
+        <v>3690</v>
       </c>
       <c r="H14" t="b">
         <v>0</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80999</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80871</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/lNroHqJY1705549448993.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/5fmQrQJ81705573963752.png</t>
         </is>
       </c>
     </row>
@@ -1091,38 +1069,36 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>上海·魔都野良神only</t>
+          <t>上海·次元裂缝-X 新年二次元偶像日</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>政通路189号五角场万达广场C栋 元气森林livehouse</t>
+          <t>海潮路133号B1 JUMP工坊</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2024.01.28 14:00-01.28 19:00</t>
+          <t>2024.01.28 14:00-01.28 18:00</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>395</v>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>129</t>
-        </is>
+        <v>30</v>
+      </c>
+      <c r="G15" t="n">
+        <v>6000</v>
       </c>
       <c r="H15" t="b">
         <v>0</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80167</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80999</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/QTp32HEM1705028548091.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/lNroHqJY1705549448993.jpeg</t>
         </is>
       </c>
     </row>
@@ -1137,7 +1113,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>上海·怀旧番ONLY</t>
+          <t>上海·寻迹冬日LOVELIVE同好会</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1153,10 +1129,8 @@
       <c r="F16" t="n">
         <v>178</v>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>83</t>
-        </is>
+      <c r="G16" t="n">
+        <v>8300</v>
       </c>
       <c r="H16" t="b">
         <v>0</v>
@@ -1183,7 +1157,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>上海·咒术only-幽暗之森1.0</t>
+          <t>上海·Coser迎春动漫展</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1197,12 +1171,10 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>525</v>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+        <v>528</v>
+      </c>
+      <c r="G17" t="n">
+        <v>6000</v>
       </c>
       <c r="H17" t="b">
         <v>0</v>
@@ -1229,7 +1201,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>上海·少女番only2.0</t>
+          <t>上海·ENP电次元派对vol.04</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1243,12 +1215,10 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>11</v>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>99</t>
-        </is>
+        <v>12</v>
+      </c>
+      <c r="G18" t="n">
+        <v>9900</v>
       </c>
       <c r="H18" t="b">
         <v>0</v>
@@ -1275,7 +1245,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>上海·次元裂缝-X 新年二次元偶像日</t>
+          <t>上海·第七届次元鹿角二次元派对</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1289,12 +1259,10 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>1256</v>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
+        <v>1257</v>
+      </c>
+      <c r="G19" t="n">
+        <v>9800</v>
       </c>
       <c r="H19" t="b">
         <v>0</v>
@@ -1321,7 +1289,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>上海·SISP动漫游戏嘉年华</t>
+          <t>上海·魔都COS漫展-情人节专场AM01</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1337,10 +1305,8 @@
       <c r="F20" t="n">
         <v>66</v>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>49</t>
-        </is>
+      <c r="G20" t="n">
+        <v>4900</v>
       </c>
       <c r="H20" t="b">
         <v>0</v>
@@ -1367,7 +1333,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>上海·同好召集令火影only</t>
+          <t>上海·第九届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1381,12 +1347,10 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>1174</v>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>65</t>
-        </is>
+        <v>1175</v>
+      </c>
+      <c r="G21" t="n">
+        <v>6590</v>
       </c>
       <c r="H21" t="b">
         <v>0</v>
@@ -1413,7 +1377,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>上海·坏孩纸物语の第33届动漫节之庄子篇</t>
+          <t>上海·少女番only2.0</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1427,12 +1391,10 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>120</v>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
+        <v>123</v>
+      </c>
+      <c r="G22" t="n">
+        <v>8000</v>
       </c>
       <c r="H22" t="b">
         <v>0</v>
@@ -1459,7 +1421,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>上海·Hello Kitty Cosmos 50周年光影特展</t>
+          <t>上海·SISP动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1475,10 +1437,8 @@
       <c r="F23" t="n">
         <v>104</v>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
+      <c r="G23" t="n">
+        <v>4800</v>
       </c>
       <c r="H23" t="b">
         <v>0</v>
@@ -1505,7 +1465,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>上海·坏孩纸物语&amp;原神游园会（第31届动漫节）</t>
+          <t>上海·第三届燃梦BACG PRO游戏动漫展-原X铁X崩同好交流</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1521,10 +1481,8 @@
       <c r="F24" t="n">
         <v>2444</v>
       </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>65</t>
-        </is>
+      <c r="G24" t="n">
+        <v>6580</v>
       </c>
       <c r="H24" t="b">
         <v>1</v>
@@ -1551,7 +1509,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>上海·多维跃迁-2023 红点设计概念大奖获奖作品展</t>
+          <t>上海·原神X星穹铁道ONLY</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1567,10 +1525,8 @@
       <c r="F25" t="n">
         <v>233</v>
       </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="G25" t="n">
+        <v>6000</v>
       </c>
       <c r="H25" t="b">
         <v>0</v>
@@ -1595,7 +1551,11 @@
           <t>2024-03-03</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr"/>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>上海·怀旧番ONLY</t>
+        </is>
+      </c>
       <c r="D26" t="inlineStr">
         <is>
           <t>逸仙路270号  上海宝丰联大酒店</t>
@@ -1609,10 +1569,8 @@
       <c r="F26" t="n">
         <v>111</v>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="G26" t="n">
+        <v>6000</v>
       </c>
       <c r="H26" t="b">
         <v>0</v>
@@ -1639,7 +1597,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>上海·25时主题同人茶会</t>
+          <t>上海·第五十三届燃梦星辰动漫嘉年华-随机宅舞</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1655,10 +1613,8 @@
       <c r="F27" t="n">
         <v>37</v>
       </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>58</t>
-        </is>
+      <c r="G27" t="n">
+        <v>5800</v>
       </c>
       <c r="H27" t="b">
         <v>1</v>
@@ -1685,7 +1641,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>上海·新海诚导演作品《铃芽之旅》展 丨 购票抽新海诚见面会门票丨 超限定复刻原画发售</t>
+          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1701,10 +1657,8 @@
       <c r="F28" t="n">
         <v>853</v>
       </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>73</t>
-        </is>
+      <c r="G28" t="n">
+        <v>7300</v>
       </c>
       <c r="H28" t="b">
         <v>0</v>
@@ -1731,7 +1685,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>上海·灌篮高手--青春永不散场</t>
+          <t>上海·坏孩纸物语の第33届动漫节之庄子篇</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1745,12 +1699,10 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>5</v>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
+        <v>6</v>
+      </c>
+      <c r="G29" t="n">
+        <v>4000</v>
       </c>
       <c r="H29" t="b">
         <v>0</v>
@@ -1777,7 +1729,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>上海·第八届次元鹿角动漫游戏展</t>
+          <t>上海·第四届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1793,10 +1745,8 @@
       <c r="F30" t="n">
         <v>60</v>
       </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="G30" t="n">
+        <v>6000</v>
       </c>
       <c r="H30" t="b">
         <v>0</v>
@@ -1823,7 +1773,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>上海·第四届次元鹿角动漫游戏展</t>
+          <t>上海·  第五十三届妖漫动漫游戏展</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1839,10 +1789,8 @@
       <c r="F31" t="n">
         <v>145</v>
       </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
+      <c r="G31" t="n">
+        <v>8000</v>
       </c>
       <c r="H31" t="b">
         <v>0</v>
@@ -1869,7 +1817,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>上海·魔都寒假漫展-CF01</t>
+          <t>上海·魔都野良神only</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1885,10 +1833,8 @@
       <c r="F32" t="n">
         <v>173</v>
       </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>79</t>
-        </is>
+      <c r="G32" t="n">
+        <v>7900</v>
       </c>
       <c r="H32" t="b">
         <v>0</v>
@@ -1915,7 +1861,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>上海·Comic World动漫游园会（取消）</t>
+          <t>上海·灌篮高手--青春永不散场</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1931,10 +1877,8 @@
       <c r="F33" t="n">
         <v>6</v>
       </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>89</t>
-        </is>
+      <c r="G33" t="n">
+        <v>8900</v>
       </c>
       <c r="H33" t="b">
         <v>0</v>
@@ -2030,7 +1974,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>上海·日本原版《数码宝贝舞台剧：游乐园之谜》</t>
+          <t>上海·爱乐汇“浪漫经典·一生必听”永恒精选2023烛光音乐会</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2046,10 +1990,8 @@
       <c r="F2" t="n">
         <v>21</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="G2" t="n">
+        <v>9000</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -2076,7 +2018,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
+          <t>上海·爱乐汇《天空之城》久石让&amp;宫崎骏动漫经典音乐作品演奏会</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2092,10 +2034,8 @@
       <c r="F3" t="n">
         <v>39</v>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="G3" t="n">
+        <v>9000</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -2122,7 +2062,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>上海·音乐剧《三星堆》</t>
+          <t>上海·沉浸式悬念剧场《9号秘事》</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2138,10 +2078,8 @@
       <c r="F4" t="n">
         <v>50</v>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>已停售</t>
-        </is>
+      <c r="G4" t="n">
+        <v>0</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -2168,7 +2106,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>上海·amazarashi Asia Tour 2024 「永遠市 -Eternal City-」上海公演</t>
+          <t>上海·音乐剧《三星堆》</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2184,10 +2122,8 @@
       <c r="F5" t="n">
         <v>18</v>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>已停售</t>
-        </is>
+      <c r="G5" t="n">
+        <v>0</v>
       </c>
       <c r="H5" t="b">
         <v>1</v>
@@ -2214,7 +2150,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>上海·次元LAB 二次元电音节</t>
+          <t>上海·七音阿卡莉 NANAOAKARI 2024 专场演出</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -2230,10 +2166,8 @@
       <c r="F6" t="n">
         <v>88</v>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>380</t>
-        </is>
+      <c r="G6" t="n">
+        <v>38000</v>
       </c>
       <c r="H6" t="b">
         <v>1</v>
@@ -2260,7 +2194,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>上海·青山吉能见面会</t>
+          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -2276,10 +2210,8 @@
       <c r="F7" t="n">
         <v>159</v>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
+      <c r="G7" t="n">
+        <v>8000</v>
       </c>
       <c r="H7" t="b">
         <v>1</v>
@@ -2306,7 +2238,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>上海·七音阿卡莉 NANAOAKARI 2024 专场演出</t>
+          <t>上海·Azurock」Azurose ACG Cover Live</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -2322,10 +2254,8 @@
       <c r="F8" t="n">
         <v>50</v>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>88</t>
-        </is>
+      <c r="G8" t="n">
+        <v>8800</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -2352,7 +2282,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>上海·三月的幻想演唱会2024「飞越蓝色时刻」</t>
+          <t>上海·日本原版《数码宝贝舞台剧：游乐园之谜》</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -2368,10 +2298,8 @@
       <c r="F9" t="n">
         <v>29</v>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
+      <c r="G9" t="n">
+        <v>12000</v>
       </c>
       <c r="H9" t="b">
         <v>1</v>
@@ -2398,7 +2326,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>上海·爱乐汇“浪漫经典·一生必听”永恒精选2023烛光音乐会</t>
+          <t>上海•Risa Yuzuki 1st ONEMAN LIVE 「Future Interlink」 追加公演</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -2414,10 +2342,8 @@
       <c r="F10" t="n">
         <v>294</v>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>278</t>
-        </is>
+      <c r="G10" t="n">
+        <v>27800</v>
       </c>
       <c r="H10" t="b">
         <v>1</v>
@@ -2444,7 +2370,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
+          <t>上海·次元LAB 二次元电音节</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -2460,10 +2386,8 @@
       <c r="F11" t="n">
         <v>605</v>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>380</t>
-        </is>
+      <c r="G11" t="n">
+        <v>38000</v>
       </c>
       <c r="H11" t="b">
         <v>1</v>
@@ -2490,7 +2414,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>上海·《四月是你的谎言》——“公生”与“薰”的钢琴小提琴唯美经典音乐集</t>
+          <t>上海·触手猴钢琴巡演·marasy piano live tour『生音』上海站·Powered by 东方弹幕神乐失落幻想</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -2504,12 +2428,10 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>289</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>480</t>
-        </is>
+        <v>293</v>
+      </c>
+      <c r="G12" t="n">
+        <v>48000</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
@@ -2534,7 +2456,11 @@
           <t>2024-02-14</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>上海·【情人节特辑】《那年我们》记忆重启韩剧经典OST音乐会《请回答1988》《来自星星的你》</t>
+        </is>
+      </c>
       <c r="D13" t="inlineStr">
         <is>
           <t>牛庄路704号 中国大戏院</t>
@@ -2548,10 +2474,8 @@
       <c r="F13" t="n">
         <v>2</v>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>已停售</t>
-        </is>
+      <c r="G13" t="n">
+        <v>0</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
@@ -2578,7 +2502,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>上海·《笑傲江湖》经典武侠影视金曲音乐会</t>
+          <t>上海·《哈利的魔法世界》动漫视听音乐会</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -2594,10 +2518,8 @@
       <c r="F14" t="n">
         <v>4</v>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>158</t>
-        </is>
+      <c r="G14" t="n">
+        <v>15800</v>
       </c>
       <c r="H14" t="b">
         <v>0</v>
@@ -2624,7 +2546,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>上海·爱乐汇《天空之城》久石让&amp;宫崎骏动漫经典音乐作品演奏会</t>
+          <t>上海·青山吉能见面会</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -2640,10 +2562,8 @@
       <c r="F15" t="n">
         <v>194</v>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>380</t>
-        </is>
+      <c r="G15" t="n">
+        <v>38000</v>
       </c>
       <c r="H15" t="b">
         <v>0</v>
@@ -2668,7 +2588,11 @@
           <t>2024-03-02</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>上海·2024藤田玲上海粉丝见面会</t>
+        </is>
+      </c>
       <c r="D16" t="inlineStr">
         <is>
           <t>宜昌路179号 万代南梦宫上海文化中心</t>
@@ -2682,10 +2606,8 @@
       <c r="F16" t="n">
         <v>3</v>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>580</t>
-        </is>
+      <c r="G16" t="n">
+        <v>58000</v>
       </c>
       <c r="H16" t="b">
         <v>1</v>
@@ -2712,7 +2634,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>上海· TRUE（唐沢美帆）上海动漫交响音乐会</t>
+          <t>上海·小山百代2024上海粉丝见面会</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -2728,10 +2650,8 @@
       <c r="F17" t="n">
         <v>208</v>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>380</t>
-        </is>
+      <c r="G17" t="n">
+        <v>38000</v>
       </c>
       <c r="H17" t="b">
         <v>1</v>
@@ -2758,7 +2678,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>上海·2024藤田玲上海粉丝见面会</t>
+          <t>上海·三月的幻想演唱会2024「飞越蓝色时刻」</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -2774,10 +2694,8 @@
       <c r="F18" t="n">
         <v>35</v>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>380</t>
-        </is>
+      <c r="G18" t="n">
+        <v>38000</v>
       </c>
       <c r="H18" t="b">
         <v>0</v>
@@ -2804,7 +2722,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>上海· 夏川里美 2024 巡回演唱会 出道 25 周年纪念专场</t>
+          <t>上海 ·《疯狂动物城》动漫视听音乐会</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -2814,28 +2732,26 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2024.03.17 19:30-03.17 21:00</t>
+          <t>2024.03.17 15:30-03.17 17:00</t>
         </is>
       </c>
       <c r="F19" t="n">
         <v>1</v>
       </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
+      <c r="G19" t="n">
+        <v>8000</v>
       </c>
       <c r="H19" t="b">
         <v>0</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80875</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81112</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/8AwIAy4I1705385447242.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/Wg8b6SRn1705651166088.png</t>
         </is>
       </c>
     </row>
@@ -2850,7 +2766,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>上海·【情人节特辑】《那年我们》记忆重启韩剧经典OST音乐会《请回答1988》《来自星星的你》</t>
+          <t>上海·amazarashi Asia Tour 2024 「永遠市 -Eternal City-」上海公演</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -2864,12 +2780,10 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>193</v>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>480</t>
-        </is>
+        <v>196</v>
+      </c>
+      <c r="G20" t="n">
+        <v>48000</v>
       </c>
       <c r="H20" t="b">
         <v>0</v>
@@ -2896,7 +2810,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>上海·沉浸式悬念剧场《9号秘事》</t>
+          <t>上海·《笑傲江湖》经典武侠影视金曲音乐会</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -2906,28 +2820,26 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2024.03.17 15:30-03.17 17:00</t>
+          <t>2024.03.17 19:30-03.17 21:00</t>
         </is>
       </c>
       <c r="F21" t="n">
         <v>1</v>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
+      <c r="G21" t="n">
+        <v>8000</v>
       </c>
       <c r="H21" t="b">
         <v>0</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81112</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80875</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/Wg8b6SRn1705651166088.png</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/8AwIAy4I1705385447242.jpeg</t>
         </is>
       </c>
     </row>
@@ -2942,7 +2854,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>上海·触手猴钢琴巡演·marasy piano live tour『生音』上海站·Powered by 东方弹幕神乐失落幻想</t>
+          <t>上海· TRUE（唐沢美帆）上海动漫交响音乐会</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2956,12 +2868,10 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>110</v>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>480</t>
-        </is>
+        <v>112</v>
+      </c>
+      <c r="G22" t="n">
+        <v>48000</v>
       </c>
       <c r="H22" t="b">
         <v>0</v>
@@ -2988,7 +2898,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>上海•Risa Yuzuki 1st ONEMAN LIVE 「Future Interlink」 追加公演</t>
+          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -3004,10 +2914,8 @@
       <c r="F23" t="n">
         <v>10</v>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
+      <c r="G23" t="n">
+        <v>8000</v>
       </c>
       <c r="H23" t="b">
         <v>1</v>
@@ -3034,7 +2942,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>上海·Azurock」Azurose ACG Cover Live</t>
+          <t>上海·《四月是你的谎言》——“公生”与“薰”的钢琴小提琴唯美经典音乐集</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -3050,10 +2958,8 @@
       <c r="F24" t="n">
         <v>166</v>
       </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
+      <c r="G24" t="n">
+        <v>8000</v>
       </c>
       <c r="H24" t="b">
         <v>1</v>
@@ -3080,7 +2986,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>上海 ·《疯狂动物城》动漫视听音乐会</t>
+          <t>上海·Laurent Coulondre“心动巴黎”2024中国巡回音乐会</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -3096,10 +3002,8 @@
       <c r="F25" t="n">
         <v>3</v>
       </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
+      <c r="G25" t="n">
+        <v>8000</v>
       </c>
       <c r="H25" t="b">
         <v>0</v>
@@ -3126,7 +3030,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>上海·Laurent Coulondre“心动巴黎”2024中国巡回音乐会</t>
+          <t>上海· 夏川里美 2024 巡回演唱会 出道 25 周年纪念专场</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -3142,10 +3046,8 @@
       <c r="F26" t="n">
         <v>6</v>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>280</t>
-        </is>
+      <c r="G26" t="n">
+        <v>28000</v>
       </c>
       <c r="H26" t="b">
         <v>0</v>
@@ -3241,7 +3143,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>上海·古影文化《1941·新和医院》大型沉浸式互动剧场</t>
+          <t>上海·日漫咖啡体验</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -3257,10 +3159,8 @@
       <c r="F2" t="n">
         <v>1715</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="G2" t="n">
+        <v>6000</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -3287,7 +3187,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>上海·方块大战（豫园店）</t>
+          <t>上海·古影文化《1941·新和医院》大型沉浸式互动剧场</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -3303,10 +3203,8 @@
       <c r="F3" t="n">
         <v>68</v>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>996</t>
-        </is>
+      <c r="G3" t="n">
+        <v>99600</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -3331,7 +3229,11 @@
           <t>2023-10-25</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>上海·方块大战（豫园店）</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>丽水路88号2楼213 城隍庙第一购物中心</t>
@@ -3345,10 +3247,8 @@
       <c r="F4" t="n">
         <v>35</v>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>49</t>
-        </is>
+      <c r="G4" t="n">
+        <v>4990</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -3375,7 +3275,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>上海·次元波板糖×时光代理人「锦瑟华年主题快闪店」</t>
+          <t>上海·2023《蔚蓝档案》x  萌果酱谷子咖啡</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -3391,10 +3291,8 @@
       <c r="F5" t="n">
         <v>1955</v>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="G5" t="n">
+        <v>3000</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -3421,7 +3319,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>上海·非人哉官方授权主题店</t>
+          <t>上海·「咒术回战  × animate cafe」</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -3435,12 +3333,10 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>2036</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+        <v>2040</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3000</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -3467,7 +3363,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>上海·2023《蔚蓝档案》x  萌果酱谷子咖啡</t>
+          <t>上海·非人哉官方授权主题店</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -3483,10 +3379,8 @@
       <c r="F7" t="n">
         <v>669</v>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="G7" t="n">
+        <v>3000</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
@@ -3513,7 +3407,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>上海·日漫咖啡体验</t>
+          <t>上海·次元波板糖×时光代理人「锦瑟华年主题快闪店」</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -3527,12 +3421,10 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>793</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+        <v>794</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3000</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -3559,7 +3451,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>上海·「咒术回战  × animate cafe」</t>
+          <t>上海·罗小黑 x HAPPY ZOO主题Cafe</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -3575,10 +3467,8 @@
       <c r="F9" t="n">
         <v>676</v>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="G9" t="n">
+        <v>1000</v>
       </c>
       <c r="H9" t="b">
         <v>0</v>
@@ -3674,7 +3564,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>上海·第五十三届燃梦星辰动漫嘉年华-随机宅舞</t>
+          <t>上海·日漫咖啡体验</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -3690,10 +3580,8 @@
       <c r="F2" t="n">
         <v>1715</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="G2" t="n">
+        <v>6000</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -3720,7 +3608,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>上海•Risa Yuzuki 1st ONEMAN LIVE 「Future Interlink」 追加公演</t>
+          <t>上海·古影文化《1941·新和医院》大型沉浸式互动剧场</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -3736,10 +3624,8 @@
       <c r="F3" t="n">
         <v>68</v>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>996</t>
-        </is>
+      <c r="G3" t="n">
+        <v>99600</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -3766,7 +3652,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>上海·  第五十三届妖漫动漫游戏展</t>
+          <t>上海·方块大战（豫园店）</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -3782,10 +3668,8 @@
       <c r="F4" t="n">
         <v>35</v>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>49</t>
-        </is>
+      <c r="G4" t="n">
+        <v>4990</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -3812,7 +3696,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>上海·方块大战（豫园店）</t>
+          <t>上海·Hello Kitty Cosmos 50周年光影特展</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -3828,10 +3712,8 @@
       <c r="F5" t="n">
         <v>116</v>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>139</t>
-        </is>
+      <c r="G5" t="n">
+        <v>13900</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -3858,7 +3740,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>上海·SISPmini动漫游戏嘉年华</t>
+          <t>上海·2023《蔚蓝档案》x  萌果酱谷子咖啡</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -3874,10 +3756,8 @@
       <c r="F6" t="n">
         <v>1955</v>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="G6" t="n">
+        <v>3000</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -3904,7 +3784,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>上海·《四月是你的谎言》——“公生”与“薰”的钢琴小提琴唯美经典音乐集</t>
+          <t>上海·「咒术回战  × animate cafe」</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -3918,12 +3798,10 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>2036</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+        <v>2040</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3000</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
@@ -3950,7 +3828,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>上海·魔都寒假漫展-CF01</t>
+          <t>上海·非人哉官方授权主题店</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -3966,10 +3844,8 @@
       <c r="F8" t="n">
         <v>669</v>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="G8" t="n">
+        <v>3000</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -3996,7 +3872,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>上海·爱乐汇《天空之城》久石让&amp;宫崎骏动漫经典音乐作品演奏会</t>
+          <t>上海·多维跃迁-2023 红点设计概念大奖获奖作品展</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -4012,10 +3888,8 @@
       <c r="F9" t="n">
         <v>30</v>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
+      <c r="G9" t="n">
+        <v>8000</v>
       </c>
       <c r="H9" t="b">
         <v>0</v>
@@ -4042,7 +3916,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>上海·寻迹冬日LOVELIVE同好会</t>
+          <t>上海·新海诚导演作品《铃芽之旅》展 丨 购票抽新海诚见面会门票丨 超限定复刻原画发售</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -4058,10 +3932,8 @@
       <c r="F10" t="n">
         <v>1659</v>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>55</t>
-        </is>
+      <c r="G10" t="n">
+        <v>5500</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
@@ -4088,7 +3960,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>上海·日本原版《数码宝贝舞台剧：游乐园之谜》</t>
+          <t>上海·爱乐汇“浪漫经典·一生必听”永恒精选2023烛光音乐会</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -4104,10 +3976,8 @@
       <c r="F11" t="n">
         <v>21</v>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="G11" t="n">
+        <v>9000</v>
       </c>
       <c r="H11" t="b">
         <v>0</v>
@@ -4132,7 +4002,11 @@
           <t>2023-12-27</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>上海·爱乐汇《天空之城》久石让&amp;宫崎骏动漫经典音乐作品演奏会</t>
+        </is>
+      </c>
       <c r="D12" t="inlineStr">
         <is>
           <t>南京西路1376号 上海商城剧院</t>
@@ -4146,10 +4020,8 @@
       <c r="F12" t="n">
         <v>39</v>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="G12" t="n">
+        <v>9000</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
@@ -4176,7 +4048,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>上海·Coser迎春动漫展</t>
+          <t>上海·次元波板糖×时光代理人「锦瑟华年主题快闪店」</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -4190,12 +4062,10 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>793</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+        <v>794</v>
+      </c>
+      <c r="G13" t="n">
+        <v>3000</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
@@ -4222,7 +4092,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>上海·坏孩纸物语&amp;原神游园会（第31届动漫节）</t>
+          <t>上海·罗小黑 x HAPPY ZOO主题Cafe</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -4238,10 +4108,8 @@
       <c r="F14" t="n">
         <v>676</v>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="G14" t="n">
+        <v>1000</v>
       </c>
       <c r="H14" t="b">
         <v>0</v>
@@ -4268,7 +4136,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>上海·触手猴钢琴巡演·marasy piano live tour『生音』上海站·Powered by 东方弹幕神乐失落幻想</t>
+          <t>上海·坏孩纸物语&amp;原神游园会（第31届动漫节）</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -4282,12 +4150,10 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>543</v>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>49</t>
-        </is>
+        <v>545</v>
+      </c>
+      <c r="G15" t="n">
+        <v>4900</v>
       </c>
       <c r="H15" t="b">
         <v>0</v>
@@ -4314,7 +4180,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>上海·怀旧番ONLY</t>
+          <t>上海·七音阿卡莉 NANAOAKARI 2024 专场演出</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -4330,10 +4196,8 @@
       <c r="F16" t="n">
         <v>88</v>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>380</t>
-        </is>
+      <c r="G16" t="n">
+        <v>38000</v>
       </c>
       <c r="H16" t="b">
         <v>1</v>
@@ -4360,7 +4224,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>上海·青山吉能见面会</t>
+          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -4376,10 +4240,8 @@
       <c r="F17" t="n">
         <v>159</v>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
+      <c r="G17" t="n">
+        <v>8000</v>
       </c>
       <c r="H17" t="b">
         <v>1</v>
@@ -4406,38 +4268,36 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>上海·2023《蔚蓝档案》x  萌果酱谷子咖啡</t>
+          <t>上海·25时主题同人茶会</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
+          <t>沪太路3100号 尚大国际</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.28 16:00</t>
+          <t>2024.01.27 12:00-01.27 18:00</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>808</v>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>49</t>
-        </is>
+        <v>109</v>
+      </c>
+      <c r="G18" t="n">
+        <v>6800</v>
       </c>
       <c r="H18" t="b">
         <v>0</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80204</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80548</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/eK96fdcg1703573110264.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/dQ4DrxCk1704683144116.png</t>
         </is>
       </c>
     </row>
@@ -4452,7 +4312,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>上海·七音阿卡莉 NANAOAKARI 2024 专场演出</t>
+          <t>上海·Azurock」Azurose ACG Cover Live</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -4468,10 +4328,8 @@
       <c r="F19" t="n">
         <v>50</v>
       </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>88</t>
-        </is>
+      <c r="G19" t="n">
+        <v>8800</v>
       </c>
       <c r="H19" t="b">
         <v>0</v>
@@ -4498,38 +4356,36 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>上海·小山百代2024上海粉丝见面会</t>
+          <t>上海·SISPmini动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>茂名南路57号近长乐路 上海兰心大戏院</t>
+          <t>淞虹路377号 长宁ArtPark大融城</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2024.01.27 15:30-01.27 20:55</t>
+          <t>2024.01.27 13:00-01.28 19:00</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>29</v>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
+        <v>338</v>
+      </c>
+      <c r="G20" t="n">
+        <v>4800</v>
       </c>
       <c r="H20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79783</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79046</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/S6nZ327b1702534484951.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202311/XmP03Vf31701070803044.jpeg</t>
         </is>
       </c>
     </row>
@@ -4544,38 +4400,36 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>上海·日漫咖啡体验</t>
+          <t>上海·同好召集令火影only</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
+          <t>市真南路1199弄1号 智创TOP综合体产城</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.27 16:00</t>
+          <t>2024.01.27 10:00-01.28 18:00</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>237</v>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>59</t>
-        </is>
+        <v>503</v>
+      </c>
+      <c r="G21" t="n">
+        <v>7800</v>
       </c>
       <c r="H21" t="b">
         <v>0</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80045</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80284</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/hUfcrw3y1703055422885.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/9xGb6MXN1704183627126.jpeg</t>
         </is>
       </c>
     </row>
@@ -4590,38 +4444,36 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>上海·次元波板糖×时光代理人「锦瑟华年主题快闪店」</t>
+          <t>上海·咒术only-幽暗之森1.0</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>淞虹路377号 长宁ArtPark大融城</t>
+          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2024.01.27 13:00-01.28 19:00</t>
+          <t>2024.01.27 10:00-01.27 16:00</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>338</v>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
+        <v>239</v>
+      </c>
+      <c r="G22" t="n">
+        <v>5900</v>
       </c>
       <c r="H22" t="b">
         <v>0</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79046</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80045</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202311/XmP03Vf31701070803044.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/hUfcrw3y1703055422885.jpeg</t>
         </is>
       </c>
     </row>
@@ -4636,38 +4488,36 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>上海·第七届次元鹿角二次元派对</t>
+          <t>上海·日本原版《数码宝贝舞台剧：游乐园之谜》</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>吴中路1588号上海爱琴海购物中心F4 竞梦元宇宙</t>
+          <t>茂名南路57号近长乐路 上海兰心大戏院</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.28 21:00</t>
+          <t>2024.01.27 15:30-01.27 20:55</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>1094</v>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>68</t>
-        </is>
+        <v>29</v>
+      </c>
+      <c r="G23" t="n">
+        <v>12000</v>
       </c>
       <c r="H23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80979</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79783</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/xPOF923U1705545223366.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/S6nZ327b1702534484951.jpeg</t>
         </is>
       </c>
     </row>
@@ -4682,38 +4532,36 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>上海·第三届燃梦BACG PRO游戏动漫展-原X铁X崩同好交流</t>
+          <t>上海·第八届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>市真南路1199弄1号 智创TOP综合体产城</t>
+          <t>吴中路1588号上海爱琴海购物中心F4 竞梦元宇宙</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.28 18:00</t>
+          <t>2024.01.27 10:00-01.28 21:00</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>503</v>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>78</t>
-        </is>
+        <v>1094</v>
+      </c>
+      <c r="G24" t="n">
+        <v>6800</v>
       </c>
       <c r="H24" t="b">
         <v>0</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80284</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80979</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/9xGb6MXN1704183627126.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/xPOF923U1705545223366.jpeg</t>
         </is>
       </c>
     </row>
@@ -4728,38 +4576,36 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
+          <t>上海·魔都寒假漫展-CF01</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>沪太路3100号 尚大国际</t>
+          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2024.01.27 12:00-01.27 18:00</t>
+          <t>2024.01.27 10:00-01.28 16:00</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>108</v>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>68</t>
-        </is>
+        <v>811</v>
+      </c>
+      <c r="G25" t="n">
+        <v>4900</v>
       </c>
       <c r="H25" t="b">
         <v>0</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80548</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80204</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/dQ4DrxCk1704683144116.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/eK96fdcg1703573110264.jpeg</t>
         </is>
       </c>
     </row>
@@ -4774,7 +4620,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>上海·魔都COS漫展-情人节专场AM01</t>
+          <t>上海•Risa Yuzuki 1st ONEMAN LIVE 「Future Interlink」 追加公演</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -4790,10 +4636,8 @@
       <c r="F26" t="n">
         <v>294</v>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>278</t>
-        </is>
+      <c r="G26" t="n">
+        <v>27800</v>
       </c>
       <c r="H26" t="b">
         <v>1</v>
@@ -4820,7 +4664,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>上海·「咒术回战  × animate cafe」</t>
+          <t>上海 ·WOW潮元原神x星铁主题二次元狂欢派对</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -4834,12 +4678,10 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>395</v>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>129</t>
-        </is>
+        <v>396</v>
+      </c>
+      <c r="G27" t="n">
+        <v>12900</v>
       </c>
       <c r="H27" t="b">
         <v>0</v>
@@ -4866,7 +4708,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>上海·Azurock」Azurose ACG Cover Live</t>
+          <t>上海·寻迹冬日LOVELIVE同好会</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -4882,10 +4724,8 @@
       <c r="F28" t="n">
         <v>178</v>
       </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>83</t>
-        </is>
+      <c r="G28" t="n">
+        <v>8300</v>
       </c>
       <c r="H28" t="b">
         <v>0</v>
@@ -4912,7 +4752,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
+          <t>上海·次元LAB 二次元电音节</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -4928,10 +4768,8 @@
       <c r="F29" t="n">
         <v>605</v>
       </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>380</t>
-        </is>
+      <c r="G29" t="n">
+        <v>38000</v>
       </c>
       <c r="H29" t="b">
         <v>1</v>
@@ -4956,7 +4794,11 @@
           <t>2024-02-03</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr"/>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>上海·Coser迎春动漫展</t>
+        </is>
+      </c>
       <c r="D30" t="inlineStr">
         <is>
           <t>海潮路133号B1 JUMP工坊</t>
@@ -4968,12 +4810,10 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>525</v>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+        <v>528</v>
+      </c>
+      <c r="G30" t="n">
+        <v>6000</v>
       </c>
       <c r="H30" t="b">
         <v>0</v>
@@ -5000,7 +4840,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>上海· TRUE（唐沢美帆）上海动漫交响音乐会</t>
+          <t>上海·第七届次元鹿角二次元派对</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -5014,12 +4854,10 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>1256</v>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
+        <v>1257</v>
+      </c>
+      <c r="G31" t="n">
+        <v>9800</v>
       </c>
       <c r="H31" t="b">
         <v>0</v>
@@ -5046,7 +4884,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>上海 ·WOW潮元原神x星铁主题二次元狂欢派对</t>
+          <t>上海·触手猴钢琴巡演·marasy piano live tour『生音』上海站·Powered by 东方弹幕神乐失落幻想</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -5060,12 +4898,10 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>289</v>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>480</t>
-        </is>
+        <v>293</v>
+      </c>
+      <c r="G32" t="n">
+        <v>48000</v>
       </c>
       <c r="H32" t="b">
         <v>0</v>
@@ -5092,7 +4928,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>上海·SISP动漫游戏嘉年华</t>
+          <t>上海·魔都COS漫展-情人节专场AM01</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -5108,10 +4944,8 @@
       <c r="F33" t="n">
         <v>66</v>
       </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>49</t>
-        </is>
+      <c r="G33" t="n">
+        <v>4900</v>
       </c>
       <c r="H33" t="b">
         <v>0</v>
@@ -5138,7 +4972,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>上海·同好召集令火影only</t>
+          <t>上海·第九届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -5152,12 +4986,10 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>1174</v>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>65</t>
-        </is>
+        <v>1175</v>
+      </c>
+      <c r="G34" t="n">
+        <v>6590</v>
       </c>
       <c r="H34" t="b">
         <v>0</v>
@@ -5184,7 +5016,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>上海·Hello Kitty Cosmos 50周年光影特展</t>
+          <t>上海·SISP动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -5200,10 +5032,8 @@
       <c r="F35" t="n">
         <v>104</v>
       </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
+      <c r="G35" t="n">
+        <v>4800</v>
       </c>
       <c r="H35" t="b">
         <v>0</v>
@@ -5230,7 +5060,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>上海·罗小黑 x HAPPY ZOO主题Cafe</t>
+          <t>上海·第三届燃梦BACG PRO游戏动漫展-原X铁X崩同好交流</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -5246,10 +5076,8 @@
       <c r="F36" t="n">
         <v>2444</v>
       </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>65</t>
-        </is>
+      <c r="G36" t="n">
+        <v>6580</v>
       </c>
       <c r="H36" t="b">
         <v>1</v>
@@ -5276,7 +5104,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>上海·多维跃迁-2023 红点设计概念大奖获奖作品展</t>
+          <t>上海·青山吉能见面会</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -5292,10 +5120,8 @@
       <c r="F37" t="n">
         <v>194</v>
       </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>380</t>
-        </is>
+      <c r="G37" t="n">
+        <v>38000</v>
       </c>
       <c r="H37" t="b">
         <v>0</v>
@@ -5322,38 +5148,36 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>上海· TRUE（唐沢美帆）上海动漫交响音乐会</t>
+          <t>上海·原神X星穹铁道ONLY</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>宜昌路179号 万代南梦宫上海文化中心</t>
+          <t>逸仙路301号靠纪念路路口 上海宝丰联大酒店</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2024.03.02 13:00-03.02 20:00</t>
+          <t>2024.03.02 10:00-03.02 17:00</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>208</v>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>380</t>
-        </is>
+        <v>233</v>
+      </c>
+      <c r="G38" t="n">
+        <v>6000</v>
       </c>
       <c r="H38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80924</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80299</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/FpA9OkKy1705467080070.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/V0xu26Cl1703753850690.jpeg</t>
         </is>
       </c>
     </row>
@@ -5368,38 +5192,36 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>上海·次元LAB 二次元电音节</t>
+          <t>上海·小山百代2024上海粉丝见面会</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>逸仙路301号靠纪念路路口 上海宝丰联大酒店</t>
+          <t>宜昌路179号 万代南梦宫上海文化中心</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2024.03.02 10:00-03.02 17:00</t>
+          <t>2024.03.02 13:00-03.02 20:00</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>233</v>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+        <v>208</v>
+      </c>
+      <c r="G39" t="n">
+        <v>38000</v>
       </c>
       <c r="H39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80299</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80924</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/V0xu26Cl1703753850690.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/FpA9OkKy1705467080070.jpeg</t>
         </is>
       </c>
     </row>
@@ -5414,7 +5236,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>上海·第八届次元鹿角动漫游戏展</t>
+          <t>上海·小山百代2024上海粉丝见面会</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -5430,10 +5252,8 @@
       <c r="F40" t="n">
         <v>208</v>
       </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>380</t>
-        </is>
+      <c r="G40" t="n">
+        <v>38000</v>
       </c>
       <c r="H40" t="b">
         <v>1</v>
@@ -5460,7 +5280,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>上海·原神X星穹铁道ONLY</t>
+          <t>上海·怀旧番ONLY</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -5476,10 +5296,8 @@
       <c r="F41" t="n">
         <v>111</v>
       </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="G41" t="n">
+        <v>6000</v>
       </c>
       <c r="H41" t="b">
         <v>0</v>
@@ -5506,7 +5324,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>上海·25时主题同人茶会</t>
+          <t>上海·第五十三届燃梦星辰动漫嘉年华-随机宅舞</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -5522,10 +5340,8 @@
       <c r="F42" t="n">
         <v>37</v>
       </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>58</t>
-        </is>
+      <c r="G42" t="n">
+        <v>5800</v>
       </c>
       <c r="H42" t="b">
         <v>1</v>
@@ -5552,7 +5368,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>上海·新海诚导演作品《铃芽之旅》展 丨 购票抽新海诚见面会门票丨 超限定复刻原画发售</t>
+          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -5568,10 +5384,8 @@
       <c r="F43" t="n">
         <v>853</v>
       </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>73</t>
-        </is>
+      <c r="G43" t="n">
+        <v>7300</v>
       </c>
       <c r="H43" t="b">
         <v>0</v>
@@ -5596,7 +5410,11 @@
           <t>2024-03-16</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr"/>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>上海·三月的幻想演唱会2024「飞越蓝色时刻」</t>
+        </is>
+      </c>
       <c r="D44" t="inlineStr">
         <is>
           <t>宜昌路179号 万代南梦宫上海文化中心</t>
@@ -5610,10 +5428,8 @@
       <c r="F44" t="n">
         <v>35</v>
       </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>380</t>
-        </is>
+      <c r="G44" t="n">
+        <v>38000</v>
       </c>
       <c r="H44" t="b">
         <v>0</v>
@@ -5640,7 +5456,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>上海·三月的幻想演唱会2024「飞越蓝色时刻」</t>
+          <t>上海· TRUE（唐沢美帆）上海动漫交响音乐会</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -5654,12 +5470,10 @@
         </is>
       </c>
       <c r="F45" t="n">
-        <v>110</v>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>480</t>
-        </is>
+        <v>112</v>
+      </c>
+      <c r="G45" t="n">
+        <v>48000</v>
       </c>
       <c r="H45" t="b">
         <v>0</v>
@@ -5686,7 +5500,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>上海·第九届次元鹿角动漫游戏展</t>
+          <t>上海· TRUE（唐沢美帆）上海动漫交响音乐会</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -5700,12 +5514,10 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>110</v>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>480</t>
-        </is>
+        <v>112</v>
+      </c>
+      <c r="G46" t="n">
+        <v>48000</v>
       </c>
       <c r="H46" t="b">
         <v>0</v>
@@ -5732,7 +5544,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>上海·爱乐汇“浪漫经典·一生必听”永恒精选2023烛光音乐会</t>
+          <t>上海·第四届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -5748,10 +5560,8 @@
       <c r="F47" t="n">
         <v>60</v>
       </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="G47" t="n">
+        <v>6000</v>
       </c>
       <c r="H47" t="b">
         <v>0</v>
@@ -5778,7 +5588,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>上海·古影文化《1941·新和医院》大型沉浸式互动剧场</t>
+          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -5794,10 +5604,8 @@
       <c r="F48" t="n">
         <v>10</v>
       </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
+      <c r="G48" t="n">
+        <v>8000</v>
       </c>
       <c r="H48" t="b">
         <v>1</v>
@@ -5824,7 +5632,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>上海·魔都野良神only</t>
+          <t>上海·《四月是你的谎言》——“公生”与“薰”的钢琴小提琴唯美经典音乐集</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -5840,10 +5648,8 @@
       <c r="F49" t="n">
         <v>166</v>
       </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
+      <c r="G49" t="n">
+        <v>8000</v>
       </c>
       <c r="H49" t="b">
         <v>1</v>
@@ -5870,7 +5676,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>上海·第四届次元鹿角动漫游戏展</t>
+          <t>上海·  第五十三届妖漫动漫游戏展</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -5886,10 +5692,8 @@
       <c r="F50" t="n">
         <v>145</v>
       </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
+      <c r="G50" t="n">
+        <v>8000</v>
       </c>
       <c r="H50" t="b">
         <v>0</v>
@@ -5916,7 +5720,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>上海·非人哉官方授权主题店</t>
+          <t>上海·魔都野良神only</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -5932,10 +5736,8 @@
       <c r="F51" t="n">
         <v>173</v>
       </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>79</t>
-        </is>
+      <c r="G51" t="n">
+        <v>7900</v>
       </c>
       <c r="H51" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Update gh-pages to output generated at efdf629
</commit_message>
<xml_diff>
--- a/上海-漫展信息.xlsx
+++ b/上海-漫展信息.xlsx
@@ -513,8 +513,10 @@
       <c r="F2" t="n">
         <v>116</v>
       </c>
-      <c r="G2" t="n">
-        <v>13900</v>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>139</t>
+        </is>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -557,8 +559,10 @@
       <c r="F3" t="n">
         <v>30</v>
       </c>
-      <c r="G3" t="n">
-        <v>8000</v>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -601,8 +605,10 @@
       <c r="F4" t="n">
         <v>1659</v>
       </c>
-      <c r="G4" t="n">
-        <v>5500</v>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -643,10 +649,12 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>545</v>
-      </c>
-      <c r="G5" t="n">
-        <v>4900</v>
+        <v>546</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -689,8 +697,10 @@
       <c r="F6" t="n">
         <v>109</v>
       </c>
-      <c r="G6" t="n">
-        <v>6800</v>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -733,8 +743,10 @@
       <c r="F7" t="n">
         <v>338</v>
       </c>
-      <c r="G7" t="n">
-        <v>4800</v>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
       </c>
       <c r="H7" t="b">
         <v>0</v>
@@ -777,8 +789,10 @@
       <c r="F8" t="n">
         <v>503</v>
       </c>
-      <c r="G8" t="n">
-        <v>7800</v>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -821,8 +835,10 @@
       <c r="F9" t="n">
         <v>239</v>
       </c>
-      <c r="G9" t="n">
-        <v>5900</v>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
       </c>
       <c r="H9" t="b">
         <v>0</v>
@@ -865,8 +881,10 @@
       <c r="F10" t="n">
         <v>1094</v>
       </c>
-      <c r="G10" t="n">
-        <v>6800</v>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
       </c>
       <c r="H10" t="b">
         <v>0</v>
@@ -907,10 +925,12 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>811</v>
-      </c>
-      <c r="G11" t="n">
-        <v>4900</v>
+        <v>812</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
       </c>
       <c r="H11" t="b">
         <v>0</v>
@@ -951,10 +971,12 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>396</v>
-      </c>
-      <c r="G12" t="n">
-        <v>12900</v>
+        <v>397</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>129</t>
+        </is>
       </c>
       <c r="H12" t="b">
         <v>0</v>
@@ -997,8 +1019,10 @@
       <c r="F13" t="n">
         <v>2225</v>
       </c>
-      <c r="G13" t="n">
-        <v>0</v>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>不可售</t>
+        </is>
       </c>
       <c r="H13" t="b">
         <v>0</v>
@@ -1039,10 +1063,12 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>551</v>
-      </c>
-      <c r="G14" t="n">
-        <v>3690</v>
+        <v>553</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
       </c>
       <c r="H14" t="b">
         <v>0</v>
@@ -1085,8 +1111,10 @@
       <c r="F15" t="n">
         <v>30</v>
       </c>
-      <c r="G15" t="n">
-        <v>6000</v>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
       </c>
       <c r="H15" t="b">
         <v>0</v>
@@ -1129,8 +1157,10 @@
       <c r="F16" t="n">
         <v>178</v>
       </c>
-      <c r="G16" t="n">
-        <v>8300</v>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
       </c>
       <c r="H16" t="b">
         <v>0</v>
@@ -1173,8 +1203,10 @@
       <c r="F17" t="n">
         <v>528</v>
       </c>
-      <c r="G17" t="n">
-        <v>6000</v>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
       </c>
       <c r="H17" t="b">
         <v>0</v>
@@ -1217,8 +1249,10 @@
       <c r="F18" t="n">
         <v>12</v>
       </c>
-      <c r="G18" t="n">
-        <v>9900</v>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
       </c>
       <c r="H18" t="b">
         <v>0</v>
@@ -1259,10 +1293,12 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>1257</v>
-      </c>
-      <c r="G19" t="n">
-        <v>9800</v>
+        <v>1258</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
       </c>
       <c r="H19" t="b">
         <v>0</v>
@@ -1305,8 +1341,10 @@
       <c r="F20" t="n">
         <v>66</v>
       </c>
-      <c r="G20" t="n">
-        <v>4900</v>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
       </c>
       <c r="H20" t="b">
         <v>0</v>
@@ -1349,8 +1387,10 @@
       <c r="F21" t="n">
         <v>1175</v>
       </c>
-      <c r="G21" t="n">
-        <v>6590</v>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
       </c>
       <c r="H21" t="b">
         <v>0</v>
@@ -1393,8 +1433,10 @@
       <c r="F22" t="n">
         <v>123</v>
       </c>
-      <c r="G22" t="n">
-        <v>8000</v>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
       </c>
       <c r="H22" t="b">
         <v>0</v>
@@ -1437,8 +1479,10 @@
       <c r="F23" t="n">
         <v>104</v>
       </c>
-      <c r="G23" t="n">
-        <v>4800</v>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
       </c>
       <c r="H23" t="b">
         <v>0</v>
@@ -1481,8 +1525,10 @@
       <c r="F24" t="n">
         <v>2444</v>
       </c>
-      <c r="G24" t="n">
-        <v>6580</v>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
       </c>
       <c r="H24" t="b">
         <v>1</v>
@@ -1525,8 +1571,10 @@
       <c r="F25" t="n">
         <v>233</v>
       </c>
-      <c r="G25" t="n">
-        <v>6000</v>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
       </c>
       <c r="H25" t="b">
         <v>0</v>
@@ -1569,8 +1617,10 @@
       <c r="F26" t="n">
         <v>111</v>
       </c>
-      <c r="G26" t="n">
-        <v>6000</v>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
       </c>
       <c r="H26" t="b">
         <v>0</v>
@@ -1613,8 +1663,10 @@
       <c r="F27" t="n">
         <v>37</v>
       </c>
-      <c r="G27" t="n">
-        <v>5800</v>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
       </c>
       <c r="H27" t="b">
         <v>1</v>
@@ -1657,8 +1709,10 @@
       <c r="F28" t="n">
         <v>853</v>
       </c>
-      <c r="G28" t="n">
-        <v>7300</v>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
       </c>
       <c r="H28" t="b">
         <v>0</v>
@@ -1701,8 +1755,10 @@
       <c r="F29" t="n">
         <v>6</v>
       </c>
-      <c r="G29" t="n">
-        <v>4000</v>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
       </c>
       <c r="H29" t="b">
         <v>0</v>
@@ -1745,8 +1801,10 @@
       <c r="F30" t="n">
         <v>60</v>
       </c>
-      <c r="G30" t="n">
-        <v>6000</v>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
       </c>
       <c r="H30" t="b">
         <v>0</v>
@@ -1789,8 +1847,10 @@
       <c r="F31" t="n">
         <v>145</v>
       </c>
-      <c r="G31" t="n">
-        <v>8000</v>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
       </c>
       <c r="H31" t="b">
         <v>0</v>
@@ -1833,8 +1893,10 @@
       <c r="F32" t="n">
         <v>173</v>
       </c>
-      <c r="G32" t="n">
-        <v>7900</v>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
       </c>
       <c r="H32" t="b">
         <v>0</v>
@@ -1877,8 +1939,10 @@
       <c r="F33" t="n">
         <v>6</v>
       </c>
-      <c r="G33" t="n">
-        <v>8900</v>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
       </c>
       <c r="H33" t="b">
         <v>0</v>
@@ -1990,8 +2054,10 @@
       <c r="F2" t="n">
         <v>21</v>
       </c>
-      <c r="G2" t="n">
-        <v>9000</v>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -2034,8 +2100,10 @@
       <c r="F3" t="n">
         <v>39</v>
       </c>
-      <c r="G3" t="n">
-        <v>9000</v>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -2078,8 +2146,10 @@
       <c r="F4" t="n">
         <v>50</v>
       </c>
-      <c r="G4" t="n">
-        <v>0</v>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>已停售</t>
+        </is>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -2122,8 +2192,10 @@
       <c r="F5" t="n">
         <v>18</v>
       </c>
-      <c r="G5" t="n">
-        <v>0</v>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>已停售</t>
+        </is>
       </c>
       <c r="H5" t="b">
         <v>1</v>
@@ -2166,8 +2238,10 @@
       <c r="F6" t="n">
         <v>88</v>
       </c>
-      <c r="G6" t="n">
-        <v>38000</v>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>380</t>
+        </is>
       </c>
       <c r="H6" t="b">
         <v>1</v>
@@ -2210,8 +2284,10 @@
       <c r="F7" t="n">
         <v>159</v>
       </c>
-      <c r="G7" t="n">
-        <v>8000</v>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
       </c>
       <c r="H7" t="b">
         <v>1</v>
@@ -2254,8 +2330,10 @@
       <c r="F8" t="n">
         <v>50</v>
       </c>
-      <c r="G8" t="n">
-        <v>8800</v>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -2298,8 +2376,10 @@
       <c r="F9" t="n">
         <v>29</v>
       </c>
-      <c r="G9" t="n">
-        <v>12000</v>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
       </c>
       <c r="H9" t="b">
         <v>1</v>
@@ -2342,8 +2422,10 @@
       <c r="F10" t="n">
         <v>294</v>
       </c>
-      <c r="G10" t="n">
-        <v>27800</v>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>278</t>
+        </is>
       </c>
       <c r="H10" t="b">
         <v>1</v>
@@ -2384,10 +2466,12 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>605</v>
-      </c>
-      <c r="G11" t="n">
-        <v>38000</v>
+        <v>606</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>380</t>
+        </is>
       </c>
       <c r="H11" t="b">
         <v>1</v>
@@ -2428,10 +2512,12 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>293</v>
-      </c>
-      <c r="G12" t="n">
-        <v>48000</v>
+        <v>294</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>480</t>
+        </is>
       </c>
       <c r="H12" t="b">
         <v>0</v>
@@ -2474,8 +2560,10 @@
       <c r="F13" t="n">
         <v>2</v>
       </c>
-      <c r="G13" t="n">
-        <v>0</v>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>已停售</t>
+        </is>
       </c>
       <c r="H13" t="b">
         <v>0</v>
@@ -2518,8 +2606,10 @@
       <c r="F14" t="n">
         <v>4</v>
       </c>
-      <c r="G14" t="n">
-        <v>15800</v>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>158</t>
+        </is>
       </c>
       <c r="H14" t="b">
         <v>0</v>
@@ -2562,8 +2652,10 @@
       <c r="F15" t="n">
         <v>194</v>
       </c>
-      <c r="G15" t="n">
-        <v>38000</v>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>380</t>
+        </is>
       </c>
       <c r="H15" t="b">
         <v>0</v>
@@ -2606,8 +2698,10 @@
       <c r="F16" t="n">
         <v>3</v>
       </c>
-      <c r="G16" t="n">
-        <v>58000</v>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>580</t>
+        </is>
       </c>
       <c r="H16" t="b">
         <v>1</v>
@@ -2650,8 +2744,10 @@
       <c r="F17" t="n">
         <v>208</v>
       </c>
-      <c r="G17" t="n">
-        <v>38000</v>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>380</t>
+        </is>
       </c>
       <c r="H17" t="b">
         <v>1</v>
@@ -2694,8 +2790,10 @@
       <c r="F18" t="n">
         <v>35</v>
       </c>
-      <c r="G18" t="n">
-        <v>38000</v>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>380</t>
+        </is>
       </c>
       <c r="H18" t="b">
         <v>0</v>
@@ -2738,8 +2836,10 @@
       <c r="F19" t="n">
         <v>1</v>
       </c>
-      <c r="G19" t="n">
-        <v>8000</v>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
       </c>
       <c r="H19" t="b">
         <v>0</v>
@@ -2782,8 +2882,10 @@
       <c r="F20" t="n">
         <v>196</v>
       </c>
-      <c r="G20" t="n">
-        <v>48000</v>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>480</t>
+        </is>
       </c>
       <c r="H20" t="b">
         <v>0</v>
@@ -2826,8 +2928,10 @@
       <c r="F21" t="n">
         <v>1</v>
       </c>
-      <c r="G21" t="n">
-        <v>8000</v>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
       </c>
       <c r="H21" t="b">
         <v>0</v>
@@ -2870,8 +2974,10 @@
       <c r="F22" t="n">
         <v>112</v>
       </c>
-      <c r="G22" t="n">
-        <v>48000</v>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>480</t>
+        </is>
       </c>
       <c r="H22" t="b">
         <v>0</v>
@@ -2914,8 +3020,10 @@
       <c r="F23" t="n">
         <v>10</v>
       </c>
-      <c r="G23" t="n">
-        <v>8000</v>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
       </c>
       <c r="H23" t="b">
         <v>1</v>
@@ -2958,8 +3066,10 @@
       <c r="F24" t="n">
         <v>166</v>
       </c>
-      <c r="G24" t="n">
-        <v>8000</v>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
       </c>
       <c r="H24" t="b">
         <v>1</v>
@@ -3002,8 +3112,10 @@
       <c r="F25" t="n">
         <v>3</v>
       </c>
-      <c r="G25" t="n">
-        <v>8000</v>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
       </c>
       <c r="H25" t="b">
         <v>0</v>
@@ -3046,8 +3158,10 @@
       <c r="F26" t="n">
         <v>6</v>
       </c>
-      <c r="G26" t="n">
-        <v>28000</v>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>280</t>
+        </is>
       </c>
       <c r="H26" t="b">
         <v>0</v>
@@ -3159,8 +3273,10 @@
       <c r="F2" t="n">
         <v>1715</v>
       </c>
-      <c r="G2" t="n">
-        <v>6000</v>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -3203,8 +3319,10 @@
       <c r="F3" t="n">
         <v>68</v>
       </c>
-      <c r="G3" t="n">
-        <v>99600</v>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>996</t>
+        </is>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -3247,8 +3365,10 @@
       <c r="F4" t="n">
         <v>35</v>
       </c>
-      <c r="G4" t="n">
-        <v>4990</v>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -3291,8 +3411,10 @@
       <c r="F5" t="n">
         <v>1955</v>
       </c>
-      <c r="G5" t="n">
-        <v>3000</v>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -3335,8 +3457,10 @@
       <c r="F6" t="n">
         <v>2040</v>
       </c>
-      <c r="G6" t="n">
-        <v>3000</v>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -3379,8 +3503,10 @@
       <c r="F7" t="n">
         <v>669</v>
       </c>
-      <c r="G7" t="n">
-        <v>3000</v>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
       </c>
       <c r="H7" t="b">
         <v>0</v>
@@ -3421,10 +3547,12 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>794</v>
-      </c>
-      <c r="G8" t="n">
-        <v>3000</v>
+        <v>795</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -3467,8 +3595,10 @@
       <c r="F9" t="n">
         <v>676</v>
       </c>
-      <c r="G9" t="n">
-        <v>1000</v>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="H9" t="b">
         <v>0</v>
@@ -3580,8 +3710,10 @@
       <c r="F2" t="n">
         <v>1715</v>
       </c>
-      <c r="G2" t="n">
-        <v>6000</v>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -3624,8 +3756,10 @@
       <c r="F3" t="n">
         <v>68</v>
       </c>
-      <c r="G3" t="n">
-        <v>99600</v>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>996</t>
+        </is>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -3668,8 +3802,10 @@
       <c r="F4" t="n">
         <v>35</v>
       </c>
-      <c r="G4" t="n">
-        <v>4990</v>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -3712,8 +3848,10 @@
       <c r="F5" t="n">
         <v>116</v>
       </c>
-      <c r="G5" t="n">
-        <v>13900</v>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>139</t>
+        </is>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -3756,8 +3894,10 @@
       <c r="F6" t="n">
         <v>1955</v>
       </c>
-      <c r="G6" t="n">
-        <v>3000</v>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -3800,8 +3940,10 @@
       <c r="F7" t="n">
         <v>2040</v>
       </c>
-      <c r="G7" t="n">
-        <v>3000</v>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
       </c>
       <c r="H7" t="b">
         <v>0</v>
@@ -3844,8 +3986,10 @@
       <c r="F8" t="n">
         <v>669</v>
       </c>
-      <c r="G8" t="n">
-        <v>3000</v>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -3888,8 +4032,10 @@
       <c r="F9" t="n">
         <v>30</v>
       </c>
-      <c r="G9" t="n">
-        <v>8000</v>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
       </c>
       <c r="H9" t="b">
         <v>0</v>
@@ -3932,8 +4078,10 @@
       <c r="F10" t="n">
         <v>1659</v>
       </c>
-      <c r="G10" t="n">
-        <v>5500</v>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="H10" t="b">
         <v>0</v>
@@ -3976,8 +4124,10 @@
       <c r="F11" t="n">
         <v>21</v>
       </c>
-      <c r="G11" t="n">
-        <v>9000</v>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
       </c>
       <c r="H11" t="b">
         <v>0</v>
@@ -4020,8 +4170,10 @@
       <c r="F12" t="n">
         <v>39</v>
       </c>
-      <c r="G12" t="n">
-        <v>9000</v>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
       </c>
       <c r="H12" t="b">
         <v>0</v>
@@ -4062,10 +4214,12 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>794</v>
-      </c>
-      <c r="G13" t="n">
-        <v>3000</v>
+        <v>795</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
       </c>
       <c r="H13" t="b">
         <v>0</v>
@@ -4108,8 +4262,10 @@
       <c r="F14" t="n">
         <v>676</v>
       </c>
-      <c r="G14" t="n">
-        <v>1000</v>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="H14" t="b">
         <v>0</v>
@@ -4150,10 +4306,12 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>545</v>
-      </c>
-      <c r="G15" t="n">
-        <v>4900</v>
+        <v>546</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
       </c>
       <c r="H15" t="b">
         <v>0</v>
@@ -4196,8 +4354,10 @@
       <c r="F16" t="n">
         <v>88</v>
       </c>
-      <c r="G16" t="n">
-        <v>38000</v>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>380</t>
+        </is>
       </c>
       <c r="H16" t="b">
         <v>1</v>
@@ -4240,8 +4400,10 @@
       <c r="F17" t="n">
         <v>159</v>
       </c>
-      <c r="G17" t="n">
-        <v>8000</v>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
       </c>
       <c r="H17" t="b">
         <v>1</v>
@@ -4284,8 +4446,10 @@
       <c r="F18" t="n">
         <v>109</v>
       </c>
-      <c r="G18" t="n">
-        <v>6800</v>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
       </c>
       <c r="H18" t="b">
         <v>0</v>
@@ -4328,8 +4492,10 @@
       <c r="F19" t="n">
         <v>50</v>
       </c>
-      <c r="G19" t="n">
-        <v>8800</v>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
       </c>
       <c r="H19" t="b">
         <v>0</v>
@@ -4372,8 +4538,10 @@
       <c r="F20" t="n">
         <v>338</v>
       </c>
-      <c r="G20" t="n">
-        <v>4800</v>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
       </c>
       <c r="H20" t="b">
         <v>0</v>
@@ -4416,8 +4584,10 @@
       <c r="F21" t="n">
         <v>503</v>
       </c>
-      <c r="G21" t="n">
-        <v>7800</v>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
       </c>
       <c r="H21" t="b">
         <v>0</v>
@@ -4460,8 +4630,10 @@
       <c r="F22" t="n">
         <v>239</v>
       </c>
-      <c r="G22" t="n">
-        <v>5900</v>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
       </c>
       <c r="H22" t="b">
         <v>0</v>
@@ -4504,8 +4676,10 @@
       <c r="F23" t="n">
         <v>29</v>
       </c>
-      <c r="G23" t="n">
-        <v>12000</v>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
       </c>
       <c r="H23" t="b">
         <v>1</v>
@@ -4548,8 +4722,10 @@
       <c r="F24" t="n">
         <v>1094</v>
       </c>
-      <c r="G24" t="n">
-        <v>6800</v>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
       </c>
       <c r="H24" t="b">
         <v>0</v>
@@ -4590,10 +4766,12 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>811</v>
-      </c>
-      <c r="G25" t="n">
-        <v>4900</v>
+        <v>812</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
       </c>
       <c r="H25" t="b">
         <v>0</v>
@@ -4636,8 +4814,10 @@
       <c r="F26" t="n">
         <v>294</v>
       </c>
-      <c r="G26" t="n">
-        <v>27800</v>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>278</t>
+        </is>
       </c>
       <c r="H26" t="b">
         <v>1</v>
@@ -4678,10 +4858,12 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>396</v>
-      </c>
-      <c r="G27" t="n">
-        <v>12900</v>
+        <v>397</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>129</t>
+        </is>
       </c>
       <c r="H27" t="b">
         <v>0</v>
@@ -4724,8 +4906,10 @@
       <c r="F28" t="n">
         <v>178</v>
       </c>
-      <c r="G28" t="n">
-        <v>8300</v>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
       </c>
       <c r="H28" t="b">
         <v>0</v>
@@ -4766,10 +4950,12 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>605</v>
-      </c>
-      <c r="G29" t="n">
-        <v>38000</v>
+        <v>606</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>380</t>
+        </is>
       </c>
       <c r="H29" t="b">
         <v>1</v>
@@ -4812,8 +4998,10 @@
       <c r="F30" t="n">
         <v>528</v>
       </c>
-      <c r="G30" t="n">
-        <v>6000</v>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
       </c>
       <c r="H30" t="b">
         <v>0</v>
@@ -4854,10 +5042,12 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>1257</v>
-      </c>
-      <c r="G31" t="n">
-        <v>9800</v>
+        <v>1258</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
       </c>
       <c r="H31" t="b">
         <v>0</v>
@@ -4898,10 +5088,12 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>293</v>
-      </c>
-      <c r="G32" t="n">
-        <v>48000</v>
+        <v>294</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>480</t>
+        </is>
       </c>
       <c r="H32" t="b">
         <v>0</v>
@@ -4944,8 +5136,10 @@
       <c r="F33" t="n">
         <v>66</v>
       </c>
-      <c r="G33" t="n">
-        <v>4900</v>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
       </c>
       <c r="H33" t="b">
         <v>0</v>
@@ -4988,8 +5182,10 @@
       <c r="F34" t="n">
         <v>1175</v>
       </c>
-      <c r="G34" t="n">
-        <v>6590</v>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
       </c>
       <c r="H34" t="b">
         <v>0</v>
@@ -5032,8 +5228,10 @@
       <c r="F35" t="n">
         <v>104</v>
       </c>
-      <c r="G35" t="n">
-        <v>4800</v>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
       </c>
       <c r="H35" t="b">
         <v>0</v>
@@ -5076,8 +5274,10 @@
       <c r="F36" t="n">
         <v>2444</v>
       </c>
-      <c r="G36" t="n">
-        <v>6580</v>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
       </c>
       <c r="H36" t="b">
         <v>1</v>
@@ -5120,8 +5320,10 @@
       <c r="F37" t="n">
         <v>194</v>
       </c>
-      <c r="G37" t="n">
-        <v>38000</v>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>380</t>
+        </is>
       </c>
       <c r="H37" t="b">
         <v>0</v>
@@ -5164,8 +5366,10 @@
       <c r="F38" t="n">
         <v>233</v>
       </c>
-      <c r="G38" t="n">
-        <v>6000</v>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
       </c>
       <c r="H38" t="b">
         <v>0</v>
@@ -5208,8 +5412,10 @@
       <c r="F39" t="n">
         <v>208</v>
       </c>
-      <c r="G39" t="n">
-        <v>38000</v>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>380</t>
+        </is>
       </c>
       <c r="H39" t="b">
         <v>1</v>
@@ -5252,8 +5458,10 @@
       <c r="F40" t="n">
         <v>208</v>
       </c>
-      <c r="G40" t="n">
-        <v>38000</v>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>380</t>
+        </is>
       </c>
       <c r="H40" t="b">
         <v>1</v>
@@ -5296,8 +5504,10 @@
       <c r="F41" t="n">
         <v>111</v>
       </c>
-      <c r="G41" t="n">
-        <v>6000</v>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
       </c>
       <c r="H41" t="b">
         <v>0</v>
@@ -5340,8 +5550,10 @@
       <c r="F42" t="n">
         <v>37</v>
       </c>
-      <c r="G42" t="n">
-        <v>5800</v>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
       </c>
       <c r="H42" t="b">
         <v>1</v>
@@ -5384,8 +5596,10 @@
       <c r="F43" t="n">
         <v>853</v>
       </c>
-      <c r="G43" t="n">
-        <v>7300</v>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
       </c>
       <c r="H43" t="b">
         <v>0</v>
@@ -5428,8 +5642,10 @@
       <c r="F44" t="n">
         <v>35</v>
       </c>
-      <c r="G44" t="n">
-        <v>38000</v>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>380</t>
+        </is>
       </c>
       <c r="H44" t="b">
         <v>0</v>
@@ -5472,8 +5688,10 @@
       <c r="F45" t="n">
         <v>112</v>
       </c>
-      <c r="G45" t="n">
-        <v>48000</v>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>480</t>
+        </is>
       </c>
       <c r="H45" t="b">
         <v>0</v>
@@ -5516,8 +5734,10 @@
       <c r="F46" t="n">
         <v>112</v>
       </c>
-      <c r="G46" t="n">
-        <v>48000</v>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>480</t>
+        </is>
       </c>
       <c r="H46" t="b">
         <v>0</v>
@@ -5560,8 +5780,10 @@
       <c r="F47" t="n">
         <v>60</v>
       </c>
-      <c r="G47" t="n">
-        <v>6000</v>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
       </c>
       <c r="H47" t="b">
         <v>0</v>
@@ -5604,8 +5826,10 @@
       <c r="F48" t="n">
         <v>10</v>
       </c>
-      <c r="G48" t="n">
-        <v>8000</v>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
       </c>
       <c r="H48" t="b">
         <v>1</v>
@@ -5648,8 +5872,10 @@
       <c r="F49" t="n">
         <v>166</v>
       </c>
-      <c r="G49" t="n">
-        <v>8000</v>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
       </c>
       <c r="H49" t="b">
         <v>1</v>
@@ -5692,8 +5918,10 @@
       <c r="F50" t="n">
         <v>145</v>
       </c>
-      <c r="G50" t="n">
-        <v>8000</v>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
       </c>
       <c r="H50" t="b">
         <v>0</v>
@@ -5736,8 +5964,10 @@
       <c r="F51" t="n">
         <v>173</v>
       </c>
-      <c r="G51" t="n">
-        <v>7900</v>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
       </c>
       <c r="H51" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Update gh-pages to output generated at a3196b5
</commit_message>
<xml_diff>
--- a/上海-漫展信息.xlsx
+++ b/上海-漫展信息.xlsx
@@ -603,7 +603,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -649,7 +649,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>546</v>
+        <v>557</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -695,7 +695,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -741,7 +741,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -787,7 +787,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -833,7 +833,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -879,7 +879,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>1094</v>
+        <v>1100</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -925,7 +925,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>812</v>
+        <v>823</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -971,7 +971,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1063,7 +1063,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>553</v>
+        <v>559</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1201,7 +1201,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1247,7 +1247,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1293,7 +1293,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1385,7 +1385,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>1175</v>
+        <v>1179</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1431,7 +1431,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1477,7 +1477,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1523,7 +1523,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>2444</v>
+        <v>2446</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1569,7 +1569,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1615,7 +1615,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1891,7 +1891,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -2466,7 +2466,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -2512,7 +2512,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -2696,7 +2696,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -2742,7 +2742,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -2880,7 +2880,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -2972,7 +2972,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -3064,7 +3064,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -3156,7 +3156,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -3271,7 +3271,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1715</v>
+        <v>1717</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -3409,7 +3409,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1955</v>
+        <v>1959</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -3455,7 +3455,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>2040</v>
+        <v>2045</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -3547,7 +3547,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -3708,7 +3708,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1715</v>
+        <v>1717</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -3800,7 +3800,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -3892,7 +3892,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1955</v>
+        <v>1959</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -3938,7 +3938,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>2040</v>
+        <v>2045</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -4076,7 +4076,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -4214,7 +4214,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -4306,7 +4306,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>546</v>
+        <v>557</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -4444,7 +4444,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -4490,7 +4490,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -4536,7 +4536,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -4582,7 +4582,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -4628,7 +4628,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -4720,7 +4720,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>1094</v>
+        <v>1100</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -4766,7 +4766,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>812</v>
+        <v>823</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -4858,7 +4858,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -4950,7 +4950,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -4996,7 +4996,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -5042,7 +5042,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -5088,7 +5088,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -5180,7 +5180,7 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>1175</v>
+        <v>1179</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -5207,30 +5207,30 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2024-02-24</t>
+          <t>2024-02-17</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>上海·SISP动漫游戏嘉年华</t>
+          <t>上海·少女番only2.0</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>年家浜路518号 周浦万达广场</t>
+          <t>营口路699号(黄兴公园地铁站2号口旁) 花嫁丽舍</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2024.02.24 13:00-02.25 19:00</t>
+          <t>2024.02.17 10:00-02.17 17:00</t>
         </is>
       </c>
       <c r="F35" t="n">
-        <v>104</v>
+        <v>135</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>80</t>
         </is>
       </c>
       <c r="H35" t="b">
@@ -5238,12 +5238,12 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80339</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81148</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/a8iuOufB1703832570508.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/j6eEZ18S1705657346664.jpeg</t>
         </is>
       </c>
     </row>
@@ -5258,38 +5258,38 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>上海·第三届燃梦BACG PRO游戏动漫展-原X铁X崩同好交流</t>
+          <t>上海·SISP动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
+          <t>年家浜路518号 周浦万达广场</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2024.02.24 11:00-02.25 16:30</t>
+          <t>2024.02.24 13:00-02.25 19:00</t>
         </is>
       </c>
       <c r="F36" t="n">
-        <v>2444</v>
+        <v>105</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>48</t>
         </is>
       </c>
       <c r="H36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77754</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80339</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202312/7eGZETK91701943985671.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/a8iuOufB1703832570508.jpeg</t>
         </is>
       </c>
     </row>
@@ -5299,43 +5299,43 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2024-02-25</t>
+          <t>2024-02-24</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>上海·青山吉能见面会</t>
+          <t>上海·第三届燃梦BACG PRO游戏动漫展-原X铁X崩同好交流</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>虹许路731号4号楼 THE BOXX•城市乐园</t>
+          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2024.02.25 14:30-02.25 19:30</t>
+          <t>2024.02.24 11:00-02.25 16:30</t>
         </is>
       </c>
       <c r="F37" t="n">
-        <v>194</v>
+        <v>2446</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>65</t>
         </is>
       </c>
       <c r="H37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80142</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=77754</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/1npuHFBM1703231674558.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/7eGZETK91701943985671.jpeg</t>
         </is>
       </c>
     </row>
@@ -5345,30 +5345,30 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2024-03-02</t>
+          <t>2024-02-25</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>上海·原神X星穹铁道ONLY</t>
+          <t>上海·青山吉能见面会</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>逸仙路301号靠纪念路路口 上海宝丰联大酒店</t>
+          <t>虹许路731号4号楼 THE BOXX•城市乐园</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2024.03.02 10:00-03.02 17:00</t>
+          <t>2024.02.25 14:30-02.25 19:30</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>233</v>
+        <v>194</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>380</t>
         </is>
       </c>
       <c r="H38" t="b">
@@ -5376,12 +5376,12 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80299</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80142</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/V0xu26Cl1703753850690.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/1npuHFBM1703231674558.jpeg</t>
         </is>
       </c>
     </row>
@@ -5396,38 +5396,38 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>上海·小山百代2024上海粉丝见面会</t>
+          <t>上海·原神X星穹铁道ONLY</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>宜昌路179号 万代南梦宫上海文化中心</t>
+          <t>逸仙路301号靠纪念路路口 上海宝丰联大酒店</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2024.03.02 13:00-03.02 20:00</t>
+          <t>2024.03.02 10:00-03.02 17:00</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>208</v>
+        <v>235</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>60</t>
         </is>
       </c>
       <c r="H39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80924</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80299</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/FpA9OkKy1705467080070.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/V0xu26Cl1703753850690.jpeg</t>
         </is>
       </c>
     </row>
@@ -5456,7 +5456,7 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -5483,43 +5483,43 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2024-03-03</t>
+          <t>2024-03-02</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>上海·怀旧番ONLY</t>
+          <t>上海·小山百代2024上海粉丝见面会</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>逸仙路270号  上海宝丰联大酒店</t>
+          <t>宜昌路179号 万代南梦宫上海文化中心</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2024.03.03 10:00-03.03 17:00</t>
+          <t>2024.03.02 13:00-03.02 20:00</t>
         </is>
       </c>
       <c r="F41" t="n">
-        <v>111</v>
+        <v>210</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>380</t>
         </is>
       </c>
       <c r="H41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80575</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80924</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/y4uWdyPT1704700763902.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/FpA9OkKy1705467080070.jpeg</t>
         </is>
       </c>
     </row>
@@ -5529,43 +5529,43 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2024-03-09</t>
+          <t>2024-03-03</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>上海·第五十三届燃梦星辰动漫嘉年华-随机宅舞</t>
+          <t>上海·怀旧番ONLY</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>周家嘴路3608号 宝龙旭辉广场</t>
+          <t>逸仙路270号  上海宝丰联大酒店</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2024.03.09 10:20-03.10 16:30</t>
+          <t>2024.03.03 10:00-03.03 17:00</t>
         </is>
       </c>
       <c r="F42" t="n">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>60</t>
         </is>
       </c>
       <c r="H42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80571</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80575</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/SHH70VXN1704700240858.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/y4uWdyPT1704700763902.jpeg</t>
         </is>
       </c>
     </row>
@@ -5580,38 +5580,38 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
+          <t>上海·第五十三届燃梦星辰动漫嘉年华-随机宅舞</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>漕宝路1688号 诺宝中心酒店</t>
+          <t>周家嘴路3608号 宝龙旭辉广场</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2024.03.09 10:00-03.09 16:30</t>
+          <t>2024.03.09 10:20-03.10 16:30</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>853</v>
+        <v>37</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>58</t>
         </is>
       </c>
       <c r="H43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=76410</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80571</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202309/fVXMrcHy1693971682397.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/SHH70VXN1704700240858.jpeg</t>
         </is>
       </c>
     </row>
@@ -5621,30 +5621,30 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2024-03-16</t>
+          <t>2024-03-09</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>上海·三月的幻想演唱会2024「飞越蓝色时刻」</t>
+          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>宜昌路179号 万代南梦宫上海文化中心</t>
+          <t>漕宝路1688号 诺宝中心酒店</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2024.03.16 19:00-03.16 20:30</t>
+          <t>2024.03.09 10:00-03.09 16:30</t>
         </is>
       </c>
       <c r="F44" t="n">
-        <v>35</v>
+        <v>853</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>73</t>
         </is>
       </c>
       <c r="H44" t="b">
@@ -5652,12 +5652,12 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80811</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=76410</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/TO6xpSqr1705289483473.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202309/fVXMrcHy1693971682397.jpeg</t>
         </is>
       </c>
     </row>
@@ -5686,7 +5686,7 @@
         </is>
       </c>
       <c r="F45" t="n">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -5732,7 +5732,7 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -5870,7 +5870,7 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -5962,7 +5962,7 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update gh-pages to output generated at 34df19c
</commit_message>
<xml_diff>
--- a/上海-漫展信息.xlsx
+++ b/上海-漫展信息.xlsx
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -649,7 +649,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -695,7 +695,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -741,7 +741,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>536</v>
+        <v>543</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -787,7 +787,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -833,7 +833,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>1167</v>
+        <v>1172</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -879,7 +879,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>923</v>
+        <v>931</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -925,7 +925,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -971,7 +971,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>2223</v>
+        <v>2224</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1017,7 +1017,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>642</v>
+        <v>648</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1063,7 +1063,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1109,7 +1109,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1155,7 +1155,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>660</v>
+        <v>672</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1201,7 +1201,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1247,7 +1247,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1293,7 +1293,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>1296</v>
+        <v>1300</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1339,7 +1339,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1385,7 +1385,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1431,7 +1431,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1477,7 +1477,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>1207</v>
+        <v>1212</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1523,7 +1523,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1569,7 +1569,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1615,7 +1615,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>2475</v>
+        <v>2486</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1661,7 +1661,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1707,7 +1707,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1753,7 +1753,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1799,7 +1799,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1845,7 +1845,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1891,7 +1891,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>872</v>
+        <v>875</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -2029,7 +2029,7 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -2121,7 +2121,7 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -2199,7 +2199,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2401,30 +2401,30 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024-01-23</t>
+          <t>2024-01-26</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>上海·七音阿卡莉 NANAOAKARI 2024 专场演出</t>
+          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>嘉兴路街道瑞虹路188号瑞虹天地月亮湾3层 Modern Sky LAB摩登天空(瑞虹天地店)</t>
+          <t>丁香路425号 上海东方艺术中心</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2024.01.23 20:00-01.23 22:00</t>
+          <t>2024.01.26 19:30-01.26 21:30</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>91</v>
+        <v>163</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>已停售</t>
+          <t>80</t>
         </is>
       </c>
       <c r="H5" t="b">
@@ -2432,12 +2432,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79641</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78418</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/CoNbgCpO1703644783043.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202311/GHpvkT5Y1699605760230.jpeg</t>
         </is>
       </c>
     </row>
@@ -2447,43 +2447,43 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2024-01-26</t>
+          <t>2024-01-27</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
+          <t>上海·Azurock」Azurose ACG Cover Live</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>丁香路425号 上海东方艺术中心</t>
+          <t>愚园路1398号 育音堂音乐公园</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2024.01.26 19:30-01.26 21:30</t>
+          <t>2024.01.27 19:00-01.27 21:30</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>163</v>
+        <v>60</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>88</t>
         </is>
       </c>
       <c r="H6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78418</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80277</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202311/GHpvkT5Y1699605760230.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/5d6O1Rf11703742965244.png</t>
         </is>
       </c>
     </row>
@@ -2498,38 +2498,38 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>上海·Azurock」Azurose ACG Cover Live</t>
+          <t>上海·日本原版《数码宝贝舞台剧：游乐园之谜》</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>愚园路1398号 育音堂音乐公园</t>
+          <t>茂名南路57号近长乐路 上海兰心大戏院</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2024.01.27 19:00-01.27 21:30</t>
+          <t>2024.01.27 15:30-01.27 20:55</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>120</t>
         </is>
       </c>
       <c r="H7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80277</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79783</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202312/5d6O1Rf11703742965244.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/S6nZ327b1702534484951.jpeg</t>
         </is>
       </c>
     </row>
@@ -2544,25 +2544,25 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>上海·日本原版《数码宝贝舞台剧：游乐园之谜》</t>
+          <t>上海•Risa Yuzuki 1st ONEMAN LIVE 「Future Interlink」 追加公演</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>茂名南路57号近长乐路 上海兰心大戏院</t>
+          <t>愚园路1250号 新歌空间</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2024.01.27 15:30-01.27 20:55</t>
+          <t>2024.01.27 18:30-01.27 21:00</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>31</v>
+        <v>298</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>278</t>
         </is>
       </c>
       <c r="H8" t="b">
@@ -2570,12 +2570,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79783</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=77773</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/S6nZ327b1702534484951.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202310/XKKYWAk51698315607196.png</t>
         </is>
       </c>
     </row>
@@ -2585,30 +2585,30 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2024-01-27</t>
+          <t>2024-02-02</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>上海•Risa Yuzuki 1st ONEMAN LIVE 「Future Interlink」 追加公演</t>
+          <t>上海·次元LAB 二次元电音节</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>愚园路1250号 新歌空间</t>
+          <t>中兴路1683号金融街购物中心L3-27 蜚声上海Livehouse</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2024.01.27 18:30-01.27 21:00</t>
+          <t>2024.02.02 12:30-02.02 21:00</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>298</v>
+        <v>631</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>278</t>
+          <t>380</t>
         </is>
       </c>
       <c r="H9" t="b">
@@ -2616,12 +2616,12 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77773</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80128</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202310/XKKYWAk51698315607196.png</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/DEW1XYty1703226993965.jpeg</t>
         </is>
       </c>
     </row>
@@ -2631,43 +2631,43 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2024-02-02</t>
+          <t>2024-02-04</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>上海·次元LAB 二次元电音节</t>
+          <t>上海·触手猴钢琴巡演·marasy piano live tour『生音』上海站·Powered by 东方弹幕神乐失落幻想</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>中兴路1683号金融街购物中心L3-27 蜚声上海Livehouse</t>
+          <t>丁香路425号(上海科技馆地铁站1号口步行460米) 上海东方艺术中心音乐厅</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2024.02.02 12:30-02.02 21:00</t>
+          <t>2024.02.04 19:30-02.04 21:00</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>624</v>
+        <v>339</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>280</t>
         </is>
       </c>
       <c r="H10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80128</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80734</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202312/DEW1XYty1703226993965.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/IcjPp0TE1704951328918.jpeg</t>
         </is>
       </c>
     </row>
@@ -2677,30 +2677,30 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2024-02-04</t>
+          <t>2024-02-14</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>上海·触手猴钢琴巡演·marasy piano live tour『生音』上海站·Powered by 东方弹幕神乐失落幻想</t>
+          <t>上海·【情人节特辑】《那年我们》记忆重启韩剧经典OST音乐会《请回答1988》《来自星星的你》</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>丁香路425号(上海科技馆地铁站1号口步行460米) 上海东方艺术中心音乐厅</t>
+          <t>牛庄路704号 中国大戏院</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2024.02.04 19:30-02.04 21:00</t>
+          <t>2024.02.14 19:30-02.14 21:00</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>334</v>
+        <v>2</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>280</t>
+          <t>已停售</t>
         </is>
       </c>
       <c r="H11" t="b">
@@ -2708,12 +2708,12 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80734</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80615</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/IcjPp0TE1704951328918.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/5DDVhKcO1704767761361.png</t>
         </is>
       </c>
     </row>
@@ -2723,30 +2723,30 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2024-02-14</t>
+          <t>2024-02-24</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>上海·【情人节特辑】《那年我们》记忆重启韩剧经典OST音乐会《请回答1988》《来自星星的你》</t>
+          <t>上海·《哈利的魔法世界》动漫视听音乐会</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>牛庄路704号 中国大戏院</t>
+          <t>都市路4889号（莘庄地铁站南广场） 上海保利城市剧院</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2024.02.14 19:30-02.14 21:00</t>
+          <t>2024.02.24 14:30-02.24 16:00</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>已停售</t>
+          <t>158</t>
         </is>
       </c>
       <c r="H12" t="b">
@@ -2754,12 +2754,12 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80615</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80639</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/5DDVhKcO1704767761361.png</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/dp013A4p1704783993628.png</t>
         </is>
       </c>
     </row>
@@ -2769,30 +2769,30 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2024-02-24</t>
+          <t>2024-02-25</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>上海·《哈利的魔法世界》动漫视听音乐会</t>
+          <t>上海·青山吉能见面会</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>都市路4889号（莘庄地铁站南广场） 上海保利城市剧院</t>
+          <t>虹许路731号4号楼 THE BOXX•城市乐园</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2024.02.24 14:30-02.24 16:00</t>
+          <t>2024.02.25 14:30-02.25 19:30</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>5</v>
+        <v>200</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>158</t>
+          <t>380</t>
         </is>
       </c>
       <c r="H13" t="b">
@@ -2800,12 +2800,12 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80639</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80142</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/dp013A4p1704783993628.png</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/1npuHFBM1703231674558.jpeg</t>
         </is>
       </c>
     </row>
@@ -2815,43 +2815,43 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2024-02-25</t>
+          <t>2024-03-02</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>上海·青山吉能见面会</t>
+          <t>上海·2024藤田玲上海粉丝见面会</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>虹许路731号4号楼 THE BOXX•城市乐园</t>
+          <t>宜昌路179号 万代南梦宫上海文化中心</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2024.02.25 14:30-02.25 19:30</t>
+          <t>2024.03.02 12:30-03.02 19:40</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>200</v>
+        <v>9</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>580</t>
         </is>
       </c>
       <c r="H14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80142</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80993</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/1npuHFBM1703231674558.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/Vm6ntgVd1705548188785.png</t>
         </is>
       </c>
     </row>
@@ -2866,7 +2866,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>上海·2024藤田玲上海粉丝见面会</t>
+          <t>上海·小山百代2024上海粉丝见面会</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -2876,15 +2876,15 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2024.03.02 12:30-03.02 19:40</t>
+          <t>2024.03.02 13:00-03.02 20:00</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>9</v>
+        <v>234</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>580</t>
+          <t>380</t>
         </is>
       </c>
       <c r="H15" t="b">
@@ -2892,12 +2892,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80993</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80924</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/Vm6ntgVd1705548188785.png</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/FpA9OkKy1705467080070.jpeg</t>
         </is>
       </c>
     </row>
@@ -2926,7 +2926,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -2953,43 +2953,43 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2024-03-02</t>
+          <t>2024-03-09</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>上海·小山百代2024上海粉丝见面会</t>
+          <t>上海·《挪威的森林》—摇滚情歌之夜演唱会</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>宜昌路179号 万代南梦宫上海文化中心</t>
+          <t>南京西路1376号 上海商城剧院</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2024.03.02 13:00-03.02 20:00</t>
+          <t>2024.03.09 19:30-03.09 21:00</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>232</v>
+        <v>0</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>72</t>
         </is>
       </c>
       <c r="H17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80924</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81241</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/FpA9OkKy1705467080070.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/1FJ0Fj5m1705915336335.jpeg</t>
         </is>
       </c>
     </row>
@@ -3004,7 +3004,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>上海·《挪威的森林》—摇滚情歌之夜演唱会</t>
+          <t>上海·爱乐之城音乐会</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -3014,7 +3014,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2024.03.09 19:30-03.09 21:00</t>
+          <t>2024.03.09 14:00-03.09 15:30</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -3022,7 +3022,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>72</t>
+          <t>60</t>
         </is>
       </c>
       <c r="H18" t="b">
@@ -3030,12 +3030,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81241</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81289</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/1FJ0Fj5m1705915336335.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/ZZXtDrwZ1705996679699.jpeg</t>
         </is>
       </c>
     </row>
@@ -3045,30 +3045,30 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2024-03-09</t>
+          <t>2024-03-16</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>上海·爱乐之城音乐会</t>
+          <t>上海·三月的幻想演唱会2024「飞越蓝色时刻」</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>南京西路1376号 上海商城剧院</t>
+          <t>宜昌路179号 万代南梦宫上海文化中心</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2024.03.09 14:00-03.09 15:30</t>
+          <t>2024.03.16 19:00-03.16 20:30</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>380</t>
         </is>
       </c>
       <c r="H19" t="b">
@@ -3076,12 +3076,12 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81289</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80811</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/ZZXtDrwZ1705996679699.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/TO6xpSqr1705289483473.png</t>
         </is>
       </c>
     </row>
@@ -3091,30 +3091,30 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2024-03-16</t>
+          <t>2024-03-17</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>上海·三月的幻想演唱会2024「飞越蓝色时刻」</t>
+          <t>上海 ·《疯狂动物城》动漫视听音乐会</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>宜昌路179号 万代南梦宫上海文化中心</t>
+          <t>牛庄路704号 中国大戏院</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2024.03.16 19:00-03.16 20:30</t>
+          <t>2024.03.17 15:30-03.17 17:00</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>80</t>
         </is>
       </c>
       <c r="H20" t="b">
@@ -3122,12 +3122,12 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80811</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81112</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/TO6xpSqr1705289483473.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/Wg8b6SRn1705651166088.png</t>
         </is>
       </c>
     </row>
@@ -3142,25 +3142,25 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>上海 ·《疯狂动物城》动漫视听音乐会</t>
+          <t>上海·amazarashi Asia Tour 2024 「永遠市 -Eternal City-」上海公演</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>牛庄路704号 中国大戏院</t>
+          <t>宜昌路179号 万代南梦宫上海文化中心</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2024.03.17 15:30-03.17 17:00</t>
+          <t>2024.03.17 18:00-03.17 19:30</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>2</v>
+        <v>469</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>480</t>
         </is>
       </c>
       <c r="H21" t="b">
@@ -3168,12 +3168,12 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81112</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81039</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/Wg8b6SRn1705651166088.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/icsawZU11705566039011.jpeg</t>
         </is>
       </c>
     </row>
@@ -3188,25 +3188,25 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>上海·amazarashi Asia Tour 2024 「永遠市 -Eternal City-」上海公演</t>
+          <t>上海·《笑傲江湖》经典武侠影视金曲音乐会</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>宜昌路179号 万代南梦宫上海文化中心</t>
+          <t>牛庄路704号 中国大戏院</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2024.03.17 18:00-03.17 19:30</t>
+          <t>2024.03.17 19:30-03.17 21:00</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>446</v>
+        <v>1</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>480</t>
+          <t>80</t>
         </is>
       </c>
       <c r="H22" t="b">
@@ -3214,12 +3214,12 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81039</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80875</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/icsawZU11705566039011.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/8AwIAy4I1705385447242.jpeg</t>
         </is>
       </c>
     </row>
@@ -3234,21 +3234,21 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>上海·《笑傲江湖》经典武侠影视金曲音乐会</t>
+          <t>上海·遇见新海诚--帝玖「这次一定」室内乐ACG音乐会</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>牛庄路704号 中国大戏院</t>
+          <t>延安东路523号 凯迪拉克·上海音乐厅</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2024.03.17 19:30-03.17 21:00</t>
+          <t>2024.03.17 14:00-03.17 16:00</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -3260,12 +3260,12 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80875</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81258</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/8AwIAy4I1705385447242.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/eysvN81k1705977896972.jpeg</t>
         </is>
       </c>
     </row>
@@ -3275,30 +3275,30 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2024-03-17</t>
+          <t>2024-03-21</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>上海·遇见新海诚--帝玖「这次一定」室内乐ACG音乐会</t>
+          <t>上海·春卷饭 十周年  2024  专场演出</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>延安东路523号 凯迪拉克·上海音乐厅</t>
+          <t>嘉兴路街道瑞虹路188号瑞虹天地月亮湾3层 Modern Sky LAB摩登天空(瑞虹天地店)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2024.03.17 14:00-03.17 16:00</t>
+          <t>2024.03.21 20:00-03.21 22:00</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>5</v>
+        <v>349</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>480</t>
         </is>
       </c>
       <c r="H24" t="b">
@@ -3306,12 +3306,12 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81258</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81190</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/eysvN81k1705977896972.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/ho9rIMg21705894649801.jpeg</t>
         </is>
       </c>
     </row>
@@ -3321,30 +3321,30 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2024-03-21</t>
+          <t>2024-03-30</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>上海·春卷饭 十周年  2024  专场演出</t>
+          <t>上海· TRUE（唐沢美帆）上海动漫交响音乐会</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>嘉兴路街道瑞虹路188号瑞虹天地月亮湾3层 Modern Sky LAB摩登天空(瑞虹天地店)</t>
+          <t>丁香路425号 上海东方艺术中心</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2024.03.21 20:00-03.21 22:00</t>
+          <t>2024.03.30 19:30-03.30 21:00</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>328</v>
+        <v>150</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>480</t>
+          <t>280</t>
         </is>
       </c>
       <c r="H25" t="b">
@@ -3352,12 +3352,12 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81190</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80906</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/ho9rIMg21705894649801.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/FaJbLvS51705401178235.jpeg</t>
         </is>
       </c>
     </row>
@@ -3367,43 +3367,43 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>上海· TRUE（唐沢美帆）上海动漫交响音乐会</t>
+          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>丁香路425号 上海东方艺术中心</t>
+          <t>复兴中路1380号 捷豹上海交响音乐厅</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2024.03.30 19:30-03.30 21:00</t>
+          <t>2024.04.06 19:30-04.06 21:30</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>145</v>
+        <v>10</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>280</t>
+          <t>80</t>
         </is>
       </c>
       <c r="H26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80906</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80050</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/FaJbLvS51705401178235.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/0iJP3TY61703056498448.jpeg</t>
         </is>
       </c>
     </row>
@@ -3413,26 +3413,26 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
+          <t>上海·《四月是你的谎言》——“公生”与“薰”的钢琴小提琴唯美经典音乐集</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>复兴中路1380号 捷豹上海交响音乐厅</t>
+          <t>丁香路425号 上海东方艺术中心</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2024.04.06 19:30-04.06 21:30</t>
+          <t>2024.04.13 19:30-04.13 21:30</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>10</v>
+        <v>172</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -3444,12 +3444,12 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80050</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78667</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/0iJP3TY61703056498448.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202311/bTP7w6GD1700130122940.jpeg</t>
         </is>
       </c>
     </row>
@@ -3459,26 +3459,26 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2024-04-13</t>
+          <t>2024-04-20</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>上海·《四月是你的谎言》——“公生”与“薰”的钢琴小提琴唯美经典音乐集</t>
+          <t>上海·Laurent Coulondre“心动巴黎”2024中国巡回音乐会</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>丁香路425号 上海东方艺术中心</t>
+          <t>汾阳路20号上海音乐学院内 上海贺绿汀音乐厅</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2024.04.13 19:30-04.13 21:30</t>
+          <t>2024.04.20 19:30-04.20 21:30</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>172</v>
+        <v>3</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -3486,16 +3486,16 @@
         </is>
       </c>
       <c r="H28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78667</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81135</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202311/bTP7w6GD1700130122940.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/wXDdS5ap1705651730828.jpeg</t>
         </is>
       </c>
     </row>
@@ -3505,30 +3505,30 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2024-04-20</t>
+          <t>2024-04-26</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>上海·Laurent Coulondre“心动巴黎”2024中国巡回音乐会</t>
+          <t>上海· 夏川里美 2024 巡回演唱会 出道 25 周年纪念专场</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>汾阳路20号上海音乐学院内 上海贺绿汀音乐厅</t>
+          <t>东大名路889号 友邦大剧院</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2024.04.20 19:30-04.20 21:30</t>
+          <t>2024.04.26 19:30-04.26 21:30</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>280</t>
         </is>
       </c>
       <c r="H29" t="b">
@@ -3536,56 +3536,10 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81135</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81139</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
-        <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/wXDdS5ap1705651730828.jpeg</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>2024-04-26</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>上海· 夏川里美 2024 巡回演唱会 出道 25 周年纪念专场</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>东大名路889号 友邦大剧院</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>2024.04.26 19:30-04.26 21:30</t>
-        </is>
-      </c>
-      <c r="F30" t="n">
-        <v>10</v>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>280</t>
-        </is>
-      </c>
-      <c r="H30" t="b">
-        <v>0</v>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81139</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
         <is>
           <t>//i2.hdslb.com/bfs/openplatform/202401/0Fj4cYOH1705652393930.jpeg</t>
         </is>
@@ -3823,7 +3777,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1990</v>
+        <v>1995</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -3869,7 +3823,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>2093</v>
+        <v>2100</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -3915,7 +3869,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>821</v>
+        <v>824</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -3961,7 +3915,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>715</v>
+        <v>726</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -4214,7 +4168,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -4260,7 +4214,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1990</v>
+        <v>1995</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -4306,7 +4260,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>2093</v>
+        <v>2100</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -4490,7 +4444,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>821</v>
+        <v>824</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -4536,7 +4490,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>715</v>
+        <v>726</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -4628,7 +4582,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -4674,7 +4628,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -4720,7 +4674,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -4766,7 +4720,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>536</v>
+        <v>543</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -4812,7 +4766,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -4904,7 +4858,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>1167</v>
+        <v>1172</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -4950,7 +4904,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>923</v>
+        <v>931</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -5042,7 +4996,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -5088,7 +5042,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -5134,7 +5088,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>624</v>
+        <v>631</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -5180,7 +5134,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>660</v>
+        <v>672</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -5226,7 +5180,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -5272,7 +5226,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -5318,7 +5272,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -5364,7 +5318,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>1207</v>
+        <v>1212</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -5410,7 +5364,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -5456,7 +5410,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -5502,7 +5456,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>2475</v>
+        <v>2486</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -5594,7 +5548,7 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -5640,7 +5594,7 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -5686,7 +5640,7 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -5732,7 +5686,7 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -5778,7 +5732,7 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -5824,7 +5778,7 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>872</v>
+        <v>875</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -5870,7 +5824,7 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -5916,7 +5870,7 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -5962,7 +5916,7 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -6008,7 +5962,7 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -6192,7 +6146,7 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -6238,7 +6192,7 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -6330,7 +6284,7 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update gh-pages to output generated at 802b57d
</commit_message>
<xml_diff>
--- a/上海-漫展信息.xlsx
+++ b/上海-漫展信息.xlsx
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="G2" t="n">
         <v>139</v>
@@ -588,7 +588,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1678</v>
+        <v>1679</v>
       </c>
       <c r="G4" t="n">
         <v>55</v>
@@ -629,7 +629,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G5" t="n">
         <v>68</v>
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G6" t="n">
         <v>48</v>
@@ -711,7 +711,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="G7" t="n">
         <v>78</v>
@@ -793,7 +793,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>1187</v>
+        <v>1190</v>
       </c>
       <c r="G9" t="n">
         <v>68</v>
@@ -834,7 +834,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="G10" t="n">
         <v>49</v>
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="G13" t="n">
         <v>36.9</v>
@@ -998,7 +998,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G14" t="n">
         <v>60</v>
@@ -1080,7 +1080,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="G16" t="n">
         <v>60</v>
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G18" t="n">
         <v>88</v>
@@ -1244,7 +1244,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G20" t="n">
         <v>49</v>
@@ -1285,7 +1285,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G21" t="n">
         <v>48.8</v>
@@ -1326,7 +1326,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G22" t="n">
         <v>49</v>
@@ -1367,7 +1367,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G23" t="n">
         <v>60</v>
@@ -1408,7 +1408,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="G24" t="n">
         <v>65.90000000000001</v>
@@ -1449,7 +1449,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="G25" t="n">
         <v>80</v>
@@ -1531,7 +1531,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G27" t="n">
         <v>65</v>
@@ -1572,7 +1572,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>2497</v>
+        <v>2498</v>
       </c>
       <c r="G28" t="n">
         <v>65.8</v>
@@ -1613,7 +1613,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G29" t="n">
         <v>148</v>
@@ -1654,7 +1654,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G30" t="n">
         <v>49</v>
@@ -1736,7 +1736,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G32" t="n">
         <v>60</v>
@@ -1777,7 +1777,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G33" t="n">
         <v>70</v>
@@ -2064,7 +2064,7 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G40" t="n">
         <v>79</v>
@@ -2132,7 +2132,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2497,7 +2497,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="G9" t="n">
         <v>380</v>
@@ -2538,7 +2538,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="G10" t="n">
         <v>280</v>
@@ -2743,7 +2743,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G15" t="n">
         <v>380</v>
@@ -2765,38 +2765,38 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2024-03-02</t>
+          <t>2024-03-09</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>上海·小山百代2024上海粉丝见面会</t>
+          <t>上海·《挪威的森林》—摇滚情歌之夜演唱会</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>宜昌路179号 万代南梦宫上海文化中心</t>
+          <t>南京西路1376号 上海商城剧院</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2024.03.02 13:00-03.02 20:00</t>
+          <t>2024.03.09 19:30-03.09 21:00</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>237</v>
+        <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>380</v>
+        <v>72</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80924</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81241</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/FpA9OkKy1705467080070.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/1FJ0Fj5m1705915336335.jpeg</t>
         </is>
       </c>
     </row>
@@ -2811,7 +2811,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>上海·《挪威的森林》—摇滚情歌之夜演唱会</t>
+          <t>上海·爱乐之城音乐会</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -2821,23 +2821,23 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2024.03.09 19:30-03.09 21:00</t>
+          <t>2024.03.09 14:00-03.09 15:30</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" t="n">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81241</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81289</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/1FJ0Fj5m1705915336335.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/ZZXtDrwZ1705996679699.jpeg</t>
         </is>
       </c>
     </row>
@@ -2847,38 +2847,38 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2024-03-09</t>
+          <t>2024-03-16</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>上海·爱乐之城音乐会</t>
+          <t>上海·三月的幻想演唱会2024「飞越蓝色时刻」</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>南京西路1376号 上海商城剧院</t>
+          <t>宜昌路179号 万代南梦宫上海文化中心</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2024.03.09 14:00-03.09 15:30</t>
+          <t>2024.03.16 19:00-03.16 20:30</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="G18" t="n">
-        <v>60</v>
+        <v>380</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81289</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80811</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/ZZXtDrwZ1705996679699.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/TO6xpSqr1705289483473.png</t>
         </is>
       </c>
     </row>
@@ -2888,38 +2888,38 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2024-03-16</t>
+          <t>2024-03-17</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>上海·三月的幻想演唱会2024「飞越蓝色时刻」</t>
+          <t>上海 ·《疯狂动物城》动漫视听音乐会</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>宜昌路179号 万代南梦宫上海文化中心</t>
+          <t>牛庄路704号 中国大戏院</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2024.03.16 19:00-03.16 20:30</t>
+          <t>2024.03.17 15:30-03.17 17:00</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="G19" t="n">
-        <v>380</v>
+        <v>80</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80811</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81112</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/TO6xpSqr1705289483473.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/Wg8b6SRn1705651166088.png</t>
         </is>
       </c>
     </row>
@@ -2934,33 +2934,33 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>上海 ·《疯狂动物城》动漫视听音乐会</t>
+          <t>上海·amazarashi Asia Tour 2024 「永遠市 -Eternal City-」上海公演</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>牛庄路704号 中国大戏院</t>
+          <t>宜昌路179号 万代南梦宫上海文化中心</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2024.03.17 15:30-03.17 17:00</t>
+          <t>2024.03.17 18:00-03.17 19:30</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>2</v>
+        <v>528</v>
       </c>
       <c r="G20" t="n">
-        <v>80</v>
+        <v>480</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81112</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81039</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/Wg8b6SRn1705651166088.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/icsawZU11705566039011.jpeg</t>
         </is>
       </c>
     </row>
@@ -2975,33 +2975,33 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>上海·amazarashi Asia Tour 2024 「永遠市 -Eternal City-」上海公演</t>
+          <t>上海·《笑傲江湖》经典武侠影视金曲音乐会</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>宜昌路179号 万代南梦宫上海文化中心</t>
+          <t>牛庄路704号 中国大戏院</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2024.03.17 18:00-03.17 19:30</t>
+          <t>2024.03.17 19:30-03.17 21:00</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>523</v>
+        <v>1</v>
       </c>
       <c r="G21" t="n">
-        <v>480</v>
+        <v>80</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81039</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80875</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/icsawZU11705566039011.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/8AwIAy4I1705385447242.jpeg</t>
         </is>
       </c>
     </row>
@@ -3016,33 +3016,33 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>上海·《笑傲江湖》经典武侠影视金曲音乐会</t>
+          <t>上海·遇见新海诚--帝玖「这次一定」室内乐ACG音乐会</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>牛庄路704号 中国大戏院</t>
+          <t>延安东路523号 凯迪拉克·上海音乐厅</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2024.03.17 19:30-03.17 21:00</t>
+          <t>2024.03.17 14:00-03.17 16:00</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G22" t="n">
         <v>80</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80875</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81258</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/8AwIAy4I1705385447242.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/eysvN81k1705977896972.jpeg</t>
         </is>
       </c>
     </row>
@@ -3052,38 +3052,38 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2024-03-17</t>
+          <t>2024-03-21</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>上海·遇见新海诚--帝玖「这次一定」室内乐ACG音乐会</t>
+          <t>上海·春卷饭 十周年  2024  专场演出</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>延安东路523号 凯迪拉克·上海音乐厅</t>
+          <t>嘉兴路街道瑞虹路188号瑞虹天地月亮湾3层 Modern Sky LAB摩登天空(瑞虹天地店)</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2024.03.17 14:00-03.17 16:00</t>
+          <t>2024.03.21 20:00-03.21 22:00</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>9</v>
+        <v>393</v>
       </c>
       <c r="G23" t="n">
-        <v>80</v>
+        <v>480</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81258</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81190</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/eysvN81k1705977896972.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/ho9rIMg21705894649801.jpeg</t>
         </is>
       </c>
     </row>
@@ -3093,38 +3093,38 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2024-03-21</t>
+          <t>2024-03-23</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>上海·春卷饭 十周年  2024  专场演出</t>
+          <t>上海·《卡农Canon in D》世界经典作品视听音乐会</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>嘉兴路街道瑞虹路188号瑞虹天地月亮湾3层 Modern Sky LAB摩登天空(瑞虹天地店)</t>
+          <t>南京西路1376号 上海商城剧院</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2024.03.21 20:00-03.21 22:00</t>
+          <t>2024.03.23 19:30-03.23 21:00</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>387</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>480</v>
+        <v>50</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81190</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81358</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/ho9rIMg21705894649801.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/Ctne29Xn1706089385959.png</t>
         </is>
       </c>
     </row>
@@ -3139,7 +3139,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>上海·《卡农Canon in D》世界经典作品视听音乐会</t>
+          <t>上海·《四月是你的谎言》友人A经典动漫音乐会</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -3149,23 +3149,23 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2024.03.23 19:30-03.23 21:00</t>
+          <t>2024.03.23 15:00-03.23 16:30</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" t="n">
         <v>50</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81358</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81361</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/Ctne29Xn1706089385959.png</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/wL0ZWVYi1706091574963.png</t>
         </is>
       </c>
     </row>
@@ -3175,38 +3175,38 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2024-03-23</t>
+          <t>2024-03-30</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>上海·《四月是你的谎言》友人A经典动漫音乐会</t>
+          <t>上海· TRUE（唐沢美帆）上海动漫交响音乐会</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>南京西路1376号 上海商城剧院</t>
+          <t>丁香路425号 上海东方艺术中心</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2024.03.23 15:00-03.23 16:30</t>
+          <t>2024.03.30 19:30-03.30 21:00</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
+        <v>164</v>
       </c>
       <c r="G26" t="n">
-        <v>50</v>
+        <v>280</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81361</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80906</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/wL0ZWVYi1706091574963.png</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/FaJbLvS51705401178235.jpeg</t>
         </is>
       </c>
     </row>
@@ -3216,38 +3216,38 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>上海· TRUE（唐沢美帆）上海动漫交响音乐会</t>
+          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>丁香路425号 上海东方艺术中心</t>
+          <t>复兴中路1380号 捷豹上海交响音乐厅</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2024.03.30 19:30-03.30 21:00</t>
+          <t>2024.04.06 19:30-04.06 21:30</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>162</v>
+        <v>10</v>
       </c>
       <c r="G27" t="n">
-        <v>280</v>
+        <v>80</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80906</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80050</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/FaJbLvS51705401178235.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/0iJP3TY61703056498448.jpeg</t>
         </is>
       </c>
     </row>
@@ -3257,38 +3257,38 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
+          <t>上海·《四月是你的谎言》——“公生”与“薰”的钢琴小提琴唯美经典音乐集</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>复兴中路1380号 捷豹上海交响音乐厅</t>
+          <t>丁香路425号 上海东方艺术中心</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2024.04.06 19:30-04.06 21:30</t>
+          <t>2024.04.13 19:30-04.13 21:30</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="G28" t="n">
         <v>80</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80050</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78667</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/0iJP3TY61703056498448.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202311/bTP7w6GD1700130122940.jpeg</t>
         </is>
       </c>
     </row>
@@ -3298,38 +3298,38 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2024-04-13</t>
+          <t>2024-04-20</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>上海·《四月是你的谎言》——“公生”与“薰”的钢琴小提琴唯美经典音乐集</t>
+          <t>上海·Laurent Coulondre“心动巴黎”2024中国巡回音乐会</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>丁香路425号 上海东方艺术中心</t>
+          <t>汾阳路20号上海音乐学院内 上海贺绿汀音乐厅</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2024.04.13 19:30-04.13 21:30</t>
+          <t>2024.04.20 19:30-04.20 21:30</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>172</v>
+        <v>3</v>
       </c>
       <c r="G29" t="n">
         <v>80</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78667</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81135</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202311/bTP7w6GD1700130122940.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/wXDdS5ap1705651730828.jpeg</t>
         </is>
       </c>
     </row>
@@ -3339,77 +3339,36 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2024-04-20</t>
+          <t>2024-04-26</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>上海·Laurent Coulondre“心动巴黎”2024中国巡回音乐会</t>
+          <t>上海· 夏川里美 2024 巡回演唱会 出道 25 周年纪念专场</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>汾阳路20号上海音乐学院内 上海贺绿汀音乐厅</t>
+          <t>东大名路889号 友邦大剧院</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2024.04.20 19:30-04.20 21:30</t>
+          <t>2024.04.26 19:30-04.26 21:30</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G30" t="n">
-        <v>80</v>
+        <v>280</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81135</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81139</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
-        <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/wXDdS5ap1705651730828.jpeg</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>2024-04-26</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>上海· 夏川里美 2024 巡回演唱会 出道 25 周年纪念专场</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>东大名路889号 友邦大剧院</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>2024.04.26 19:30-04.26 21:30</t>
-        </is>
-      </c>
-      <c r="F31" t="n">
-        <v>11</v>
-      </c>
-      <c r="G31" t="n">
-        <v>280</v>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81139</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr">
         <is>
           <t>//i2.hdslb.com/bfs/openplatform/202401/0Fj4cYOH1705652393930.jpeg</t>
         </is>
@@ -3668,7 +3627,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>2115</v>
+        <v>2117</v>
       </c>
       <c r="G6" t="n">
         <v>30</v>
@@ -3709,7 +3668,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="G7" t="n">
         <v>30</v>
@@ -3750,7 +3709,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="G8" t="n">
         <v>10</v>
@@ -3873,7 +3832,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>571</v>
+        <v>624</v>
       </c>
       <c r="G11" t="n">
         <v>30</v>
@@ -3914,7 +3873,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="G12" t="n">
         <v>30</v>
@@ -3955,7 +3914,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G13" t="n">
         <v>30</v>
@@ -3982,7 +3941,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4142,7 +4101,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="G4" t="n">
         <v>139</v>
@@ -4224,7 +4183,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>2115</v>
+        <v>2117</v>
       </c>
       <c r="G6" t="n">
         <v>30</v>
@@ -4265,7 +4224,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>1678</v>
+        <v>1679</v>
       </c>
       <c r="G7" t="n">
         <v>55</v>
@@ -4388,7 +4347,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="G10" t="n">
         <v>30</v>
@@ -4429,7 +4388,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="G11" t="n">
         <v>10</v>
@@ -4511,7 +4470,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G13" t="n">
         <v>68</v>
@@ -4593,7 +4552,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G15" t="n">
         <v>48</v>
@@ -4634,7 +4593,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="G16" t="n">
         <v>78</v>
@@ -4757,7 +4716,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>1187</v>
+        <v>1190</v>
       </c>
       <c r="G19" t="n">
         <v>68</v>
@@ -4798,7 +4757,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="G20" t="n">
         <v>49</v>
@@ -4962,7 +4921,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="G24" t="n">
         <v>380</v>
@@ -5003,7 +4962,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="G25" t="n">
         <v>60</v>
@@ -5044,7 +5003,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G26" t="n">
         <v>88</v>
@@ -5085,7 +5044,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="G27" t="n">
         <v>280</v>
@@ -5126,7 +5085,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G28" t="n">
         <v>49</v>
@@ -5167,7 +5126,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="G29" t="n">
         <v>65.90000000000001</v>
@@ -5208,7 +5167,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="G30" t="n">
         <v>80</v>
@@ -5331,7 +5290,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>2497</v>
+        <v>2498</v>
       </c>
       <c r="G33" t="n">
         <v>65.8</v>
@@ -5372,7 +5331,7 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G34" t="n">
         <v>49</v>
@@ -5476,38 +5435,38 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2024-03-02</t>
+          <t>2024-03-03</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>上海·小山百代2024上海粉丝见面会</t>
+          <t>上海·怀旧番ONLY</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>宜昌路179号 万代南梦宫上海文化中心</t>
+          <t>逸仙路270号  上海宝丰联大酒店</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2024.03.02 13:00-03.02 20:00</t>
+          <t>2024.03.03 10:00-03.03 17:00</t>
         </is>
       </c>
       <c r="F37" t="n">
-        <v>237</v>
+        <v>138</v>
       </c>
       <c r="G37" t="n">
-        <v>380</v>
+        <v>60</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80924</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80575</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/FpA9OkKy1705467080070.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/y4uWdyPT1704700763902.jpeg</t>
         </is>
       </c>
     </row>
@@ -5517,38 +5476,38 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2024-03-03</t>
+          <t>2024-03-09</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>上海·怀旧番ONLY</t>
+          <t>上海·S·CGE动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>逸仙路270号  上海宝丰联大酒店</t>
+          <t>军工路1076号 纪希片场(秀场)</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2024.03.03 10:00-03.03 17:00</t>
+          <t>2024.03.09 10:00-03.10 17:00</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>137</v>
+        <v>40</v>
       </c>
       <c r="G38" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80575</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81173</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/y4uWdyPT1704700763902.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/TYA5FLkE1705891815532.jpeg</t>
         </is>
       </c>
     </row>
@@ -5563,33 +5522,33 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>上海·S·CGE动漫游戏嘉年华</t>
+          <t>上海·第五十三届燃梦星辰动漫嘉年华-随机宅舞</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>军工路1076号 纪希片场(秀场)</t>
+          <t>周家嘴路3608号 宝龙旭辉广场</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2024.03.09 10:00-03.10 17:00</t>
+          <t>2024.03.09 10:20-03.10 16:30</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="G39" t="n">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81173</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80571</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/TYA5FLkE1705891815532.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/SHH70VXN1704700240858.jpeg</t>
         </is>
       </c>
     </row>
@@ -5604,33 +5563,33 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>上海·第五十三届燃梦星辰动漫嘉年华-随机宅舞</t>
+          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>周家嘴路3608号 宝龙旭辉广场</t>
+          <t>漕宝路1688号 诺宝中心酒店</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2024.03.09 10:20-03.10 16:30</t>
+          <t>2024.03.09 10:00-03.09 16:30</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>45</v>
+        <v>881</v>
       </c>
       <c r="G40" t="n">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80571</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=76410</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/SHH70VXN1704700240858.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202309/fVXMrcHy1693971682397.jpeg</t>
         </is>
       </c>
     </row>
@@ -5640,38 +5599,38 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2024-03-09</t>
+          <t>2024-03-16</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
+          <t>上海·三月的幻想演唱会2024「飞越蓝色时刻」</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>漕宝路1688号 诺宝中心酒店</t>
+          <t>宜昌路179号 万代南梦宫上海文化中心</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2024.03.09 10:00-03.09 16:30</t>
+          <t>2024.03.16 19:00-03.16 20:30</t>
         </is>
       </c>
       <c r="F41" t="n">
-        <v>881</v>
+        <v>43</v>
       </c>
       <c r="G41" t="n">
-        <v>73</v>
+        <v>380</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=76410</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80811</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202309/fVXMrcHy1693971682397.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/TO6xpSqr1705289483473.png</t>
         </is>
       </c>
     </row>
@@ -5686,33 +5645,33 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>上海·三月的幻想演唱会2024「飞越蓝色时刻」</t>
+          <t>上海·坏孩纸物语の第33届动漫节之庄子篇</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>宜昌路179号 万代南梦宫上海文化中心</t>
+          <t>中山北路3300号4楼L4001号 环球港上海世嘉都市乐园</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2024.03.16 19:00-03.16 20:30</t>
+          <t>2024.03.16 10:00-03.17 21:00</t>
         </is>
       </c>
       <c r="F42" t="n">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="G42" t="n">
-        <v>380</v>
+        <v>40</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80811</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81138</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/TO6xpSqr1705289483473.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/jpr1lCt21705652306481.png</t>
         </is>
       </c>
     </row>
@@ -5722,38 +5681,38 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2024-03-16</t>
+          <t>2024-03-30</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>上海·坏孩纸物语の第33届动漫节之庄子篇</t>
+          <t>上海· TRUE（唐沢美帆）上海动漫交响音乐会</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>中山北路3300号4楼L4001号 环球港上海世嘉都市乐园</t>
+          <t>丁香路425号 上海东方艺术中心</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2024.03.16 10:00-03.17 21:00</t>
+          <t>2024.03.30 19:30-03.30 21:00</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>23</v>
+        <v>164</v>
       </c>
       <c r="G43" t="n">
-        <v>40</v>
+        <v>280</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81138</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80906</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/jpr1lCt21705652306481.png</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/FaJbLvS51705401178235.jpeg</t>
         </is>
       </c>
     </row>
@@ -5763,38 +5722,38 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>上海· TRUE（唐沢美帆）上海动漫交响音乐会</t>
+          <t>上海·第四届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>丁香路425号 上海东方艺术中心</t>
+          <t>顾村镇蕰川路6号 智慧湾科创园</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2024.03.30 19:30-03.30 21:00</t>
+          <t>2024.04.05 10:00-04.06 17:00</t>
         </is>
       </c>
       <c r="F44" t="n">
-        <v>162</v>
+        <v>61</v>
       </c>
       <c r="G44" t="n">
-        <v>280</v>
+        <v>60</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80906</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78228</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/FaJbLvS51705401178235.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202311/jgqIFxhx1699344723568.jpeg</t>
         </is>
       </c>
     </row>
@@ -5804,38 +5763,38 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>上海· TRUE（唐沢美帆）上海动漫交响音乐会</t>
+          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>丁香路425号 上海东方艺术中心</t>
+          <t>复兴中路1380号 捷豹上海交响音乐厅</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2024.03.30 19:30-03.30 21:00</t>
+          <t>2024.04.06 19:30-04.06 21:30</t>
         </is>
       </c>
       <c r="F45" t="n">
-        <v>162</v>
+        <v>10</v>
       </c>
       <c r="G45" t="n">
-        <v>280</v>
+        <v>80</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80906</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80050</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/FaJbLvS51705401178235.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/0iJP3TY61703056498448.jpeg</t>
         </is>
       </c>
     </row>
@@ -5845,38 +5804,38 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-26</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>上海·第四届次元鹿角动漫游戏展</t>
+          <t>上海· 夏川里美 2024 巡回演唱会 出道 25 周年纪念专场</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>顾村镇蕰川路6号 智慧湾科创园</t>
+          <t>东大名路889号 友邦大剧院</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2024.04.05 10:00-04.06 17:00</t>
+          <t>2024.04.26 19:30-04.26 21:30</t>
         </is>
       </c>
       <c r="F46" t="n">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="G46" t="n">
-        <v>60</v>
+        <v>280</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78228</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81139</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202311/jgqIFxhx1699344723568.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/0Fj4cYOH1705652393930.jpeg</t>
         </is>
       </c>
     </row>
@@ -5886,38 +5845,38 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-27</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
+          <t>上海·  第五十三届妖漫动漫游戏展</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>复兴中路1380号 捷豹上海交响音乐厅</t>
+          <t>曹杨路1888号 复悦荟</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2024.04.06 19:30-04.06 21:30</t>
+          <t>2024.04.27 10:00-04.27 17:00</t>
         </is>
       </c>
       <c r="F47" t="n">
-        <v>10</v>
+        <v>149</v>
       </c>
       <c r="G47" t="n">
         <v>80</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80050</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78657</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/0iJP3TY61703056498448.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/tamNdgEN1705331335847.jpeg</t>
         </is>
       </c>
     </row>
@@ -5927,38 +5886,38 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2024-04-26</t>
+          <t>2024-05-01</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>上海· 夏川里美 2024 巡回演唱会 出道 25 周年纪念专场</t>
+          <t>上海·S·CGE动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>东大名路889号 友邦大剧院</t>
+          <t>军工路1076号 纪希片场(秀场)</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2024.04.26 19:30-04.26 21:30</t>
+          <t>2024.05.01 10:00-05.02 17:00</t>
         </is>
       </c>
       <c r="F48" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G48" t="n">
-        <v>280</v>
+        <v>70</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81139</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81204</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/0Fj4cYOH1705652393930.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/nbFRULYe1705904589212.jpeg</t>
         </is>
       </c>
     </row>
@@ -5968,118 +5927,36 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2024-04-27</t>
+          <t>2024-05-01</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>上海·  第五十三届妖漫动漫游戏展</t>
+          <t>上海·魔都野良神only</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>曹杨路1888号 复悦荟</t>
+          <t>南京东路830号 第一百货</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2024.04.27 10:00-04.27 17:00</t>
+          <t>2024.05.01 10:00-05.01 17:00</t>
         </is>
       </c>
       <c r="F49" t="n">
-        <v>149</v>
+        <v>196</v>
       </c>
       <c r="G49" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78657</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80321</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
-        <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/tamNdgEN1705331335847.jpeg</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>2024-05-01</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>上海·S·CGE动漫游戏嘉年华</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>军工路1076号 纪希片场(秀场)</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>2024.05.01 10:00-05.02 17:00</t>
-        </is>
-      </c>
-      <c r="F50" t="n">
-        <v>6</v>
-      </c>
-      <c r="G50" t="n">
-        <v>70</v>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81204</t>
-        </is>
-      </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/nbFRULYe1705904589212.jpeg</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>2024-05-01</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>上海·魔都野良神only</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>南京东路830号 第一百货</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>2024.05.01 10:00-05.01 17:00</t>
-        </is>
-      </c>
-      <c r="F51" t="n">
-        <v>195</v>
-      </c>
-      <c r="G51" t="n">
-        <v>79</v>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80321</t>
-        </is>
-      </c>
-      <c r="I51" t="inlineStr">
         <is>
           <t>//i2.hdslb.com/bfs/openplatform/202401/KBlb0enU1704358750268.jpeg</t>
         </is>

</xml_diff>

<commit_message>
Update gh-pages to output generated at 7921097
</commit_message>
<xml_diff>
--- a/上海-漫展信息.xlsx
+++ b/上海-漫展信息.xlsx
@@ -588,7 +588,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1684</v>
+        <v>1685</v>
       </c>
       <c r="G4" t="n">
         <v>55</v>
@@ -629,7 +629,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G5" t="n">
         <v>68</v>
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>1197</v>
+        <v>1200</v>
       </c>
       <c r="G8" t="n">
         <v>68</v>
@@ -834,7 +834,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="G10" t="n">
         <v>129</v>
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G13" t="n">
         <v>60</v>
@@ -1039,7 +1039,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="G15" t="n">
         <v>60</v>
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>1312</v>
+        <v>1314</v>
       </c>
       <c r="G18" t="n">
         <v>98</v>
@@ -1203,7 +1203,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G19" t="n">
         <v>49</v>
@@ -1408,7 +1408,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="G24" t="n">
         <v>80</v>
@@ -1449,7 +1449,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G25" t="n">
         <v>48</v>
@@ -1531,7 +1531,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G27" t="n">
         <v>65</v>
@@ -2064,7 +2064,7 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G40" t="n">
         <v>70</v>
@@ -2292,7 +2292,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G3" t="n">
         <v>90</v>
@@ -2415,7 +2415,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G6" t="n">
         <v>88</v>
@@ -2538,7 +2538,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="G9" t="n">
         <v>380</v>
@@ -2866,7 +2866,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G17" t="n">
         <v>60</v>
@@ -2907,7 +2907,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G18" t="n">
         <v>380</v>
@@ -2989,7 +2989,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="G20" t="n">
         <v>480</v>
@@ -3112,7 +3112,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="G23" t="n">
         <v>480</v>
@@ -3194,7 +3194,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G25" t="n">
         <v>50</v>
@@ -3235,7 +3235,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="G26" t="n">
         <v>280</v>
@@ -3668,7 +3668,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="G5" t="n">
         <v>30</v>
@@ -3709,7 +3709,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>2126</v>
+        <v>2127</v>
       </c>
       <c r="G6" t="n">
         <v>30</v>
@@ -3791,7 +3791,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="G8" t="n">
         <v>10</v>
@@ -3914,7 +3914,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>751</v>
+        <v>761</v>
       </c>
       <c r="G11" t="n">
         <v>30</v>
@@ -3955,7 +3955,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="G12" t="n">
         <v>30</v>
@@ -4224,7 +4224,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="G5" t="n">
         <v>30</v>
@@ -4265,7 +4265,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>2126</v>
+        <v>2127</v>
       </c>
       <c r="G6" t="n">
         <v>30</v>
@@ -4306,7 +4306,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>1684</v>
+        <v>1685</v>
       </c>
       <c r="G7" t="n">
         <v>55</v>
@@ -4388,7 +4388,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G9" t="n">
         <v>90</v>
@@ -4470,7 +4470,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="G11" t="n">
         <v>10</v>
@@ -4511,7 +4511,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G12" t="n">
         <v>68</v>
@@ -4552,7 +4552,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G13" t="n">
         <v>88</v>
@@ -4716,7 +4716,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>1197</v>
+        <v>1200</v>
       </c>
       <c r="G17" t="n">
         <v>68</v>
@@ -4839,7 +4839,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="G20" t="n">
         <v>129</v>
@@ -4921,7 +4921,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="G22" t="n">
         <v>380</v>
@@ -4962,7 +4962,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="G23" t="n">
         <v>60</v>
@@ -5085,7 +5085,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G26" t="n">
         <v>49</v>
@@ -5167,7 +5167,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="G28" t="n">
         <v>80</v>
@@ -5208,7 +5208,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G29" t="n">
         <v>48</v>
@@ -5372,7 +5372,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G33" t="n">
         <v>49</v>
@@ -5659,7 +5659,7 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G40" t="n">
         <v>380</v>
@@ -5741,7 +5741,7 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G42" t="n">
         <v>280</v>
@@ -5987,7 +5987,7 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G48" t="n">
         <v>70</v>

</xml_diff>

<commit_message>
Update gh-pages to output generated at c4999d5
</commit_message>
<xml_diff>
--- a/上海-漫展信息.xlsx
+++ b/上海-漫展信息.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -547,7 +547,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G3" t="n">
         <v>80</v>
@@ -588,7 +588,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1690</v>
+        <v>1693</v>
       </c>
       <c r="G4" t="n">
         <v>55</v>
@@ -615,33 +615,33 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>上海·25时主题同人茶会</t>
+          <t>上海·同好召集令火影only</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>沪太路3100号 尚大国际</t>
+          <t>市真南路1199弄1号 智创TOP综合体产城</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2024.01.27 12:00-01.27 18:00</t>
+          <t>2024.01.27 10:00-01.28 18:00</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>146</v>
+        <v>574</v>
       </c>
       <c r="G5" t="n">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80548</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80284</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/dQ4DrxCk1704683144116.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/9xGb6MXN1704183627126.jpeg</t>
         </is>
       </c>
     </row>
@@ -656,33 +656,33 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>上海·同好召集令火影only</t>
+          <t>上海·第八届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>市真南路1199弄1号 智创TOP综合体产城</t>
+          <t>吴中路1588号上海爱琴海购物中心F4 竞梦元宇宙</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.28 18:00</t>
+          <t>2024.01.27 10:00-01.28 21:00</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>570</v>
+        <v>1237</v>
       </c>
       <c r="G6" t="n">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80284</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80979</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/9xGb6MXN1704183627126.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/xPOF923U1705545223366.jpeg</t>
         </is>
       </c>
     </row>
@@ -697,7 +697,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>上海·咒术only-幽暗之森1.0</t>
+          <t>上海·魔都寒假漫展-CF01</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -707,23 +707,23 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.27 16:00</t>
+          <t>2024.01.27 10:00-01.28 16:00</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>261</v>
+        <v>1019</v>
       </c>
       <c r="G7" t="n">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80045</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80204</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/hUfcrw3y1703055422885.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/eK96fdcg1703573110264.jpeg</t>
         </is>
       </c>
     </row>
@@ -733,38 +733,38 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024-01-27</t>
+          <t>2024-01-28</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>上海·第八届次元鹿角动漫游戏展</t>
+          <t>上海 ·WOW潮元原神x星铁主题二次元狂欢派对</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>吴中路1588号上海爱琴海购物中心F4 竞梦元宇宙</t>
+          <t>政通路189号五角场万达广场C栋 元气森林livehouse</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.28 21:00</t>
+          <t>2024.01.28 14:00-01.28 19:00</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>1232</v>
+        <v>456</v>
       </c>
       <c r="G8" t="n">
-        <v>98</v>
+        <v>149</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80979</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80167</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/xPOF923U1705545223366.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/QTp32HEM1705028548091.jpeg</t>
         </is>
       </c>
     </row>
@@ -774,38 +774,40 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2024-01-27</t>
+          <t>2024-01-28</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>上海·魔都寒假漫展-CF01</t>
+          <t>上海·Comic World动漫游园会（取消）</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
+          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.28 16:00</t>
+          <t>2024.01.28 09:30-01.28 17:00</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>992</v>
-      </c>
-      <c r="G9" t="n">
-        <v>59</v>
+        <v>2220</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>不可售</t>
+        </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80204</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78523</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/eK96fdcg1703573110264.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/HAkxl2611705480975408.jpeg</t>
         </is>
       </c>
     </row>
@@ -820,33 +822,33 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>上海 ·WOW潮元原神x星铁主题二次元狂欢派对</t>
+          <t>上海·坏孩纸物语の第32届动漫节之冬日季</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>政通路189号五角场万达广场C栋 元气森林livehouse</t>
+          <t>剑川路1000号 闵行龙湖天街</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2024.01.28 14:00-01.28 19:00</t>
+          <t>2024.01.28 14:00-01.28 20:00</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>444</v>
+        <v>744</v>
       </c>
       <c r="G10" t="n">
-        <v>129</v>
+        <v>36.9</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80167</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80871</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/QTp32HEM1705028548091.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/5fmQrQJ81705573963752.png</t>
         </is>
       </c>
     </row>
@@ -861,33 +863,33 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>上海·Comic World动漫游园会（取消）</t>
+          <t>上海·次元裂缝-X 新年二次元偶像日</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
+          <t>海潮路133号B1 JUMP工坊</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2024.01.28 09:30-01.28 17:00</t>
+          <t>2024.01.28 14:00-01.28 18:00</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>2220</v>
+        <v>89</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78523</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80999</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/HAkxl2611705480975408.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/lNroHqJY1705549448993.jpeg</t>
         </is>
       </c>
     </row>
@@ -897,38 +899,38 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2024-01-28</t>
+          <t>2024-01-31</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>上海·坏孩纸物语の第32届动漫节之冬日季</t>
+          <t>上海·寻迹冬日LOVELIVE同好会</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>剑川路1000号 闵行龙湖天街</t>
+          <t>愚园路1250号 新歌空间</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2024.01.28 14:00-01.28 20:00</t>
+          <t>2024.01.31 11:30-01.31 17:00</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>707</v>
+        <v>194</v>
       </c>
       <c r="G12" t="n">
-        <v>36.9</v>
+        <v>83</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80871</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79332</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/5fmQrQJ81705573963752.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/Ewreg1JT1701677993728.jpeg</t>
         </is>
       </c>
     </row>
@@ -938,12 +940,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2024-01-28</t>
+          <t>2024-02-03</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>上海·次元裂缝-X 新年二次元偶像日</t>
+          <t>上海·Coser迎春动漫展</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -953,23 +955,23 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2024.01.28 14:00-01.28 18:00</t>
+          <t>2024.02.03 10:00-02.04 17:00</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>77</v>
+        <v>855</v>
       </c>
       <c r="G13" t="n">
         <v>60</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80999</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80646</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/lNroHqJY1705549448993.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/4WVkFc4d1704787729064.jpeg</t>
         </is>
       </c>
     </row>
@@ -979,38 +981,38 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2024-01-31</t>
+          <t>2024-02-03</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>上海·寻迹冬日LOVELIVE同好会</t>
+          <t>上海·ENP电次元派对vol.04</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>愚园路1250号 新歌空间</t>
+          <t>人民大道221号 迪美购物中心</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2024.01.31 11:30-01.31 17:00</t>
+          <t>2024.02.03 18:30-02.03 22:00</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>189</v>
+        <v>22</v>
       </c>
       <c r="G14" t="n">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79332</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80945</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/Ewreg1JT1701677993728.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/1sjalWS51705479361512.jpeg</t>
         </is>
       </c>
     </row>
@@ -1025,33 +1027,33 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>上海·Coser迎春动漫展</t>
+          <t>上海·偶像梦幻祭红白歌合战Only</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>海潮路133号B1 JUMP工坊</t>
+          <t>虹许路731号4号楼 THE BOXX•城市乐园</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2024.02.03 10:00-02.04 17:00</t>
+          <t>2024.02.03 13:30-02.03 22:00</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>786</v>
+        <v>93</v>
       </c>
       <c r="G15" t="n">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80646</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81199</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/4WVkFc4d1704787729064.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/C7E7svbZ1705903245860.jpeg</t>
         </is>
       </c>
     </row>
@@ -1066,33 +1068,33 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>上海·ENP电次元派对vol.04</t>
+          <t>上海·第七届次元鹿角二次元派对</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>人民大道221号 迪美购物中心</t>
+          <t>长宁路1191号来福士西区(W)B1层01号、11号 星零界</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2024.02.03 18:30-02.03 22:00</t>
+          <t>2024.02.03 10:00-02.04 17:00</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>19</v>
+        <v>1331</v>
       </c>
       <c r="G16" t="n">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80945</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79938</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/1sjalWS51705479361512.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/b1XT2w4T1705027781100.jpeg</t>
         </is>
       </c>
     </row>
@@ -1102,38 +1104,38 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2024-02-03</t>
+          <t>2024-02-10</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>上海·偶像梦幻祭红白歌合战Only</t>
+          <t>上海·寒假CF漫展-春节档-神龙在世</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>虹许路731号4号楼 THE BOXX•城市乐园</t>
+          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2024.02.03 13:30-02.03 22:00</t>
+          <t>2024.02.10 10:00-02.17 16:00</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>86</v>
+        <v>38</v>
       </c>
       <c r="G17" t="n">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81199</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81192</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/C7E7svbZ1705903245860.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/S8XxkA631705896741998.jpeg</t>
         </is>
       </c>
     </row>
@@ -1143,38 +1145,38 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2024-02-03</t>
+          <t>2024-02-14</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>上海·第七届次元鹿角二次元派对</t>
+          <t>上海·原X铁X崩only</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>长宁路1191号来福士西区(W)B1层01号、11号 星零界</t>
+          <t>澳门路168号 月星国际家居</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2024.02.03 10:00-02.04 17:00</t>
+          <t>2024.02.14 10:30-02.14 16:30</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>1322</v>
+        <v>26</v>
       </c>
       <c r="G18" t="n">
-        <v>98</v>
+        <v>60</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79938</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81446</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/b1XT2w4T1705027781100.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/IIePRulM1706248855263.jpeg</t>
         </is>
       </c>
     </row>
@@ -1184,38 +1186,38 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2024-02-10</t>
+          <t>2024-02-14</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>上海·寒假CF漫展-春节档-神龙在世</t>
+          <t>上海·奇卡波利动漫嘉年华</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
+          <t>申滨路36号 虹桥丽宝广场</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2024.02.10 10:00-02.17 16:00</t>
+          <t>2024.02.14 10:00-02.14 17:00</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="G19" t="n">
-        <v>49</v>
+        <v>48.8</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81192</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81260</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/S8XxkA631705896741998.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/9OHovK2V1705978109130.jpeg</t>
         </is>
       </c>
     </row>
@@ -1230,33 +1232,33 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>上海·原X铁X崩only</t>
+          <t>上海·魔都COS漫展-情人节专场AM01</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>澳门路168号 月星国际家居</t>
+          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2024.02.14 10:30-02.14 16:30</t>
+          <t>2024.02.14 10:00-02.14 16:00</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>11</v>
+        <v>101</v>
       </c>
       <c r="G20" t="n">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81446</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80691</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/IIePRulM1706248855263.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/aSdjV6Kw1704868345679.jpeg</t>
         </is>
       </c>
     </row>
@@ -1266,38 +1268,38 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2024-02-14</t>
+          <t>2024-02-16</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>上海·奇卡波利动漫嘉年华</t>
+          <t>上海·次元裂缝-X 新年anikura派对</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>申滨路36号 虹桥丽宝广场</t>
+          <t>海潮路133号B1 JUMP工坊</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2024.02.14 10:00-02.14 17:00</t>
+          <t>2024.02.16 14:00-02.16 19:00</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="G21" t="n">
-        <v>48.8</v>
+        <v>60</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81260</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81314</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/9OHovK2V1705978109130.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/OrhHWKdR1706062360956.jpeg</t>
         </is>
       </c>
     </row>
@@ -1307,38 +1309,38 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2024-02-14</t>
+          <t>2024-02-16</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>上海·魔都COS漫展-情人节专场AM01</t>
+          <t>上海·第九届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
+          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2024.02.14 10:00-02.14 16:00</t>
+          <t>2024.02.16 11:00-02.17 18:00</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>99</v>
+        <v>1250</v>
       </c>
       <c r="G22" t="n">
-        <v>49</v>
+        <v>65.90000000000001</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80691</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80497</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/aSdjV6Kw1704868345679.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/0duSXTQy1704423309244.jpeg</t>
         </is>
       </c>
     </row>
@@ -1348,38 +1350,38 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2024-02-16</t>
+          <t>2024-02-17</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>上海·次元裂缝-X 新年anikura派对</t>
+          <t>上海·少女番only2.0</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>海潮路133号B1 JUMP工坊</t>
+          <t>营口路699号(黄兴公园地铁站2号口旁) 花嫁丽舍</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2024.02.16 14:00-02.16 19:00</t>
+          <t>2024.02.17 10:00-02.17 17:00</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>22</v>
+        <v>349</v>
       </c>
       <c r="G23" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81314</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81148</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/OrhHWKdR1706062360956.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/j6eEZ18S1705657346664.jpeg</t>
         </is>
       </c>
     </row>
@@ -1389,38 +1391,38 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2024-02-16</t>
+          <t>2024-02-24</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>上海·第九届次元鹿角动漫游戏展</t>
+          <t>上海·SISPmini动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
+          <t>剑川路1000号 龙湖上海闵行天街</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2024.02.16 11:00-02.17 18:00</t>
+          <t>2024.02.24 13:00-02.25 19:00</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>1242</v>
+        <v>426</v>
       </c>
       <c r="G24" t="n">
-        <v>65.90000000000001</v>
+        <v>48</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80497</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79046</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/0duSXTQy1704423309244.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/jzovdppq1706166165502.jpeg</t>
         </is>
       </c>
     </row>
@@ -1430,38 +1432,38 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2024-02-17</t>
+          <t>2024-02-24</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>上海·少女番only2.0</t>
+          <t>上海·SISP动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>营口路699号(黄兴公园地铁站2号口旁) 花嫁丽舍</t>
+          <t>年家浜路518号 周浦万达广场</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2024.02.17 10:00-02.17 17:00</t>
+          <t>2024.02.24 13:00-02.25 19:00</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>327</v>
+        <v>119</v>
       </c>
       <c r="G25" t="n">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81148</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80339</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/j6eEZ18S1705657346664.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/a8iuOufB1703832570508.jpeg</t>
         </is>
       </c>
     </row>
@@ -1476,33 +1478,33 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>上海·SISPmini动漫游戏嘉年华</t>
+          <t>上海·原神×崩坏×星铁only旅行盛宴2.0</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>剑川路1000号 龙湖上海闵行天街</t>
+          <t>西藏南路1号 上海大世界</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2024.02.24 13:00-02.25 19:00</t>
+          <t>2024.02.24 10:00-02.25 17:00</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>422</v>
+        <v>118</v>
       </c>
       <c r="G26" t="n">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79046</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81276</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/jzovdppq1706166165502.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/82hU3z8m1706155835021.png</t>
         </is>
       </c>
     </row>
@@ -1517,33 +1519,33 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>上海·SISP动漫游戏嘉年华</t>
+          <t>上海·第三届燃梦BACG PRO游戏动漫展-原X铁X崩同好交流</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>年家浜路518号 周浦万达广场</t>
+          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2024.02.24 13:00-02.25 19:00</t>
+          <t>2024.02.24 11:00-02.25 16:30</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>118</v>
+        <v>2511</v>
       </c>
       <c r="G27" t="n">
-        <v>48</v>
+        <v>65.8</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80339</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=77754</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/a8iuOufB1703832570508.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/7eGZETK91701943985671.jpeg</t>
         </is>
       </c>
     </row>
@@ -1558,33 +1560,33 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>上海·原神×崩坏×星铁only旅行盛宴2.0</t>
+          <t>上海·趣元界&amp;斗罗大陆上元佳节次元派对</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>西藏南路1号 上海大世界</t>
+          <t>长宁路1191号长宁来福士B1 长宁来福士</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2024.02.24 10:00-02.25 17:00</t>
+          <t>2024.02.24 11:30-02.25 17:30</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>89</v>
+        <v>509</v>
       </c>
       <c r="G28" t="n">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81276</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81415</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/82hU3z8m1706155835021.png</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/yis4JHfE1706169986733.jpeg</t>
         </is>
       </c>
     </row>
@@ -1599,33 +1601,33 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>上海·第三届燃梦BACG PRO游戏动漫展-原X铁X崩同好交流</t>
+          <t>上海·魔都元宵节漫展-COS为王</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
+          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2024.02.24 11:00-02.25 16:30</t>
+          <t>2024.02.24 10:00-02.25 16:00</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>2508</v>
+        <v>11</v>
       </c>
       <c r="G29" t="n">
-        <v>65.8</v>
+        <v>49</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77754</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81238</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202312/7eGZETK91701943985671.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/KxQZPADR1705913896609.jpeg</t>
         </is>
       </c>
     </row>
@@ -1640,33 +1642,33 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>上海·趣元界&amp;斗罗大陆上元佳节次元派对</t>
+          <t>上海·魔都多厨狂喜漫展-CH01</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>长宁路1191号长宁来福士B1 长宁来福士</t>
+          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2024.02.24 11:30-02.25 17:30</t>
+          <t>2024.02.24 10:00-02.25 16:00</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>508</v>
+        <v>1</v>
       </c>
       <c r="G30" t="n">
-        <v>98</v>
+        <v>49</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81415</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81423</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/yis4JHfE1706169986733.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/axpOY3zo1706173660010.jpeg</t>
         </is>
       </c>
     </row>
@@ -1676,38 +1678,38 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2024-02-24</t>
+          <t>2024-03-02</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>上海·魔都元宵节漫展-COS为王</t>
+          <t>上海·原神X星穹铁道ONLY</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
+          <t>逸仙路301号靠纪念路路口 上海宝丰联大酒店</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2024.02.24 10:00-02.25 16:00</t>
+          <t>2024.03.02 10:00-03.02 17:00</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>11</v>
+        <v>260</v>
       </c>
       <c r="G31" t="n">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81238</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80299</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/KxQZPADR1705913896609.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/V0xu26Cl1703753850690.jpeg</t>
         </is>
       </c>
     </row>
@@ -1717,38 +1719,38 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2024-02-24</t>
+          <t>2024-03-03</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>上海·魔都多厨狂喜漫展-CH01</t>
+          <t>上海·怀旧番ONLY</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
+          <t>逸仙路270号  上海宝丰联大酒店</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2024.02.24 10:00-02.25 16:00</t>
+          <t>2024.03.03 10:00-03.03 17:00</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>1</v>
+        <v>152</v>
       </c>
       <c r="G32" t="n">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81423</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80575</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/axpOY3zo1706173660010.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/y4uWdyPT1704700763902.jpeg</t>
         </is>
       </c>
     </row>
@@ -1758,38 +1760,38 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2024-03-02</t>
+          <t>2024-03-08</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>上海·原神X星穹铁道ONLY</t>
+          <t>上海·第八届ACBC动漫盛典-国潮汉服游园会</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>逸仙路301号靠纪念路路口 上海宝丰联大酒店</t>
+          <t>浦锦南路1586弄2号 奇迹花园</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2024.03.02 10:00-03.02 17:00</t>
+          <t>2024.03.08 10:00-03.10 17:00</t>
         </is>
       </c>
       <c r="F33" t="n">
-        <v>259</v>
+        <v>4</v>
       </c>
       <c r="G33" t="n">
         <v>60</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80299</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81456</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/V0xu26Cl1703753850690.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/qZtpawf51706254849667.jpeg</t>
         </is>
       </c>
     </row>
@@ -1799,38 +1801,38 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2024-03-03</t>
+          <t>2024-03-09</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>上海·怀旧番ONLY</t>
+          <t>上海·S·CGE动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>逸仙路270号  上海宝丰联大酒店</t>
+          <t>军工路1076号 纪希片场(秀场)</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2024.03.03 10:00-03.03 17:00</t>
+          <t>2024.03.09 10:00-03.10 17:00</t>
         </is>
       </c>
       <c r="F34" t="n">
-        <v>146</v>
+        <v>62</v>
       </c>
       <c r="G34" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80575</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81173</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/y4uWdyPT1704700763902.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/TYA5FLkE1705891815532.jpeg</t>
         </is>
       </c>
     </row>
@@ -1840,38 +1842,38 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2024-03-08</t>
+          <t>2024-03-09</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>上海·第八届ACBC动漫盛典-国潮汉服游园会</t>
+          <t>上海·第五十三届燃梦星辰动漫嘉年华-随机宅舞</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>浦锦南路1586弄2号 奇迹花园</t>
+          <t>周家嘴路3608号 宝龙旭辉广场</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2024.03.08 10:00-03.10 17:00</t>
+          <t>2024.03.09 10:20-03.10 16:30</t>
         </is>
       </c>
       <c r="F35" t="n">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="G35" t="n">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81456</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80571</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/qZtpawf51706254849667.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/SHH70VXN1704700240858.jpeg</t>
         </is>
       </c>
     </row>
@@ -1886,33 +1888,33 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>上海·S·CGE动漫游戏嘉年华</t>
+          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>军工路1076号 纪希片场(秀场)</t>
+          <t>漕宝路1688号 诺宝中心酒店</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2024.03.09 10:00-03.10 17:00</t>
+          <t>2024.03.09 10:00-03.09 16:30</t>
         </is>
       </c>
       <c r="F36" t="n">
-        <v>56</v>
+        <v>893</v>
       </c>
       <c r="G36" t="n">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81173</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=76410</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/TYA5FLkE1705891815532.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202309/fVXMrcHy1693971682397.jpeg</t>
         </is>
       </c>
     </row>
@@ -1922,38 +1924,38 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2024-03-09</t>
+          <t>2024-03-16</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>上海·第五十三届燃梦星辰动漫嘉年华-随机宅舞</t>
+          <t>上海·坏孩纸物语の第33届动漫节之庄子篇</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>周家嘴路3608号 宝龙旭辉广场</t>
+          <t>中山北路3300号4楼L4001号 环球港上海世嘉都市乐园</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2024.03.09 10:20-03.10 16:30</t>
+          <t>2024.03.16 10:00-03.17 21:00</t>
         </is>
       </c>
       <c r="F37" t="n">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="G37" t="n">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80571</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81138</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/SHH70VXN1704700240858.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/jpr1lCt21705652306481.png</t>
         </is>
       </c>
     </row>
@@ -1963,38 +1965,38 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2024-03-09</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
+          <t>上海·第四届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>漕宝路1688号 诺宝中心酒店</t>
+          <t>顾村镇蕰川路6号 智慧湾科创园</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2024.03.09 10:00-03.09 16:30</t>
+          <t>2024.04.05 10:00-04.06 17:00</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>888</v>
+        <v>63</v>
       </c>
       <c r="G38" t="n">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=76410</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78228</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202309/fVXMrcHy1693971682397.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202311/jgqIFxhx1699344723568.jpeg</t>
         </is>
       </c>
     </row>
@@ -2004,38 +2006,38 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2024-03-16</t>
+          <t>2024-04-27</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>上海·坏孩纸物语の第33届动漫节之庄子篇</t>
+          <t>上海·  第五十三届妖漫动漫游戏展</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>中山北路3300号4楼L4001号 环球港上海世嘉都市乐园</t>
+          <t>曹杨路1888号 复悦荟</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2024.03.16 10:00-03.17 21:00</t>
+          <t>2024.04.27 10:00-04.27 17:00</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>24</v>
+        <v>149</v>
       </c>
       <c r="G39" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81138</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78657</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/jpr1lCt21705652306481.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/tamNdgEN1705331335847.jpeg</t>
         </is>
       </c>
     </row>
@@ -2045,38 +2047,38 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-05-01</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>上海·第四届次元鹿角动漫游戏展</t>
+          <t>上海·S·CGE动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>顾村镇蕰川路6号 智慧湾科创园</t>
+          <t>军工路1076号 纪希片场(秀场)</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2024.04.05 10:00-04.06 17:00</t>
+          <t>2024.05.01 10:00-05.02 17:00</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="G40" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78228</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81204</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202311/jgqIFxhx1699344723568.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/nbFRULYe1705904589212.jpeg</t>
         </is>
       </c>
     </row>
@@ -2086,38 +2088,38 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2024-04-27</t>
+          <t>2024-05-01</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>上海·  第五十三届妖漫动漫游戏展</t>
+          <t>上海·魔都野良神only</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>曹杨路1888号 复悦荟</t>
+          <t>南京东路830号 第一百货</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2024.04.27 10:00-04.27 17:00</t>
+          <t>2024.05.01 10:00-05.01 17:00</t>
         </is>
       </c>
       <c r="F41" t="n">
-        <v>149</v>
+        <v>209</v>
       </c>
       <c r="G41" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78657</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80321</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/tamNdgEN1705331335847.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/KBlb0enU1704358750268.jpeg</t>
         </is>
       </c>
     </row>
@@ -2127,118 +2129,36 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2024-05-01</t>
+          <t>2024-05-05</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>上海·S·CGE动漫游戏嘉年华</t>
+          <t>上海·灌篮高手--青春永不散场</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>军工路1076号 纪希片场(秀场)</t>
+          <t>逸仙路1328弄 新业坊</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2024.05.01 10:00-05.02 17:00</t>
+          <t>2024.05.05 10:00-05.05 17:00</t>
         </is>
       </c>
       <c r="F42" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G42" t="n">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81204</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80835</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
-        <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/nbFRULYe1705904589212.jpeg</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>2024-05-01</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>上海·魔都野良神only</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>南京东路830号 第一百货</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>2024.05.01 10:00-05.01 17:00</t>
-        </is>
-      </c>
-      <c r="F43" t="n">
-        <v>204</v>
-      </c>
-      <c r="G43" t="n">
-        <v>79</v>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80321</t>
-        </is>
-      </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/KBlb0enU1704358750268.jpeg</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>2024-05-05</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>上海·灌篮高手--青春永不散场</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>逸仙路1328弄 新业坊</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>2024.05.05 10:00-05.05 17:00</t>
-        </is>
-      </c>
-      <c r="F44" t="n">
-        <v>14</v>
-      </c>
-      <c r="G44" t="n">
-        <v>89</v>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80835</t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr">
         <is>
           <t>//i1.hdslb.com/bfs/openplatform/202401/hdaVclFC1705301931054.jpeg</t>
         </is>
@@ -2255,7 +2175,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2374,7 +2294,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G3" t="n">
         <v>90</v>
@@ -2417,8 +2337,10 @@
       <c r="F4" t="n">
         <v>50</v>
       </c>
-      <c r="G4" t="n">
-        <v>0</v>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>不可售</t>
+        </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -2437,38 +2359,38 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024-01-27</t>
+          <t>2024-02-02</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>上海·Azurock」Azurose ACG Cover Live</t>
+          <t>上海·次元LAB 二次元电音节</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>愚园路1398号 育音堂音乐公园</t>
+          <t>中兴路1683号金融街购物中心L3-27 蜚声上海Livehouse</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2024.01.27 19:00-01.27 21:30</t>
+          <t>2024.02.02 12:30-02.02 21:00</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>73</v>
+        <v>672</v>
       </c>
       <c r="G5" t="n">
-        <v>108</v>
+        <v>380</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80277</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80128</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202312/5d6O1Rf11703742965244.png</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/DEW1XYty1703226993965.jpeg</t>
         </is>
       </c>
     </row>
@@ -2478,38 +2400,38 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2024-01-27</t>
+          <t>2024-02-04</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>上海·日本原版《数码宝贝舞台剧：游乐园之谜》</t>
+          <t>上海·触手猴钢琴巡演·marasy piano live tour『生音』上海站·Powered by 东方弹幕神乐失落幻想</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>茂名南路57号近长乐路 上海兰心大戏院</t>
+          <t>丁香路425号(上海科技馆地铁站1号口步行460米) 上海东方艺术中心音乐厅</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2024.01.27 15:30-01.27 20:55</t>
+          <t>2024.02.04 19:30-02.04 21:00</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>34</v>
+        <v>470</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>280</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79783</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80734</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/S6nZ327b1702534484951.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/IcjPp0TE1704951328918.jpeg</t>
         </is>
       </c>
     </row>
@@ -2519,38 +2441,38 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024-01-27</t>
+          <t>2024-02-14</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>上海•Risa Yuzuki 1st ONEMAN LIVE 「Future Interlink」 追加公演</t>
+          <t>上海·【情人节特辑】《那年我们》记忆重启韩剧经典OST音乐会《请回答1988》《来自星星的你》</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>愚园路1250号 新歌空间</t>
+          <t>牛庄路704号 中国大戏院</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2024.01.27 18:30-01.27 21:00</t>
+          <t>2024.02.14 19:30-02.14 21:00</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>300</v>
+        <v>4</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77773</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80615</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202310/XKKYWAk51698315607196.png</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/5DDVhKcO1704767761361.png</t>
         </is>
       </c>
     </row>
@@ -2560,38 +2482,38 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024-02-02</t>
+          <t>2024-02-24</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>上海·次元LAB 二次元电音节</t>
+          <t>上海·《哈利的魔法世界》动漫视听音乐会</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>中兴路1683号金融街购物中心L3-27 蜚声上海Livehouse</t>
+          <t>都市路4889号（莘庄地铁站南广场） 上海保利城市剧院</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2024.02.02 12:30-02.02 21:00</t>
+          <t>2024.02.24 14:30-02.24 16:00</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>659</v>
+        <v>9</v>
       </c>
       <c r="G8" t="n">
-        <v>380</v>
+        <v>158</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80128</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80639</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202312/DEW1XYty1703226993965.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/4PieCC9N1706261750579.jpeg</t>
         </is>
       </c>
     </row>
@@ -2601,38 +2523,38 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2024-02-04</t>
+          <t>2024-02-25</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>上海·触手猴钢琴巡演·marasy piano live tour『生音』上海站·Powered by 东方弹幕神乐失落幻想</t>
+          <t>上海·青山吉能见面会</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>丁香路425号(上海科技馆地铁站1号口步行460米) 上海东方艺术中心音乐厅</t>
+          <t>虹许路731号4号楼 THE BOXX•城市乐园</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2024.02.04 19:30-02.04 21:00</t>
+          <t>2024.02.25 14:30-02.25 19:30</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>372</v>
+        <v>205</v>
       </c>
       <c r="G9" t="n">
-        <v>280</v>
+        <v>380</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80734</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80142</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/IcjPp0TE1704951328918.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/1npuHFBM1703231674558.jpeg</t>
         </is>
       </c>
     </row>
@@ -2642,38 +2564,38 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2024-02-14</t>
+          <t>2024-03-02</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>上海·【情人节特辑】《那年我们》记忆重启韩剧经典OST音乐会《请回答1988》《来自星星的你》</t>
+          <t>上海·2024藤田玲上海粉丝见面会</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>牛庄路704号 中国大戏院</t>
+          <t>宜昌路179号 万代南梦宫上海文化中心</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2024.02.14 19:30-02.14 21:00</t>
+          <t>2024.03.02 12:30-03.02 19:40</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G10" t="n">
-        <v>80</v>
+        <v>580</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80615</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80993</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/5DDVhKcO1704767761361.png</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/Vm6ntgVd1705548188785.png</t>
         </is>
       </c>
     </row>
@@ -2683,38 +2605,38 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2024-02-24</t>
+          <t>2024-03-02</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>上海·《哈利的魔法世界》动漫视听音乐会</t>
+          <t>上海·小山百代2024上海粉丝见面会</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>都市路4889号（莘庄地铁站南广场） 上海保利城市剧院</t>
+          <t>宜昌路179号 万代南梦宫上海文化中心</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2024.02.24 14:30-02.24 16:00</t>
+          <t>2024.03.02 13:00-03.02 20:00</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>8</v>
+        <v>249</v>
       </c>
       <c r="G11" t="n">
-        <v>158</v>
+        <v>380</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80639</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80924</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/4PieCC9N1706261750579.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/FpA9OkKy1705467080070.jpeg</t>
         </is>
       </c>
     </row>
@@ -2724,38 +2646,38 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2024-02-25</t>
+          <t>2024-03-09</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>上海·青山吉能见面会</t>
+          <t>上海·《挪威的森林》—摇滚情歌之夜演唱会</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>虹许路731号4号楼 THE BOXX•城市乐园</t>
+          <t>南京西路1376号 上海商城剧院</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2024.02.25 14:30-02.25 19:30</t>
+          <t>2024.03.09 19:30-03.09 21:00</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>204</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>380</v>
+        <v>72</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80142</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81241</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/1npuHFBM1703231674558.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/1FJ0Fj5m1705915336335.jpeg</t>
         </is>
       </c>
     </row>
@@ -2765,38 +2687,38 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2024-03-02</t>
+          <t>2024-03-09</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>上海·2024藤田玲上海粉丝见面会</t>
+          <t>上海·爱乐之城音乐会</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>宜昌路179号 万代南梦宫上海文化中心</t>
+          <t>南京西路1376号 上海商城剧院</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2024.03.02 12:30-03.02 19:40</t>
+          <t>2024.03.09 14:00-03.09 15:30</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G13" t="n">
-        <v>580</v>
+        <v>60</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80993</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81289</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/Vm6ntgVd1705548188785.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/ZZXtDrwZ1705996679699.jpeg</t>
         </is>
       </c>
     </row>
@@ -2806,12 +2728,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2024-03-02</t>
+          <t>2024-03-16</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>上海·小山百代2024上海粉丝见面会</t>
+          <t>上海·三月的幻想演唱会2024「飞越蓝色时刻」</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -2821,23 +2743,23 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2024.03.02 13:00-03.02 20:00</t>
+          <t>2024.03.16 19:00-03.16 20:30</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>247</v>
+        <v>49</v>
       </c>
       <c r="G14" t="n">
         <v>380</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80924</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80811</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/FpA9OkKy1705467080070.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/TO6xpSqr1705289483473.png</t>
         </is>
       </c>
     </row>
@@ -2847,38 +2769,38 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2024-03-09</t>
+          <t>2024-03-17</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>上海·《挪威的森林》—摇滚情歌之夜演唱会</t>
+          <t>上海 ·《疯狂动物城》动漫视听音乐会</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>南京西路1376号 上海商城剧院</t>
+          <t>牛庄路704号 中国大戏院</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2024.03.09 19:30-03.09 21:00</t>
+          <t>2024.03.17 15:30-03.17 17:00</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G15" t="n">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81241</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81112</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/1FJ0Fj5m1705915336335.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/Wg8b6SRn1705651166088.png</t>
         </is>
       </c>
     </row>
@@ -2888,38 +2810,38 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2024-03-09</t>
+          <t>2024-03-17</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>上海·爱乐之城音乐会</t>
+          <t>上海·amazarashi Asia Tour 2024 「永遠市 -Eternal City-」上海公演</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>南京西路1376号 上海商城剧院</t>
+          <t>宜昌路179号 万代南梦宫上海文化中心</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2024.03.09 14:00-03.09 15:30</t>
+          <t>2024.03.17 18:00-03.17 19:30</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>2</v>
+        <v>641</v>
       </c>
       <c r="G16" t="n">
-        <v>60</v>
+        <v>480</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81289</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81039</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/ZZXtDrwZ1705996679699.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/icsawZU11705566039011.jpeg</t>
         </is>
       </c>
     </row>
@@ -2929,38 +2851,38 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2024-03-16</t>
+          <t>2024-03-17</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>上海·三月的幻想演唱会2024「飞越蓝色时刻」</t>
+          <t>上海·《笑傲江湖》经典武侠影视金曲音乐会</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>宜昌路179号 万代南梦宫上海文化中心</t>
+          <t>牛庄路704号 中国大戏院</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2024.03.16 19:00-03.16 20:30</t>
+          <t>2024.03.17 19:30-03.17 21:00</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="G17" t="n">
-        <v>380</v>
+        <v>80</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80811</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80875</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/TO6xpSqr1705289483473.png</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/8AwIAy4I1705385447242.jpeg</t>
         </is>
       </c>
     </row>
@@ -2975,33 +2897,33 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>上海 ·《疯狂动物城》动漫视听音乐会</t>
+          <t>上海·遇见新海诚--帝玖「这次一定」室内乐ACG音乐会</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>牛庄路704号 中国大戏院</t>
+          <t>延安东路523号 凯迪拉克·上海音乐厅</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2024.03.17 15:30-03.17 17:00</t>
+          <t>2024.03.17 14:00-03.17 16:00</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="G18" t="n">
         <v>80</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81112</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81258</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/Wg8b6SRn1705651166088.png</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/eysvN81k1705977896972.jpeg</t>
         </is>
       </c>
     </row>
@@ -3011,38 +2933,38 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2024-03-17</t>
+          <t>2024-03-21</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>上海·amazarashi Asia Tour 2024 「永遠市 -Eternal City-」上海公演</t>
+          <t>上海·春卷饭 十周年  2024  专场演出</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>宜昌路179号 万代南梦宫上海文化中心</t>
+          <t>嘉兴路街道瑞虹路188号瑞虹天地月亮湾3层 Modern Sky LAB摩登天空(瑞虹天地店)</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2024.03.17 18:00-03.17 19:30</t>
+          <t>2024.03.21 20:00-03.21 22:00</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>614</v>
+        <v>470</v>
       </c>
       <c r="G19" t="n">
         <v>480</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81039</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81190</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/icsawZU11705566039011.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/ho9rIMg21705894649801.jpeg</t>
         </is>
       </c>
     </row>
@@ -3052,38 +2974,38 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2024-03-17</t>
+          <t>2024-03-23</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>上海·《笑傲江湖》经典武侠影视金曲音乐会</t>
+          <t>上海·《卡农Canon in D》世界经典作品视听音乐会</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>牛庄路704号 中国大戏院</t>
+          <t>南京西路1376号 上海商城剧院</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2024.03.17 19:30-03.17 21:00</t>
+          <t>2024.03.23 19:30-03.23 21:00</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80875</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81358</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/8AwIAy4I1705385447242.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/Ctne29Xn1706089385959.png</t>
         </is>
       </c>
     </row>
@@ -3093,38 +3015,38 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2024-03-17</t>
+          <t>2024-03-23</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>上海·遇见新海诚--帝玖「这次一定」室内乐ACG音乐会</t>
+          <t>上海·《四月是你的谎言》友人A经典动漫音乐会</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>延安东路523号 凯迪拉克·上海音乐厅</t>
+          <t>南京西路1376号 上海商城剧院</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2024.03.17 14:00-03.17 16:00</t>
+          <t>2024.03.23 15:00-03.23 16:30</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G21" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81258</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81361</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/eysvN81k1705977896972.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/wL0ZWVYi1706091574963.png</t>
         </is>
       </c>
     </row>
@@ -3134,38 +3056,38 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2024-03-21</t>
+          <t>2024-03-30</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>上海·春卷饭 十周年  2024  专场演出</t>
+          <t>上海· TRUE（唐沢美帆）上海动漫交响音乐会</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>嘉兴路街道瑞虹路188号瑞虹天地月亮湾3层 Modern Sky LAB摩登天空(瑞虹天地店)</t>
+          <t>丁香路425号 上海东方艺术中心</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2024.03.21 20:00-03.21 22:00</t>
+          <t>2024.03.30 19:30-03.30 21:00</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>437</v>
+        <v>190</v>
       </c>
       <c r="G22" t="n">
         <v>480</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81190</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80906</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/ho9rIMg21705894649801.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/FaJbLvS51705401178235.jpeg</t>
         </is>
       </c>
     </row>
@@ -3175,38 +3097,38 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2024-03-23</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>上海·《卡农Canon in D》世界经典作品视听音乐会</t>
+          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>南京西路1376号 上海商城剧院</t>
+          <t>复兴中路1380号 捷豹上海交响音乐厅</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2024.03.23 19:30-03.23 21:00</t>
+          <t>2024.04.06 19:30-04.06 21:30</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G23" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81358</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80050</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/Ctne29Xn1706089385959.png</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202312/0iJP3TY61703056498448.jpeg</t>
         </is>
       </c>
     </row>
@@ -3216,38 +3138,38 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2024-03-23</t>
+          <t>2024-04-13</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>上海·《四月是你的谎言》友人A经典动漫音乐会</t>
+          <t>上海·《四月是你的谎言》——“公生”与“薰”的钢琴小提琴唯美经典音乐集</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>南京西路1376号 上海商城剧院</t>
+          <t>丁香路425号 上海东方艺术中心</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2024.03.23 15:00-03.23 16:30</t>
+          <t>2024.04.13 19:30-04.13 21:30</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>9</v>
+        <v>178</v>
       </c>
       <c r="G24" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81361</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78667</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/wL0ZWVYi1706091574963.png</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202311/bTP7w6GD1700130122940.jpeg</t>
         </is>
       </c>
     </row>
@@ -3257,38 +3179,38 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-20</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>上海· TRUE（唐沢美帆）上海动漫交响音乐会</t>
+          <t>上海·Laurent Coulondre“心动巴黎”2024中国巡回音乐会</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>丁香路425号 上海东方艺术中心</t>
+          <t>汾阳路20号上海音乐学院内 上海贺绿汀音乐厅</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2024.03.30 19:30-03.30 21:00</t>
+          <t>2024.04.20 19:30-04.20 21:30</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>186</v>
+        <v>3</v>
       </c>
       <c r="G25" t="n">
-        <v>280</v>
+        <v>80</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80906</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81135</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/FaJbLvS51705401178235.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/wXDdS5ap1705651730828.jpeg</t>
         </is>
       </c>
     </row>
@@ -3298,38 +3220,38 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-26</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>上海·从Butter-Fly到夏目之爱してる —— “好想大声说爱你”动漫钢琴演奏会</t>
+          <t>上海· 夏川里美 2024 巡回演唱会 出道 25 周年纪念专场</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>复兴中路1380号 捷豹上海交响音乐厅</t>
+          <t>东大名路889号 友邦大剧院</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2024.04.06 19:30-04.06 21:30</t>
+          <t>2024.04.26 19:30-04.26 21:30</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G26" t="n">
-        <v>80</v>
+        <v>280</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80050</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81139</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/0iJP3TY61703056498448.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/0Fj4cYOH1705652393930.jpeg</t>
         </is>
       </c>
     </row>
@@ -3339,159 +3261,36 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2024-04-13</t>
+          <t>2024-06-08</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>上海·《四月是你的谎言》——“公生”与“薰”的钢琴小提琴唯美经典音乐集</t>
+          <t>上海·菊次郎的夏天——久石让钢琴曲梦幻之旅演奏会</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>丁香路425号 上海东方艺术中心</t>
+          <t>延安东路523号 凯迪拉克·上海音乐厅</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2024.04.13 19:30-04.13 21:30</t>
+          <t>2024.06.08 19:30-06.08 21:00</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>178</v>
+        <v>2</v>
       </c>
       <c r="G27" t="n">
         <v>80</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78667</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81413</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
-        <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202311/bTP7w6GD1700130122940.jpeg</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>2024-04-20</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>上海·Laurent Coulondre“心动巴黎”2024中国巡回音乐会</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>汾阳路20号上海音乐学院内 上海贺绿汀音乐厅</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>2024.04.20 19:30-04.20 21:30</t>
-        </is>
-      </c>
-      <c r="F28" t="n">
-        <v>3</v>
-      </c>
-      <c r="G28" t="n">
-        <v>80</v>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81135</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/wXDdS5ap1705651730828.jpeg</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>2024-04-26</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>上海· 夏川里美 2024 巡回演唱会 出道 25 周年纪念专场</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>东大名路889号 友邦大剧院</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>2024.04.26 19:30-04.26 21:30</t>
-        </is>
-      </c>
-      <c r="F29" t="n">
-        <v>12</v>
-      </c>
-      <c r="G29" t="n">
-        <v>280</v>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81139</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/0Fj4cYOH1705652393930.jpeg</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>2024-06-08</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>上海·菊次郎的夏天——久石让钢琴曲梦幻之旅演奏会</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>延安东路523号 凯迪拉克·上海音乐厅</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>2024.06.08 19:30-06.08 21:00</t>
-        </is>
-      </c>
-      <c r="F30" t="n">
-        <v>0</v>
-      </c>
-      <c r="G30" t="n">
-        <v>80</v>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81413</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
         <is>
           <t>//i2.hdslb.com/bfs/openplatform/202401/QqKuy4611706169245363.jpeg</t>
         </is>
@@ -3586,7 +3385,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1733</v>
+        <v>1735</v>
       </c>
       <c r="G2" t="n">
         <v>60</v>
@@ -3709,7 +3508,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>2022</v>
+        <v>2026</v>
       </c>
       <c r="G5" t="n">
         <v>30</v>
@@ -3750,7 +3549,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>2154</v>
+        <v>2174</v>
       </c>
       <c r="G6" t="n">
         <v>30</v>
@@ -3791,7 +3590,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>844</v>
+        <v>857</v>
       </c>
       <c r="G7" t="n">
         <v>30</v>
@@ -3832,7 +3631,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>809</v>
+        <v>832</v>
       </c>
       <c r="G8" t="n">
         <v>10</v>
@@ -3955,7 +3754,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>853</v>
+        <v>944</v>
       </c>
       <c r="G11" t="n">
         <v>30</v>
@@ -3996,7 +3795,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>140</v>
+        <v>167</v>
       </c>
       <c r="G12" t="n">
         <v>30</v>
@@ -4037,7 +3836,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="G13" t="n">
         <v>30</v>
@@ -4142,7 +3941,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1733</v>
+        <v>1735</v>
       </c>
       <c r="G2" t="n">
         <v>60</v>
@@ -4164,38 +3963,38 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>2023-12-01</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>上海·Hello Kitty Cosmos 50周年光影特展</t>
+          <t>上海·2023《蔚蓝档案》x  萌果酱谷子咖啡</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>漕宝路3055号 宝龙美术馆</t>
+          <t>南京东路340号百联ZX 萌果酱谷子咖啡（百联）</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023.11.02 10:00-2024.01.28 18:00</t>
+          <t>2023.12.01 00:00-2024.01.31 23:59</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>124</v>
+        <v>2026</v>
       </c>
       <c r="G3" t="n">
-        <v>139</v>
+        <v>30</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77862</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79005</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202310/QnmD4yOd1698652192047.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202311/02P8eD3Z1700821985538.jpeg</t>
         </is>
       </c>
     </row>
@@ -4205,38 +4004,38 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2023-12-01</t>
+          <t>2023-12-06</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>上海·2023《蔚蓝档案》x  萌果酱谷子咖啡</t>
+          <t>上海·「咒术回战  × animate cafe」</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>南京东路340号百联ZX 萌果酱谷子咖啡（百联）</t>
+          <t>西藏北路198号大悦城北座8楼N809-1 animate cafe上海店</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023.12.01 00:00-2024.01.31 23:59</t>
+          <t>2023.12.06 00:00-2024.02.27 23:59</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>2022</v>
+        <v>2174</v>
       </c>
       <c r="G4" t="n">
         <v>30</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79005</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79292</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202311/02P8eD3Z1700821985538.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/LyD46Kty1705488020552.jpeg</t>
         </is>
       </c>
     </row>
@@ -4246,38 +4045,38 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2023-12-06</t>
+          <t>2023-12-10</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>上海·「咒术回战  × animate cafe」</t>
+          <t>上海·多维跃迁-2023 红点设计概念大奖获奖作品展</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>西藏北路198号大悦城北座8楼N809-1 animate cafe上海店</t>
+          <t>国展路1099号 上海世博展览馆</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023.12.06 00:00-2024.02.27 23:59</t>
+          <t>2023.12.10 12:00-2024.02.16 17:00</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>2154</v>
+        <v>34</v>
       </c>
       <c r="G5" t="n">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79292</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=78809</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/LyD46Kty1705488020552.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202311/YsBoZAOW1700551290654.jpeg</t>
         </is>
       </c>
     </row>
@@ -4306,7 +4105,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1690</v>
+        <v>1693</v>
       </c>
       <c r="G6" t="n">
         <v>55</v>
@@ -4388,7 +4187,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G8" t="n">
         <v>90</v>
@@ -4410,38 +4209,38 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2023-12-31</t>
+          <t>2024-01-06</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>上海·次元波板糖×时光代理人「锦瑟华年主题快闪店」</t>
+          <t>上海·罗小黑 x HAPPY ZOO主题Cafe</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>西藏北路166静安大悦城北座6楼611号 次元波板糖</t>
+          <t>南京东路340号 百联zx创趣场</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2023.12.31 00:00-2024.01.29 23:59</t>
+          <t>2024.01.06 00:00-02.29 23:59</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>844</v>
+        <v>832</v>
       </c>
       <c r="G9" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79972</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80171</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202312/z7bFCMqM1702972063289.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/chPePM8d1703485388734.png</t>
         </is>
       </c>
     </row>
@@ -4451,38 +4250,38 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2024-01-06</t>
+          <t>2024-01-22</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>上海·罗小黑 x HAPPY ZOO主题Cafe</t>
+          <t>上海·「新春特惠」世嘉都市乐园-JP国潮杂技嘉年华</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>南京东路340号 百联zx创趣场</t>
+          <t>中山北路3300号环球港购物中心4楼 上海世嘉都市乐园</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2024.01.06 00:00-02.29 23:59</t>
+          <t>2024.01.22 14:00-03.03 18:40</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>809</v>
+        <v>1</v>
       </c>
       <c r="G10" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80171</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81210</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/chPePM8d1703485388734.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/sw2khwYM1706086166106.jpeg</t>
         </is>
       </c>
     </row>
@@ -4492,38 +4291,38 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2024-01-22</t>
+          <t>2024-01-27</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>上海·「新春特惠」世嘉都市乐园-JP国潮杂技嘉年华</t>
+          <t>上海·同好召集令火影only</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>中山北路3300号环球港购物中心4楼 上海世嘉都市乐园</t>
+          <t>市真南路1199弄1号 智创TOP综合体产城</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2024.01.22 14:00-03.03 18:40</t>
+          <t>2024.01.27 10:00-01.28 18:00</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>574</v>
       </c>
       <c r="G11" t="n">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81210</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80284</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/sw2khwYM1706086166106.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/9xGb6MXN1704183627126.jpeg</t>
         </is>
       </c>
     </row>
@@ -4538,33 +4337,33 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>上海·25时主题同人茶会</t>
+          <t>上海·魔都寒假漫展-CF01</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>沪太路3100号 尚大国际</t>
+          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2024.01.27 12:00-01.27 18:00</t>
+          <t>2024.01.27 10:00-01.28 16:00</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>146</v>
+        <v>1019</v>
       </c>
       <c r="G12" t="n">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80548</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80204</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/dQ4DrxCk1704683144116.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/eK96fdcg1703573110264.jpeg</t>
         </is>
       </c>
     </row>
@@ -4579,33 +4378,33 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>上海·Azurock」Azurose ACG Cover Live</t>
+          <t>上海・明日方舟主题店·[SWEET ZONE甜蜜区域]</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>愚园路1398号 育音堂音乐公园</t>
+          <t>南京东路830号第一百货商业中心B馆5楼(海底捞旁边) 第一百货商业中心</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2024.01.27 19:00-01.27 21:30</t>
+          <t>2024.01.27 00:00-03.31 23:59</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>73</v>
+        <v>944</v>
       </c>
       <c r="G13" t="n">
-        <v>108</v>
+        <v>30</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80277</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81277</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202312/5d6O1Rf11703742965244.png</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/hp6D0Drt1705991831205.jpeg</t>
         </is>
       </c>
     </row>
@@ -4615,38 +4414,38 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2024-01-27</t>
+          <t>2024-01-28</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>上海·同好召集令火影only</t>
+          <t>上海 ·WOW潮元原神x星铁主题二次元狂欢派对</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>市真南路1199弄1号 智创TOP综合体产城</t>
+          <t>政通路189号五角场万达广场C栋 元气森林livehouse</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.28 18:00</t>
+          <t>2024.01.28 14:00-01.28 19:00</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>570</v>
+        <v>456</v>
       </c>
       <c r="G14" t="n">
-        <v>88</v>
+        <v>149</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80284</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80167</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/9xGb6MXN1704183627126.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/QTp32HEM1705028548091.jpeg</t>
         </is>
       </c>
     </row>
@@ -4656,38 +4455,38 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2024-01-27</t>
+          <t>2024-01-28</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>上海·咒术only-幽暗之森1.0</t>
+          <t>上海·坏孩纸物语の第32届动漫节之冬日季</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
+          <t>剑川路1000号 闵行龙湖天街</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.27 16:00</t>
+          <t>2024.01.28 14:00-01.28 20:00</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>261</v>
+        <v>744</v>
       </c>
       <c r="G15" t="n">
-        <v>69</v>
+        <v>36.9</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80045</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80871</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/hUfcrw3y1703055422885.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/5fmQrQJ81705573963752.png</t>
         </is>
       </c>
     </row>
@@ -4697,38 +4496,38 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2024-01-27</t>
+          <t>2024-01-31</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>上海·第八届次元鹿角动漫游戏展</t>
+          <t>上海·寻迹冬日LOVELIVE同好会</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>吴中路1588号上海爱琴海购物中心F4 竞梦元宇宙</t>
+          <t>愚园路1250号 新歌空间</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.28 21:00</t>
+          <t>2024.01.31 11:30-01.31 17:00</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>1232</v>
+        <v>194</v>
       </c>
       <c r="G16" t="n">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80979</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79332</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/xPOF923U1705545223366.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/Ewreg1JT1701677993728.jpeg</t>
         </is>
       </c>
     </row>
@@ -4738,38 +4537,38 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2024-01-27</t>
+          <t>2024-02-01</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>上海·魔都寒假漫展-CF01</t>
+          <t>上海·次元波板糖×线条小狗MALTESE 主题快闪店</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
+          <t>西藏北路166静安大悦城北座6楼611号 次元波板糖</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2024.01.27 10:00-01.28 16:00</t>
+          <t>2024.02.01 00:00-03.01 23:59</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>992</v>
+        <v>167</v>
       </c>
       <c r="G17" t="n">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80204</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81345</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/eK96fdcg1703573110264.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/Qbpful951706080847394.png</t>
         </is>
       </c>
     </row>
@@ -4779,38 +4578,38 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2024-01-27</t>
+          <t>2024-02-02</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>上海・明日方舟主题店·[SWEET ZONE甜蜜区域]</t>
+          <t>上海·2024《永远的7日之都》x  萌果酱谷子咖啡</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>南京东路830号第一百货商业中心B馆5楼(海底捞旁边) 第一百货商业中心</t>
+          <t>南京东路340号百联ZX 萌果酱谷子咖啡（百联）</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2024.01.27 00:00-03.31 23:59</t>
+          <t>2024.02.02 00:00-03.10 23:59</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>853</v>
+        <v>35</v>
       </c>
       <c r="G18" t="n">
         <v>30</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81277</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81357</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/hp6D0Drt1705991831205.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/5OYoWSGL1706087914805.jpeg</t>
         </is>
       </c>
     </row>
@@ -4820,38 +4619,38 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2024-01-28</t>
+          <t>2024-02-02</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>上海 ·WOW潮元原神x星铁主题二次元狂欢派对</t>
+          <t>上海·次元LAB 二次元电音节</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>政通路189号五角场万达广场C栋 元气森林livehouse</t>
+          <t>中兴路1683号金融街购物中心L3-27 蜚声上海Livehouse</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2024.01.28 14:00-01.28 19:00</t>
+          <t>2024.02.02 12:30-02.02 21:00</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>444</v>
+        <v>672</v>
       </c>
       <c r="G19" t="n">
-        <v>129</v>
+        <v>380</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80167</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80128</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/QTp32HEM1705028548091.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202312/DEW1XYty1703226993965.jpeg</t>
         </is>
       </c>
     </row>
@@ -4861,38 +4660,38 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2024-01-31</t>
+          <t>2024-02-03</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>上海·寻迹冬日LOVELIVE同好会</t>
+          <t>上海·Coser迎春动漫展</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>愚园路1250号 新歌空间</t>
+          <t>海潮路133号B1 JUMP工坊</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2024.01.31 11:30-01.31 17:00</t>
+          <t>2024.02.03 10:00-02.04 17:00</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>189</v>
+        <v>855</v>
       </c>
       <c r="G20" t="n">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79332</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80646</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/Ewreg1JT1701677993728.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/4WVkFc4d1704787729064.jpeg</t>
         </is>
       </c>
     </row>
@@ -4902,38 +4701,38 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2024-02-01</t>
+          <t>2024-02-03</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>上海·次元波板糖×线条小狗MALTESE 主题快闪店</t>
+          <t>上海·ENP电次元派对vol.04</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>西藏北路166静安大悦城北座6楼611号 次元波板糖</t>
+          <t>人民大道221号 迪美购物中心</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2024.02.01 00:00-03.01 23:59</t>
+          <t>2024.02.03 18:30-02.03 22:00</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>140</v>
+        <v>22</v>
       </c>
       <c r="G21" t="n">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81345</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80945</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/Qbpful951706080847394.png</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/1sjalWS51705479361512.jpeg</t>
         </is>
       </c>
     </row>
@@ -4943,38 +4742,38 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2024-02-02</t>
+          <t>2024-02-03</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>上海·2024《永远的7日之都》x  萌果酱谷子咖啡</t>
+          <t>上海·偶像梦幻祭红白歌合战Only</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>南京东路340号百联ZX 萌果酱谷子咖啡（百联）</t>
+          <t>虹许路731号4号楼 THE BOXX•城市乐园</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2024.02.02 00:00-03.10 23:59</t>
+          <t>2024.02.03 13:30-02.03 22:00</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="G22" t="n">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81357</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81199</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/5OYoWSGL1706087914805.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/C7E7svbZ1705903245860.jpeg</t>
         </is>
       </c>
     </row>
@@ -4984,38 +4783,38 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2024-02-02</t>
+          <t>2024-02-03</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>上海·次元LAB 二次元电音节</t>
+          <t>上海·第七届次元鹿角二次元派对</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>中兴路1683号金融街购物中心L3-27 蜚声上海Livehouse</t>
+          <t>长宁路1191号来福士西区(W)B1层01号、11号 星零界</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2024.02.02 12:30-02.02 21:00</t>
+          <t>2024.02.03 10:00-02.04 17:00</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>659</v>
+        <v>1331</v>
       </c>
       <c r="G23" t="n">
-        <v>380</v>
+        <v>98</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80128</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79938</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202312/DEW1XYty1703226993965.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/b1XT2w4T1705027781100.jpeg</t>
         </is>
       </c>
     </row>
@@ -5025,38 +4824,38 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2024-02-03</t>
+          <t>2024-02-04</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>上海·Coser迎春动漫展</t>
+          <t>上海·触手猴钢琴巡演·marasy piano live tour『生音』上海站·Powered by 东方弹幕神乐失落幻想</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>海潮路133号B1 JUMP工坊</t>
+          <t>丁香路425号(上海科技馆地铁站1号口步行460米) 上海东方艺术中心音乐厅</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2024.02.03 10:00-02.04 17:00</t>
+          <t>2024.02.04 19:30-02.04 21:00</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>786</v>
+        <v>470</v>
       </c>
       <c r="G24" t="n">
-        <v>60</v>
+        <v>280</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80646</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80734</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/4WVkFc4d1704787729064.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/IcjPp0TE1704951328918.jpeg</t>
         </is>
       </c>
     </row>
@@ -5066,38 +4865,38 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2024-02-03</t>
+          <t>2024-02-10</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>上海·偶像梦幻祭红白歌合战Only</t>
+          <t>上海·寒假CF漫展-春节档-神龙在世</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>虹许路731号4号楼 THE BOXX•城市乐园</t>
+          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2024.02.03 13:30-02.03 22:00</t>
+          <t>2024.02.10 10:00-02.17 16:00</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>86</v>
+        <v>38</v>
       </c>
       <c r="G25" t="n">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81199</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81192</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/C7E7svbZ1705903245860.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/S8XxkA631705896741998.jpeg</t>
         </is>
       </c>
     </row>
@@ -5107,38 +4906,38 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2024-02-04</t>
+          <t>2024-02-14</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>上海·触手猴钢琴巡演·marasy piano live tour『生音』上海站·Powered by 东方弹幕神乐失落幻想</t>
+          <t>上海·原X铁X崩only</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>丁香路425号(上海科技馆地铁站1号口步行460米) 上海东方艺术中心音乐厅</t>
+          <t>澳门路168号 月星国际家居</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2024.02.04 19:30-02.04 21:00</t>
+          <t>2024.02.14 10:30-02.14 16:30</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>372</v>
+        <v>26</v>
       </c>
       <c r="G26" t="n">
-        <v>280</v>
+        <v>60</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80734</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81446</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/IcjPp0TE1704951328918.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/IIePRulM1706248855263.jpeg</t>
         </is>
       </c>
     </row>
@@ -5148,38 +4947,38 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2024-02-10</t>
+          <t>2024-02-14</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>上海·寒假CF漫展-春节档-神龙在世</t>
+          <t>上海·奇卡波利动漫嘉年华</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
+          <t>申滨路36号 虹桥丽宝广场</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2024.02.10 10:00-02.17 16:00</t>
+          <t>2024.02.14 10:00-02.14 17:00</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="G27" t="n">
-        <v>49</v>
+        <v>48.8</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81192</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81260</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/S8XxkA631705896741998.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/9OHovK2V1705978109130.jpeg</t>
         </is>
       </c>
     </row>
@@ -5194,33 +4993,33 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>上海·奇卡波利动漫嘉年华</t>
+          <t>上海·魔都COS漫展-情人节专场AM01</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>申滨路36号 虹桥丽宝广场</t>
+          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2024.02.14 10:00-02.14 17:00</t>
+          <t>2024.02.14 10:00-02.14 16:00</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="G28" t="n">
-        <v>48.8</v>
+        <v>49</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81260</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80691</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/9OHovK2V1705978109130.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/aSdjV6Kw1704868345679.jpeg</t>
         </is>
       </c>
     </row>
@@ -5230,38 +5029,38 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2024-02-14</t>
+          <t>2024-02-16</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>上海·魔都COS漫展-情人节专场AM01</t>
+          <t>上海·次元裂缝-X 新年anikura派对</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
+          <t>海潮路133号B1 JUMP工坊</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2024.02.14 10:00-02.14 16:00</t>
+          <t>2024.02.16 14:00-02.16 19:00</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="G29" t="n">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80691</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81314</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/aSdjV6Kw1704868345679.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/OrhHWKdR1706062360956.jpeg</t>
         </is>
       </c>
     </row>
@@ -5276,33 +5075,33 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>上海·次元裂缝-X 新年anikura派对</t>
+          <t>上海·第九届次元鹿角动漫游戏展</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>海潮路133号B1 JUMP工坊</t>
+          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2024.02.16 14:00-02.16 19:00</t>
+          <t>2024.02.16 11:00-02.17 18:00</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>22</v>
+        <v>1250</v>
       </c>
       <c r="G30" t="n">
-        <v>60</v>
+        <v>65.90000000000001</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81314</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80497</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/OrhHWKdR1706062360956.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/0duSXTQy1704423309244.jpeg</t>
         </is>
       </c>
     </row>
@@ -5312,38 +5111,38 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2024-02-16</t>
+          <t>2024-02-17</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>上海·第九届次元鹿角动漫游戏展</t>
+          <t>上海·少女番only2.0</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
+          <t>营口路699号(黄兴公园地铁站2号口旁) 花嫁丽舍</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2024.02.16 11:00-02.17 18:00</t>
+          <t>2024.02.17 10:00-02.17 17:00</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>1242</v>
+        <v>349</v>
       </c>
       <c r="G31" t="n">
-        <v>65.90000000000001</v>
+        <v>80</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80497</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81148</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/0duSXTQy1704423309244.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/j6eEZ18S1705657346664.jpeg</t>
         </is>
       </c>
     </row>
@@ -5353,38 +5152,38 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2024-02-17</t>
+          <t>2024-02-24</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>上海·少女番only2.0</t>
+          <t>上海·SISPmini动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>营口路699号(黄兴公园地铁站2号口旁) 花嫁丽舍</t>
+          <t>剑川路1000号 龙湖上海闵行天街</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2024.02.17 10:00-02.17 17:00</t>
+          <t>2024.02.24 13:00-02.25 19:00</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>327</v>
+        <v>426</v>
       </c>
       <c r="G32" t="n">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81148</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=79046</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/j6eEZ18S1705657346664.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/jzovdppq1706166165502.jpeg</t>
         </is>
       </c>
     </row>
@@ -5399,33 +5198,33 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>上海·SISPmini动漫游戏嘉年华</t>
+          <t>上海·原神×崩坏×星铁only旅行盛宴2.0</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>剑川路1000号 龙湖上海闵行天街</t>
+          <t>西藏南路1号 上海大世界</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2024.02.24 13:00-02.25 19:00</t>
+          <t>2024.02.24 10:00-02.25 17:00</t>
         </is>
       </c>
       <c r="F33" t="n">
-        <v>422</v>
+        <v>118</v>
       </c>
       <c r="G33" t="n">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79046</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81276</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/jzovdppq1706166165502.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/82hU3z8m1706155835021.png</t>
         </is>
       </c>
     </row>
@@ -5440,33 +5239,33 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>上海·原神×崩坏×星铁only旅行盛宴2.0</t>
+          <t>上海·趣元界&amp;斗罗大陆上元佳节次元派对</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>西藏南路1号 上海大世界</t>
+          <t>长宁路1191号长宁来福士B1 长宁来福士</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2024.02.24 10:00-02.25 17:00</t>
+          <t>2024.02.24 11:30-02.25 17:30</t>
         </is>
       </c>
       <c r="F34" t="n">
-        <v>89</v>
+        <v>509</v>
       </c>
       <c r="G34" t="n">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81276</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81415</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/82hU3z8m1706155835021.png</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/yis4JHfE1706169986733.jpeg</t>
         </is>
       </c>
     </row>
@@ -5481,33 +5280,33 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>上海·第三届燃梦BACG PRO游戏动漫展-原X铁X崩同好交流</t>
+          <t>上海·魔都元宵节漫展-COS为王</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>盈浦街道淀山浦社区淀山湖大道851号青浦万达茂F3 万达汽车乐园(青浦万达茂店)</t>
+          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2024.02.24 11:00-02.25 16:30</t>
+          <t>2024.02.24 10:00-02.25 16:00</t>
         </is>
       </c>
       <c r="F35" t="n">
-        <v>2508</v>
+        <v>11</v>
       </c>
       <c r="G35" t="n">
-        <v>65.8</v>
+        <v>49</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77754</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81238</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202312/7eGZETK91701943985671.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/KxQZPADR1705913896609.jpeg</t>
         </is>
       </c>
     </row>
@@ -5522,33 +5321,33 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>上海·趣元界&amp;斗罗大陆上元佳节次元派对</t>
+          <t>上海·魔都多厨狂喜漫展-CH01</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>长宁路1191号长宁来福士B1 长宁来福士</t>
+          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2024.02.24 11:30-02.25 17:30</t>
+          <t>2024.02.24 10:00-02.25 16:00</t>
         </is>
       </c>
       <c r="F36" t="n">
-        <v>508</v>
+        <v>1</v>
       </c>
       <c r="G36" t="n">
-        <v>98</v>
+        <v>49</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81415</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81423</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/yis4JHfE1706169986733.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/axpOY3zo1706173660010.jpeg</t>
         </is>
       </c>
     </row>
@@ -5558,38 +5357,38 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2024-02-24</t>
+          <t>2024-03-02</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>上海·魔都元宵节漫展-COS为王</t>
+          <t>上海·原神X星穹铁道ONLY</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>澳门路168号月星家居(江宁路地铁站1号口步行420米) 月星广场</t>
+          <t>逸仙路301号靠纪念路路口 上海宝丰联大酒店</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2024.02.24 10:00-02.25 16:00</t>
+          <t>2024.03.02 10:00-03.02 17:00</t>
         </is>
       </c>
       <c r="F37" t="n">
-        <v>11</v>
+        <v>260</v>
       </c>
       <c r="G37" t="n">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81238</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80299</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/KxQZPADR1705913896609.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202312/V0xu26Cl1703753850690.jpeg</t>
         </is>
       </c>
     </row>
@@ -5604,33 +5403,33 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>上海·原神X星穹铁道ONLY</t>
+          <t>上海·小山百代2024上海粉丝见面会</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>逸仙路301号靠纪念路路口 上海宝丰联大酒店</t>
+          <t>宜昌路179号 万代南梦宫上海文化中心</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2024.03.02 10:00-03.02 17:00</t>
+          <t>2024.03.02 13:00-03.02 20:00</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="G38" t="n">
-        <v>60</v>
+        <v>380</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80299</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=80924</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202312/V0xu26Cl1703753850690.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/FpA9OkKy1705467080070.jpeg</t>
         </is>
       </c>
     </row>
@@ -5659,7 +5458,7 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="G39" t="n">
         <v>60</v>
@@ -5681,38 +5480,38 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2024-03-09</t>
+          <t>2024-03-08</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>上海·S·CGE动漫游戏嘉年华</t>
+          <t>上海·第八届ACBC动漫盛典-国潮汉服游园会</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>军工路1076号 纪希片场(秀场)</t>
+          <t>浦锦南路1586弄2号 奇迹花园</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2024.03.09 10:00-03.10 17:00</t>
+          <t>2024.03.08 10:00-03.10 17:00</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="G40" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81173</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81456</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/TYA5FLkE1705891815532.jpeg</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/qZtpawf51706254849667.jpeg</t>
         </is>
       </c>
     </row>
@@ -5727,33 +5526,33 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>上海·爱乐之城音乐会</t>
+          <t>上海·S·CGE动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>南京西路1376号 上海商城剧院</t>
+          <t>军工路1076号 纪希片场(秀场)</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2024.03.09 14:00-03.09 15:30</t>
+          <t>2024.03.09 10:00-03.10 17:00</t>
         </is>
       </c>
       <c r="F41" t="n">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="G41" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81289</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81173</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202401/ZZXtDrwZ1705996679699.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/TYA5FLkE1705891815532.jpeg</t>
         </is>
       </c>
     </row>
@@ -5768,33 +5567,33 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
+          <t>上海·爱乐之城音乐会</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>漕宝路1688号 诺宝中心酒店</t>
+          <t>南京西路1376号 上海商城剧院</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2024.03.09 10:00-03.09 16:30</t>
+          <t>2024.03.09 14:00-03.09 15:30</t>
         </is>
       </c>
       <c r="F42" t="n">
-        <v>888</v>
+        <v>2</v>
       </c>
       <c r="G42" t="n">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=76410</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81289</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>//i2.hdslb.com/bfs/openplatform/202309/fVXMrcHy1693971682397.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/ZZXtDrwZ1705996679699.jpeg</t>
         </is>
       </c>
     </row>
@@ -5804,38 +5603,38 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2024-03-16</t>
+          <t>2024-03-09</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>上海·三月的幻想演唱会2024「飞越蓝色时刻」</t>
+          <t>上海·青山刚昌ONLY【名侦探柯南&amp;魔术快斗】</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>宜昌路179号 万代南梦宫上海文化中心</t>
+          <t>漕宝路1688号 诺宝中心酒店</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2024.03.16 19:00-03.16 20:30</t>
+          <t>2024.03.09 10:00-03.09 16:30</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>47</v>
+        <v>893</v>
       </c>
       <c r="G43" t="n">
-        <v>380</v>
+        <v>73</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80811</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=76410</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/TO6xpSqr1705289483473.png</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202309/fVXMrcHy1693971682397.jpeg</t>
         </is>
       </c>
     </row>
@@ -5845,38 +5644,38 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2024-03-17</t>
+          <t>2024-03-16</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>上海·遇见新海诚--帝玖「这次一定」室内乐ACG音乐会</t>
+          <t>上海·坏孩纸物语の第33届动漫节之庄子篇</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>延安东路523号 凯迪拉克·上海音乐厅</t>
+          <t>中山北路3300号4楼L4001号 环球港上海世嘉都市乐园</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2024.03.17 14:00-03.17 16:00</t>
+          <t>2024.03.16 10:00-03.17 21:00</t>
         </is>
       </c>
       <c r="F44" t="n">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="G44" t="n">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81258</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81138</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>//i1.hdslb.com/bfs/openplatform/202401/eysvN81k1705977896972.jpeg</t>
+          <t>//i2.hdslb.com/bfs/openplatform/202401/jpr1lCt21705652306481.png</t>
         </is>
       </c>
     </row>
@@ -5886,38 +5685,38 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2024-03-23</t>
+          <t>2024-03-17</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>上海·《四月是你的谎言》友人A经典动漫音乐会</t>
+          <t>上海·遇见新海诚--帝玖「这次一定」室内乐ACG音乐会</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>南京西路1376号 上海商城剧院</t>
+          <t>延安东路523号 凯迪拉克·上海音乐厅</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2024.03.23 15:00-03.23 16:30</t>
+          <t>2024.03.17 14:00-03.17 16:00</t>
         </is>
       </c>
       <c r="F45" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G45" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81361</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81258</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/wL0ZWVYi1706091574963.png</t>
+          <t>//i1.hdslb.com/bfs/openplatform/202401/eysvN81k1705977896972.jpeg</t>
         </is>
       </c>
     </row>
@@ -5927,38 +5726,38 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-03-23</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>上海· TRUE（唐沢美帆）上海动漫交响音乐会</t>
+          <t>上海·《四月是你的谎言》友人A经典动漫音乐会</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>丁香路425号 上海东方艺术中心</t>
+          <t>南京西路1376号 上海商城剧院</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2024.03.30 19:30-03.30 21:00</t>
+          <t>2024.03.23 15:00-03.23 16:30</t>
         </is>
       </c>
       <c r="F46" t="n">
-        <v>186</v>
+        <v>12</v>
       </c>
       <c r="G46" t="n">
-        <v>280</v>
+        <v>50</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80906</t>
+          <t>https://show.bilibili.com/platform/detail.html?id=81361</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>//i0.hdslb.com/bfs/openplatform/202401/FaJbLvS51705401178235.jpeg</t>
+          <t>//i0.hdslb.com/bfs/openplatform/202401/wL0ZWVYi1706091574963.png</t>
         </is>
       </c>
     </row>
@@ -6069,7 +5868,7 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G49" t="n">
         <v>70</v>
@@ -6110,7 +5909,7 @@
         </is>
       </c>
       <c r="F50" t="n">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="G50" t="n">
         <v>79</v>

</xml_diff>

<commit_message>
Update gh-pages to output generated at 3967b19
</commit_message>
<xml_diff>
--- a/上海-漫展信息.xlsx
+++ b/上海-漫展信息.xlsx
@@ -836,7 +836,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="G10" t="n">
         <v>36.9</v>
@@ -1205,7 +1205,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G19" t="n">
         <v>48.8</v>
@@ -1369,7 +1369,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="G23" t="n">
         <v>80</v>
@@ -2419,7 +2419,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="G6" t="n">
         <v>280</v>
@@ -2952,7 +2952,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="G19" t="n">
         <v>480</v>
@@ -3385,7 +3385,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1735</v>
+        <v>1736</v>
       </c>
       <c r="G2" t="n">
         <v>60</v>
@@ -3549,7 +3549,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>2174</v>
+        <v>2175</v>
       </c>
       <c r="G6" t="n">
         <v>30</v>
@@ -3631,7 +3631,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="G8" t="n">
         <v>10</v>
@@ -3941,7 +3941,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1735</v>
+        <v>1736</v>
       </c>
       <c r="G2" t="n">
         <v>60</v>
@@ -4023,7 +4023,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>2174</v>
+        <v>2175</v>
       </c>
       <c r="G4" t="n">
         <v>30</v>
@@ -4228,7 +4228,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="G9" t="n">
         <v>10</v>
@@ -4474,7 +4474,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="G15" t="n">
         <v>36.9</v>
@@ -4843,7 +4843,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="G24" t="n">
         <v>280</v>
@@ -4966,7 +4966,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G27" t="n">
         <v>48.8</v>
@@ -5130,7 +5130,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="G31" t="n">
         <v>80</v>

</xml_diff>

<commit_message>
Update gh-pages to output generated at 456a3b4
</commit_message>
<xml_diff>
--- a/上海-漫展信息.xlsx
+++ b/上海-漫展信息.xlsx
@@ -711,7 +711,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="G7" t="n">
         <v>59</v>
@@ -4351,7 +4351,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="G12" t="n">
         <v>59</v>

</xml_diff>